<commit_message>
Organize two notebooks into example/Example.ipynb
</commit_message>
<xml_diff>
--- a/example/DoesCal.xlsx
+++ b/example/DoesCal.xlsx
@@ -3,11 +3,15 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15500" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Initial" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="420.0MeV" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="333.0MeV" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="362.0MeV" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="391.0MeV" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="303.0MeV" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
@@ -17,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -33,43 +37,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Aptos Narrow"/>
-      <b val="1"/>
-      <sz val="12"/>
-    </font>
-    <font>
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -82,7 +72,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
@@ -96,19 +86,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -510,8 +503,8 @@
   </sheetPr>
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -520,8 +513,8 @@
     <col width="16.83203125" customWidth="1" style="1" min="9" max="12"/>
     <col width="14.83203125" customWidth="1" style="1" min="13" max="15"/>
     <col width="12.83203125" customWidth="1" style="1" min="16" max="17"/>
-    <col width="10.83203125" customWidth="1" style="1" min="18" max="22"/>
-    <col width="10.83203125" customWidth="1" style="1" min="23" max="16384"/>
+    <col width="10.83203125" customWidth="1" style="1" min="18" max="23"/>
+    <col width="10.83203125" customWidth="1" style="1" min="24" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -530,7 +523,7 @@
           <t>Target</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>27Al</t>
         </is>
@@ -540,7 +533,7 @@
           <t>Beam</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>84Kr</t>
         </is>
@@ -572,7 +565,7 @@
           <t>Z</t>
         </is>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="5" t="n">
         <v>13</v>
       </c>
       <c r="E2" s="1" t="inlineStr">
@@ -580,13 +573,13 @@
           <t>Z</t>
         </is>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="I2" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="J2" s="5" t="n">
         <v>420</v>
       </c>
       <c r="K2" t="n">
@@ -602,7 +595,7 @@
           <t>N</t>
         </is>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="5" t="n">
         <v>14</v>
       </c>
       <c r="E3" s="1" t="inlineStr">
@@ -610,14 +603,20 @@
           <t>N</t>
         </is>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="5" t="n">
         <v>48</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="I3" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="J3" s="5" t="n">
         <v>391</v>
+      </c>
+      <c r="K3" t="n">
+        <v>295.892</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1121.6</v>
       </c>
     </row>
     <row r="4">
@@ -626,7 +625,7 @@
           <t>A</t>
         </is>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="5" t="n">
         <v>27</v>
       </c>
       <c r="E4" s="1" t="inlineStr">
@@ -634,14 +633,20 @@
           <t>A</t>
         </is>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="5" t="n">
         <v>84</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="I4" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="J4" s="1" t="n">
+      <c r="J4" s="5" t="n">
         <v>362</v>
+      </c>
+      <c r="K4" t="n">
+        <v>273.946</v>
+      </c>
+      <c r="L4" t="n">
+        <v>984.693</v>
       </c>
     </row>
     <row r="5">
@@ -650,7 +655,7 @@
           <t>thickness</t>
         </is>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="5" t="n">
         <v>15</v>
       </c>
       <c r="C5" s="4" t="inlineStr">
@@ -663,7 +668,7 @@
           <t>Energy</t>
         </is>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G5" s="4" t="inlineStr">
@@ -671,15 +676,21 @@
           <t>MeV/u</t>
         </is>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="I5" s="5" t="n">
         <v>9</v>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="J5" s="5" t="n">
         <v>333</v>
       </c>
+      <c r="K5" t="n">
+        <v>252</v>
+      </c>
+      <c r="L5" t="n">
+        <v>813.499</v>
+      </c>
     </row>
     <row r="6" ht="17" customHeight="1">
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="5" t="n">
         <v>4.053</v>
       </c>
       <c r="C6" s="4" t="inlineStr">
@@ -687,7 +698,7 @@
           <t>mg/cm2</t>
         </is>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="5" t="n">
         <v>420</v>
       </c>
       <c r="G6" s="4" t="inlineStr">
@@ -695,11 +706,17 @@
           <t>MeV</t>
         </is>
       </c>
-      <c r="I6" s="1" t="n">
+      <c r="I6" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="J6" s="1" t="n">
+      <c r="J6" s="5" t="n">
         <v>303</v>
+      </c>
+      <c r="K6" t="n">
+        <v>229.297</v>
+      </c>
+      <c r="L6" t="n">
+        <v>590.221</v>
       </c>
     </row>
     <row r="7">
@@ -708,7 +725,7 @@
           <t>Molar Mass</t>
         </is>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="5" t="n">
         <v>26.9815</v>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -721,7 +738,7 @@
           <t>Rate</t>
         </is>
       </c>
-      <c r="F7" s="5" t="n">
+      <c r="F7" s="7" t="n">
         <v>1000000000</v>
       </c>
       <c r="G7" s="4" t="inlineStr">
@@ -731,7 +748,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="5" t="n">
         <v>4.481976744186046e-23</v>
       </c>
       <c r="C8" s="2" t="inlineStr">
@@ -744,7 +761,7 @@
           <t>Running Time</t>
         </is>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="5" t="n">
         <v>3600</v>
       </c>
       <c r="G8" s="4" t="inlineStr">
@@ -807,548 +824,2313 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="n">
+      <c r="A2" s="10" t="n">
         <v>49</v>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="10" t="n">
         <v>57</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="10" t="n">
         <v>106</v>
       </c>
-      <c r="D2" s="7" t="inlineStr">
+      <c r="D2" s="10" t="inlineStr">
         <is>
           <t>In</t>
         </is>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="10" t="n">
         <v>40.6</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="n">
+      <c r="A3" s="10" t="n">
         <v>48</v>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="10" t="n">
         <v>58</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="10" t="n">
         <v>106</v>
       </c>
-      <c r="D3" s="7" t="inlineStr">
+      <c r="D3" s="10" t="inlineStr">
         <is>
           <t>Cd</t>
         </is>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="10" t="n">
         <v>62.7</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="n">
+      <c r="A4" s="10" t="n">
         <v>47</v>
       </c>
-      <c r="B4" s="7" t="n">
+      <c r="B4" s="10" t="n">
         <v>59</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="10" t="n">
         <v>106</v>
       </c>
-      <c r="D4" s="7" t="inlineStr">
+      <c r="D4" s="10" t="inlineStr">
         <is>
           <t>Ag</t>
         </is>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="10" t="n">
         <v>8.609999999999999</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="n">
+      <c r="A5" s="10" t="n">
         <v>49</v>
       </c>
-      <c r="B5" s="7" t="n">
+      <c r="B5" s="10" t="n">
         <v>56</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="10" t="n">
         <v>105</v>
       </c>
-      <c r="D5" s="7" t="inlineStr">
+      <c r="D5" s="10" t="inlineStr">
         <is>
           <t>In</t>
         </is>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="10" t="n">
         <v>72.59999999999999</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="n">
+      <c r="A6" s="10" t="n">
         <v>48</v>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="10" t="n">
         <v>57</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="10" t="n">
         <v>105</v>
       </c>
-      <c r="D6" s="7" t="inlineStr">
+      <c r="D6" s="10" t="inlineStr">
         <is>
           <t>Cd</t>
         </is>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="10" t="n">
         <v>320</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="n">
+      <c r="A7" s="10" t="n">
         <v>47</v>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="10" t="n">
         <v>58</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="10" t="n">
         <v>105</v>
       </c>
-      <c r="D7" s="7" t="inlineStr">
+      <c r="D7" s="10" t="inlineStr">
         <is>
           <t>Ag</t>
         </is>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="10" t="n">
         <v>68.90000000000001</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="n">
+      <c r="A8" s="10" t="n">
         <v>46</v>
       </c>
-      <c r="B8" s="7" t="n">
+      <c r="B8" s="10" t="n">
         <v>59</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="10" t="n">
         <v>105</v>
       </c>
-      <c r="D8" s="7" t="inlineStr">
+      <c r="D8" s="10" t="inlineStr">
         <is>
           <t>Pd</t>
         </is>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="10" t="n">
         <v>3.69</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="n">
+      <c r="A9" s="10" t="n">
         <v>49</v>
       </c>
-      <c r="B9" s="7" t="n">
+      <c r="B9" s="10" t="n">
         <v>55</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="10" t="n">
         <v>104</v>
       </c>
-      <c r="D9" s="7" t="inlineStr">
+      <c r="D9" s="10" t="inlineStr">
         <is>
           <t>In</t>
         </is>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="10" t="n">
         <v>4.92</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="n">
+      <c r="A10" s="10" t="n">
         <v>48</v>
       </c>
-      <c r="B10" s="7" t="n">
+      <c r="B10" s="10" t="n">
         <v>56</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="10" t="n">
         <v>104</v>
       </c>
-      <c r="D10" s="7" t="inlineStr">
+      <c r="D10" s="10" t="inlineStr">
         <is>
           <t>Cd</t>
         </is>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E10" s="10" t="n">
         <v>51.7</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="n">
+      <c r="A11" s="10" t="n">
         <v>47</v>
       </c>
-      <c r="B11" s="7" t="n">
+      <c r="B11" s="10" t="n">
         <v>57</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="10" t="n">
         <v>104</v>
       </c>
-      <c r="D11" s="7" t="inlineStr">
+      <c r="D11" s="10" t="inlineStr">
         <is>
           <t>Ag</t>
         </is>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="E11" s="10" t="n">
         <v>20.9</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="n">
+      <c r="A12" s="10" t="n">
         <v>47</v>
       </c>
-      <c r="B12" s="7" t="n">
+      <c r="B12" s="10" t="n">
         <v>56</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="10" t="n">
         <v>103</v>
       </c>
-      <c r="D12" s="7" t="inlineStr">
+      <c r="D12" s="10" t="inlineStr">
         <is>
           <t>Ag</t>
         </is>
       </c>
-      <c r="E12" s="7" t="n">
+      <c r="E12" s="10" t="n">
         <v>84.90000000000001</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="n">
+      <c r="A13" s="10" t="n">
         <v>46</v>
       </c>
-      <c r="B13" s="7" t="n">
+      <c r="B13" s="10" t="n">
         <v>57</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="10" t="n">
         <v>103</v>
       </c>
-      <c r="D13" s="7" t="inlineStr">
+      <c r="D13" s="10" t="inlineStr">
         <is>
           <t>Pd</t>
         </is>
       </c>
-      <c r="E13" s="7" t="n">
+      <c r="E13" s="10" t="n">
         <v>43.1</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="n">
+      <c r="A14" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="B14" s="7" t="n">
+      <c r="B14" s="10" t="n">
         <v>58</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="10" t="n">
         <v>103</v>
       </c>
-      <c r="D14" s="7" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
         <is>
           <t>Rh</t>
         </is>
       </c>
-      <c r="E14" s="7" t="n">
+      <c r="E14" s="10" t="n">
         <v>4.92</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="n">
+      <c r="A15" s="10" t="n">
         <v>44</v>
       </c>
-      <c r="B15" s="7" t="n">
+      <c r="B15" s="10" t="n">
         <v>59</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="10" t="n">
         <v>103</v>
       </c>
-      <c r="D15" s="7" t="inlineStr">
+      <c r="D15" s="10" t="inlineStr">
         <is>
           <t>Ru</t>
         </is>
       </c>
-      <c r="E15" s="7" t="n">
+      <c r="E15" s="10" t="n">
         <v>1.23</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="n">
+      <c r="A16" s="10" t="n">
         <v>47</v>
       </c>
-      <c r="B16" s="7" t="n">
+      <c r="B16" s="10" t="n">
         <v>55</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="10" t="n">
         <v>102</v>
       </c>
-      <c r="D16" s="7" t="inlineStr">
+      <c r="D16" s="10" t="inlineStr">
         <is>
           <t>Ag</t>
         </is>
       </c>
-      <c r="E16" s="7" t="n">
+      <c r="E16" s="10" t="n">
         <v>157</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="n">
+      <c r="A17" s="10" t="n">
         <v>46</v>
       </c>
-      <c r="B17" s="7" t="n">
+      <c r="B17" s="10" t="n">
         <v>56</v>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="10" t="n">
         <v>102</v>
       </c>
-      <c r="D17" s="7" t="inlineStr">
+      <c r="D17" s="10" t="inlineStr">
         <is>
           <t>Pd</t>
         </is>
       </c>
-      <c r="E17" s="7" t="n">
+      <c r="E17" s="10" t="n">
         <v>135</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="n">
+      <c r="A18" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="B18" s="7" t="n">
+      <c r="B18" s="10" t="n">
         <v>57</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="10" t="n">
         <v>102</v>
       </c>
-      <c r="D18" s="7" t="inlineStr">
+      <c r="D18" s="10" t="inlineStr">
         <is>
           <t>Rh</t>
         </is>
       </c>
-      <c r="E18" s="7" t="n">
+      <c r="E18" s="10" t="n">
         <v>17.2</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="n">
+      <c r="A19" s="10" t="n">
         <v>47</v>
       </c>
-      <c r="B19" s="7" t="n">
+      <c r="B19" s="10" t="n">
         <v>54</v>
       </c>
-      <c r="C19" s="7" t="n">
+      <c r="C19" s="10" t="n">
         <v>101</v>
       </c>
-      <c r="D19" s="7" t="inlineStr">
+      <c r="D19" s="10" t="inlineStr">
         <is>
           <t>Ag</t>
         </is>
       </c>
-      <c r="E19" s="7" t="n">
+      <c r="E19" s="10" t="n">
         <v>4.92</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="7" t="n">
+      <c r="A20" s="10" t="n">
         <v>46</v>
       </c>
-      <c r="B20" s="7" t="n">
+      <c r="B20" s="10" t="n">
         <v>55</v>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="C20" s="10" t="n">
         <v>101</v>
       </c>
-      <c r="D20" s="7" t="inlineStr">
+      <c r="D20" s="10" t="inlineStr">
         <is>
           <t>Pd</t>
         </is>
       </c>
-      <c r="E20" s="7" t="n">
+      <c r="E20" s="10" t="n">
         <v>11.1</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="7" t="n">
+      <c r="A21" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B21" s="10" t="n">
         <v>56</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="10" t="n">
         <v>101</v>
       </c>
-      <c r="D21" s="7" t="inlineStr">
+      <c r="D21" s="10" t="inlineStr">
         <is>
           <t>Rh</t>
         </is>
       </c>
-      <c r="E21" s="7" t="n">
+      <c r="E21" s="10" t="n">
         <v>1.23</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="n">
+      <c r="A22" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="B22" s="7" t="n">
+      <c r="B22" s="10" t="n">
         <v>55</v>
       </c>
-      <c r="C22" s="7" t="n">
+      <c r="C22" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="D22" s="7" t="inlineStr">
+      <c r="D22" s="10" t="inlineStr">
         <is>
           <t>Rh</t>
         </is>
       </c>
-      <c r="E22" s="7" t="n">
+      <c r="E22" s="10" t="n">
         <v>33.2</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="7" t="n">
+      <c r="A23" s="10" t="n">
         <v>44</v>
       </c>
-      <c r="B23" s="7" t="n">
+      <c r="B23" s="10" t="n">
         <v>56</v>
       </c>
-      <c r="C23" s="7" t="n">
+      <c r="C23" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="D23" s="7" t="inlineStr">
+      <c r="D23" s="10" t="inlineStr">
         <is>
           <t>Ru</t>
         </is>
       </c>
-      <c r="E23" s="7" t="n">
+      <c r="E23" s="10" t="n">
         <v>7.38</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="7" t="n">
+      <c r="A24" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="B24" s="7" t="n">
+      <c r="B24" s="10" t="n">
         <v>54</v>
       </c>
-      <c r="C24" s="7" t="n">
+      <c r="C24" s="10" t="n">
         <v>99</v>
       </c>
-      <c r="D24" s="7" t="inlineStr">
+      <c r="D24" s="10" t="inlineStr">
         <is>
           <t>Rh</t>
         </is>
       </c>
-      <c r="E24" s="7" t="n">
+      <c r="E24" s="10" t="n">
         <v>52.9</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="n">
+      <c r="A25" s="10" t="n">
         <v>44</v>
       </c>
-      <c r="B25" s="7" t="n">
+      <c r="B25" s="10" t="n">
         <v>55</v>
       </c>
-      <c r="C25" s="7" t="n">
+      <c r="C25" s="10" t="n">
         <v>99</v>
       </c>
-      <c r="D25" s="7" t="inlineStr">
+      <c r="D25" s="10" t="inlineStr">
         <is>
           <t>Ru</t>
         </is>
       </c>
-      <c r="E25" s="7" t="n">
+      <c r="E25" s="10" t="n">
         <v>12.3</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="7" t="n">
+      <c r="A26" s="10" t="n">
         <v>45</v>
       </c>
-      <c r="B26" s="7" t="n">
+      <c r="B26" s="10" t="n">
         <v>53</v>
       </c>
-      <c r="C26" s="7" t="n">
+      <c r="C26" s="10" t="n">
         <v>98</v>
       </c>
-      <c r="D26" s="7" t="inlineStr">
+      <c r="D26" s="10" t="inlineStr">
         <is>
           <t>Rh</t>
         </is>
       </c>
-      <c r="E26" s="7" t="n">
+      <c r="E26" s="10" t="n">
         <v>1.23</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="7" t="n">
+      <c r="A27" s="10" t="n">
         <v>44</v>
       </c>
-      <c r="B27" s="7" t="n">
+      <c r="B27" s="10" t="n">
         <v>54</v>
       </c>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="10" t="n">
         <v>98</v>
       </c>
-      <c r="D27" s="7" t="inlineStr">
+      <c r="D27" s="10" t="inlineStr">
         <is>
           <t>Ru</t>
         </is>
       </c>
-      <c r="E27" s="7" t="n">
+      <c r="E27" s="10" t="n">
         <v>2.46</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="7" t="n">
+      <c r="A28" s="10" t="n">
         <v>43</v>
       </c>
-      <c r="B28" s="7" t="n">
+      <c r="B28" s="10" t="n">
         <v>54</v>
       </c>
-      <c r="C28" s="7" t="n">
+      <c r="C28" s="10" t="n">
         <v>97</v>
       </c>
-      <c r="D28" s="7" t="inlineStr">
+      <c r="D28" s="10" t="inlineStr">
         <is>
           <t>Tc</t>
         </is>
       </c>
-      <c r="E28" s="7" t="n">
+      <c r="E28" s="10" t="n">
         <v>2.46</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="7" t="n">
+      <c r="A29" s="10" t="n">
         <v>43</v>
       </c>
-      <c r="B29" s="7" t="n">
+      <c r="B29" s="10" t="n">
         <v>53</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C29" s="10" t="n">
         <v>96</v>
       </c>
-      <c r="D29" s="7" t="inlineStr">
+      <c r="D29" s="10" t="inlineStr">
         <is>
           <t>Tc</t>
         </is>
       </c>
-      <c r="E29" s="7" t="n">
+      <c r="E29" s="10" t="n">
         <v>2.46</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="7" t="inlineStr">
+      <c r="A30" s="10" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B30" s="7" t="inlineStr"/>
-      <c r="C30" s="7" t="inlineStr"/>
-      <c r="D30" s="7" t="inlineStr"/>
-      <c r="E30" s="7" t="n">
+      <c r="B30" s="10" t="inlineStr"/>
+      <c r="C30" s="10" t="inlineStr"/>
+      <c r="D30" s="10" t="inlineStr"/>
+      <c r="E30" s="10" t="n">
         <v>1230.27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>isotope</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
+        <is>
+          <t>x-section(mb)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B2" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>108</v>
+      </c>
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="n">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="n">
+        <v>75.7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <v>60</v>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E5" s="10" t="n">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D7" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>60</v>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D9" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>0.8129999999999999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="D10" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="D11" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>86.2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="D12" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>24.4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B13" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E13" s="10" t="n">
+        <v>69.09999999999999</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B14" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E14" s="10" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B15" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>101</v>
+      </c>
+      <c r="D15" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E15" s="10" t="n">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="n">
+        <v>44</v>
+      </c>
+      <c r="B16" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>101</v>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>Ru</t>
+        </is>
+      </c>
+      <c r="E16" s="10" t="n">
+        <v>0.8129999999999999</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B17" s="10" t="n">
+        <v>55</v>
+      </c>
+      <c r="C17" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E17" s="10" t="n">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="n">
+        <v>43</v>
+      </c>
+      <c r="B18" s="10" t="n">
+        <v>55</v>
+      </c>
+      <c r="C18" s="10" t="n">
+        <v>98</v>
+      </c>
+      <c r="D18" s="10" t="inlineStr">
+        <is>
+          <t>Tc</t>
+        </is>
+      </c>
+      <c r="E18" s="10" t="n">
+        <v>0.8129999999999999</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B19" s="10" t="inlineStr"/>
+      <c r="C19" s="10" t="inlineStr"/>
+      <c r="D19" s="10" t="inlineStr"/>
+      <c r="E19" s="10" t="n">
+        <v>813.499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>isotope</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
+        <is>
+          <t>x-section(mb)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B2" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="n">
+        <v>37.4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>21.7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <v>60</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="n">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E5" s="10" t="n">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D7" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="D9" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>38.4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="D10" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>9.85</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="D11" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="D12" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B13" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E13" s="10" t="n">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B14" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E14" s="10" t="n">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B15" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="D15" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E15" s="10" t="n">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B16" s="10" t="n">
+        <v>55</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>102</v>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E16" s="10" t="n">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B17" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C17" s="10" t="n">
+        <v>102</v>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E17" s="10" t="n">
+        <v>5.91</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B18" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C18" s="10" t="n">
+        <v>102</v>
+      </c>
+      <c r="D18" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E18" s="10" t="n">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B19" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C19" s="10" t="n">
+        <v>101</v>
+      </c>
+      <c r="D19" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E19" s="10" t="n">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="n">
+        <v>44</v>
+      </c>
+      <c r="B20" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C20" s="10" t="n">
+        <v>101</v>
+      </c>
+      <c r="D20" s="10" t="inlineStr">
+        <is>
+          <t>Ru</t>
+        </is>
+      </c>
+      <c r="E20" s="10" t="n">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B21" s="10" t="n">
+        <v>55</v>
+      </c>
+      <c r="C21" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E21" s="10" t="n">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="n">
+        <v>44</v>
+      </c>
+      <c r="B22" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C22" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D22" s="10" t="inlineStr">
+        <is>
+          <t>Ru</t>
+        </is>
+      </c>
+      <c r="E22" s="10" t="n">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B23" s="10" t="n">
+        <v>54</v>
+      </c>
+      <c r="C23" s="10" t="n">
+        <v>99</v>
+      </c>
+      <c r="D23" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E23" s="10" t="n">
+        <v>0.985</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B24" s="10" t="inlineStr"/>
+      <c r="C24" s="10" t="inlineStr"/>
+      <c r="D24" s="10" t="inlineStr"/>
+      <c r="E24" s="10" t="n">
+        <v>984.693</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>isotope</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
+        <is>
+          <t>x-section(mb)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B2" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="n">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <v>60</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="n">
+        <v>1.12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E5" s="10" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D7" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>60.6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="D9" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="D10" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="D11" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>2.24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="D12" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>19.1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B13" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E13" s="10" t="n">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B14" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E14" s="10" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B15" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="D15" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E15" s="10" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B16" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E16" s="10" t="n">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B17" s="10" t="n">
+        <v>55</v>
+      </c>
+      <c r="C17" s="10" t="n">
+        <v>102</v>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E17" s="10" t="n">
+        <v>85.2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B18" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C18" s="10" t="n">
+        <v>102</v>
+      </c>
+      <c r="D18" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E18" s="10" t="n">
+        <v>40.4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B19" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C19" s="10" t="n">
+        <v>101</v>
+      </c>
+      <c r="D19" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E19" s="10" t="n">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B20" s="10" t="n">
+        <v>55</v>
+      </c>
+      <c r="C20" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D20" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E20" s="10" t="n">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="n">
+        <v>44</v>
+      </c>
+      <c r="B21" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C21" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" s="10" t="inlineStr">
+        <is>
+          <t>Ru</t>
+        </is>
+      </c>
+      <c r="E21" s="10" t="n">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B22" s="10" t="n">
+        <v>54</v>
+      </c>
+      <c r="C22" s="10" t="n">
+        <v>99</v>
+      </c>
+      <c r="D22" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E22" s="10" t="n">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="n">
+        <v>44</v>
+      </c>
+      <c r="B23" s="10" t="n">
+        <v>55</v>
+      </c>
+      <c r="C23" s="10" t="n">
+        <v>99</v>
+      </c>
+      <c r="D23" s="10" t="inlineStr">
+        <is>
+          <t>Ru</t>
+        </is>
+      </c>
+      <c r="E23" s="10" t="n">
+        <v>2.24</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="n">
+        <v>43</v>
+      </c>
+      <c r="B24" s="10" t="n">
+        <v>54</v>
+      </c>
+      <c r="C24" s="10" t="n">
+        <v>97</v>
+      </c>
+      <c r="D24" s="10" t="inlineStr">
+        <is>
+          <t>Tc</t>
+        </is>
+      </c>
+      <c r="E24" s="10" t="n">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="10" t="n">
+        <v>41</v>
+      </c>
+      <c r="B25" s="10" t="n">
+        <v>53</v>
+      </c>
+      <c r="C25" s="10" t="n">
+        <v>94</v>
+      </c>
+      <c r="D25" s="10" t="inlineStr">
+        <is>
+          <t>Nb</t>
+        </is>
+      </c>
+      <c r="E25" s="10" t="n">
+        <v>1.12</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="10" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B26" s="10" t="inlineStr"/>
+      <c r="C26" s="10" t="inlineStr"/>
+      <c r="D26" s="10" t="inlineStr"/>
+      <c r="E26" s="10" t="n">
+        <v>1121.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="16" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="16" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>Z</t>
+        </is>
+      </c>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>isotope</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
+        <is>
+          <t>x-section(mb)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B2" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>108</v>
+      </c>
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="n">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <v>60</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>108</v>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>4.13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="E5" s="10" t="n">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <v>60</v>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="n">
+        <v>49</v>
+      </c>
+      <c r="B7" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D7" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>34.2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="B8" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>30.1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B9" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="D9" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B10" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="D10" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>8.85</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B11" s="10" t="n">
+        <v>59</v>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="D11" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="D12" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B13" s="10" t="n">
+        <v>58</v>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E13" s="10" t="n">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="n">
+        <v>47</v>
+      </c>
+      <c r="B14" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="E14" s="10" t="n">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="n">
+        <v>46</v>
+      </c>
+      <c r="B15" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="D15" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="E15" s="10" t="n">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B16" s="10" t="n">
+        <v>57</v>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>102</v>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E16" s="10" t="n">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="n">
+        <v>45</v>
+      </c>
+      <c r="B17" s="10" t="n">
+        <v>56</v>
+      </c>
+      <c r="C17" s="10" t="n">
+        <v>101</v>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="E17" s="10" t="n">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B18" s="10" t="inlineStr"/>
+      <c r="C18" s="10" t="inlineStr"/>
+      <c r="D18" s="10" t="inlineStr"/>
+      <c r="E18" s="10" t="n">
+        <v>590.221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add recoil energy for each isotopes (only in example.ipynb)
</commit_message>
<xml_diff>
--- a/example/DoesCal.xlsx
+++ b/example/DoesCal.xlsx
@@ -7,11 +7,11 @@
   </bookViews>
   <sheets>
     <sheet name="Initial" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="420.0MeV" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="333.0MeV" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="362.0MeV" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="391.0MeV" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="303.0MeV" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="0um_420MeV" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="9um_333MeV" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="6um_362MeV" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="3um_391MeV" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="12um_303MeV" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
@@ -781,7 +781,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -797,6 +797,7 @@
     <col width="16" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
+    <col width="16" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -827,15 +828,20 @@
       </c>
       <c r="F1" s="9" t="inlineStr">
         <is>
+          <t>Recoil_E(MeV)</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
           <t>t1/2</t>
         </is>
       </c>
-      <c r="G1" s="9" t="inlineStr">
+      <c r="H1" s="9" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="H1" s="9" t="inlineStr">
+      <c r="I1" s="9" t="inlineStr">
         <is>
           <t>t1/2(s)</t>
         </is>
@@ -860,14 +866,17 @@
         <v>40.6</v>
       </c>
       <c r="F2" s="10" t="n">
+        <v>303.520972972973</v>
+      </c>
+      <c r="G2" s="10" t="n">
         <v>6.2</v>
       </c>
-      <c r="G2" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I2" s="10" t="n">
         <v>372</v>
       </c>
     </row>
@@ -890,14 +899,17 @@
         <v>40.6</v>
       </c>
       <c r="F3" s="10" t="n">
+        <v>303.520972972973</v>
+      </c>
+      <c r="G3" s="10" t="n">
         <v>5.2</v>
       </c>
-      <c r="G3" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H3" s="10" t="n">
+      <c r="H3" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I3" s="10" t="n">
         <v>312</v>
       </c>
     </row>
@@ -920,14 +932,17 @@
         <v>62.7</v>
       </c>
       <c r="F4" s="10" t="n">
+        <v>303.520972972973</v>
+      </c>
+      <c r="G4" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="H4" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H4" s="10" t="n">
+      <c r="I4" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -950,14 +965,17 @@
         <v>8.609999999999999</v>
       </c>
       <c r="F5" s="10" t="n">
+        <v>303.520972972973</v>
+      </c>
+      <c r="G5" s="10" t="n">
         <v>23.96</v>
       </c>
-      <c r="G5" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H5" s="10" t="n">
+      <c r="H5" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I5" s="10" t="n">
         <v>1437.6</v>
       </c>
     </row>
@@ -980,14 +998,17 @@
         <v>8.609999999999999</v>
       </c>
       <c r="F6" s="10" t="n">
+        <v>303.520972972973</v>
+      </c>
+      <c r="G6" s="10" t="n">
         <v>8.279999999999999</v>
       </c>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="H6" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H6" s="10" t="n">
+      <c r="I6" s="10" t="n">
         <v>715392</v>
       </c>
     </row>
@@ -1010,14 +1031,17 @@
         <v>72.59999999999999</v>
       </c>
       <c r="F7" s="10" t="n">
+        <v>300.6575675675676</v>
+      </c>
+      <c r="G7" s="10" t="n">
         <v>5.07</v>
       </c>
-      <c r="G7" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H7" s="10" t="n">
+      <c r="H7" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I7" s="10" t="n">
         <v>304.2</v>
       </c>
     </row>
@@ -1040,14 +1064,17 @@
         <v>72.59999999999999</v>
       </c>
       <c r="F8" s="10" t="n">
+        <v>300.6575675675676</v>
+      </c>
+      <c r="G8" s="10" t="n">
         <v>48</v>
       </c>
-      <c r="G8" s="10" t="inlineStr">
+      <c r="H8" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H8" s="10" t="n">
+      <c r="I8" s="10" t="n">
         <v>48</v>
       </c>
     </row>
@@ -1070,14 +1097,17 @@
         <v>320</v>
       </c>
       <c r="F9" s="10" t="n">
+        <v>300.6575675675676</v>
+      </c>
+      <c r="G9" s="10" t="n">
         <v>55.5</v>
       </c>
-      <c r="G9" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H9" s="10" t="n">
+      <c r="H9" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I9" s="10" t="n">
         <v>3330</v>
       </c>
     </row>
@@ -1100,14 +1130,17 @@
         <v>68.90000000000001</v>
       </c>
       <c r="F10" s="10" t="n">
+        <v>300.6575675675676</v>
+      </c>
+      <c r="G10" s="10" t="n">
         <v>41.29</v>
       </c>
-      <c r="G10" s="10" t="inlineStr">
+      <c r="H10" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H10" s="10" t="n">
+      <c r="I10" s="10" t="n">
         <v>3567456</v>
       </c>
     </row>
@@ -1130,14 +1163,17 @@
         <v>68.90000000000001</v>
       </c>
       <c r="F11" s="10" t="n">
+        <v>300.6575675675676</v>
+      </c>
+      <c r="G11" s="10" t="n">
         <v>7.23</v>
       </c>
-      <c r="G11" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H11" s="10" t="n">
+      <c r="H11" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I11" s="10" t="n">
         <v>433.8</v>
       </c>
     </row>
@@ -1160,14 +1196,17 @@
         <v>3.69</v>
       </c>
       <c r="F12" s="10" t="n">
+        <v>300.6575675675676</v>
+      </c>
+      <c r="G12" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G12" s="10" t="inlineStr">
+      <c r="H12" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H12" s="10" t="n">
+      <c r="I12" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -1190,14 +1229,17 @@
         <v>4.92</v>
       </c>
       <c r="F13" s="10" t="n">
+        <v>297.7941621621621</v>
+      </c>
+      <c r="G13" s="10" t="n">
         <v>1.8</v>
       </c>
-      <c r="G13" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H13" s="10" t="n">
+      <c r="H13" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I13" s="10" t="n">
         <v>108</v>
       </c>
     </row>
@@ -1220,14 +1262,17 @@
         <v>51.7</v>
       </c>
       <c r="F14" s="10" t="n">
+        <v>297.7941621621621</v>
+      </c>
+      <c r="G14" s="10" t="n">
         <v>57.7</v>
       </c>
-      <c r="G14" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H14" s="10" t="n">
+      <c r="H14" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I14" s="10" t="n">
         <v>3462</v>
       </c>
     </row>
@@ -1250,14 +1295,17 @@
         <v>20.9</v>
       </c>
       <c r="F15" s="10" t="n">
+        <v>297.7941621621621</v>
+      </c>
+      <c r="G15" s="10" t="n">
         <v>69.2</v>
       </c>
-      <c r="G15" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H15" s="10" t="n">
+      <c r="H15" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="n">
         <v>4152</v>
       </c>
     </row>
@@ -1280,14 +1328,17 @@
         <v>20.9</v>
       </c>
       <c r="F16" s="10" t="n">
+        <v>297.7941621621621</v>
+      </c>
+      <c r="G16" s="10" t="n">
         <v>33.5</v>
       </c>
-      <c r="G16" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H16" s="10" t="n">
+      <c r="H16" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I16" s="10" t="n">
         <v>2010</v>
       </c>
     </row>
@@ -1310,14 +1361,17 @@
         <v>84.90000000000001</v>
       </c>
       <c r="F17" s="10" t="n">
+        <v>294.9307567567568</v>
+      </c>
+      <c r="G17" s="10" t="n">
         <v>65.7</v>
       </c>
-      <c r="G17" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H17" s="10" t="n">
+      <c r="H17" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I17" s="10" t="n">
         <v>3942</v>
       </c>
     </row>
@@ -1340,14 +1394,17 @@
         <v>43.1</v>
       </c>
       <c r="F18" s="10" t="n">
+        <v>294.9307567567568</v>
+      </c>
+      <c r="G18" s="10" t="n">
         <v>16.991</v>
       </c>
-      <c r="G18" s="10" t="inlineStr">
+      <c r="H18" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H18" s="10" t="n">
+      <c r="I18" s="10" t="n">
         <v>1468022.4</v>
       </c>
     </row>
@@ -1370,14 +1427,17 @@
         <v>4.92</v>
       </c>
       <c r="F19" s="10" t="n">
+        <v>294.9307567567568</v>
+      </c>
+      <c r="G19" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G19" s="10" t="inlineStr">
+      <c r="H19" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H19" s="10" t="n">
+      <c r="I19" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -1400,14 +1460,17 @@
         <v>4.92</v>
       </c>
       <c r="F20" s="10" t="n">
+        <v>294.9307567567568</v>
+      </c>
+      <c r="G20" s="10" t="n">
         <v>56.114</v>
       </c>
-      <c r="G20" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H20" s="10" t="n">
+      <c r="H20" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I20" s="10" t="n">
         <v>3366.84</v>
       </c>
     </row>
@@ -1430,14 +1493,17 @@
         <v>1.23</v>
       </c>
       <c r="F21" s="10" t="n">
+        <v>294.9307567567568</v>
+      </c>
+      <c r="G21" s="10" t="n">
         <v>39.247</v>
       </c>
-      <c r="G21" s="10" t="inlineStr">
+      <c r="H21" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H21" s="10" t="n">
+      <c r="I21" s="10" t="n">
         <v>3390940.8</v>
       </c>
     </row>
@@ -1460,14 +1526,17 @@
         <v>157</v>
       </c>
       <c r="F22" s="10" t="n">
+        <v>292.0673513513514</v>
+      </c>
+      <c r="G22" s="10" t="n">
         <v>12.9</v>
       </c>
-      <c r="G22" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H22" s="10" t="n">
+      <c r="H22" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I22" s="10" t="n">
         <v>774</v>
       </c>
     </row>
@@ -1490,14 +1559,17 @@
         <v>157</v>
       </c>
       <c r="F23" s="10" t="n">
+        <v>292.0673513513514</v>
+      </c>
+      <c r="G23" s="10" t="n">
         <v>7.7</v>
       </c>
-      <c r="G23" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H23" s="10" t="n">
+      <c r="H23" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I23" s="10" t="n">
         <v>462</v>
       </c>
     </row>
@@ -1520,14 +1592,17 @@
         <v>135</v>
       </c>
       <c r="F24" s="10" t="n">
+        <v>292.0673513513514</v>
+      </c>
+      <c r="G24" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G24" s="10" t="inlineStr">
+      <c r="H24" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H24" s="10" t="n">
+      <c r="I24" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -1550,14 +1625,17 @@
         <v>17.2</v>
       </c>
       <c r="F25" s="10" t="n">
+        <v>292.0673513513514</v>
+      </c>
+      <c r="G25" s="10" t="n">
         <v>207.3</v>
       </c>
-      <c r="G25" s="10" t="inlineStr">
+      <c r="H25" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H25" s="10" t="n">
+      <c r="I25" s="10" t="n">
         <v>17910720</v>
       </c>
     </row>
@@ -1580,14 +1658,17 @@
         <v>17.2</v>
       </c>
       <c r="F26" s="10" t="n">
+        <v>292.0673513513514</v>
+      </c>
+      <c r="G26" s="10" t="n">
         <v>3.742</v>
       </c>
-      <c r="G26" s="10" t="inlineStr">
+      <c r="H26" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H26" s="10" t="n">
+      <c r="I26" s="10" t="n">
         <v>118007712</v>
       </c>
     </row>
@@ -1610,14 +1691,17 @@
         <v>4.92</v>
       </c>
       <c r="F27" s="10" t="n">
+        <v>289.203945945946</v>
+      </c>
+      <c r="G27" s="10" t="n">
         <v>11.1</v>
       </c>
-      <c r="G27" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H27" s="10" t="n">
+      <c r="H27" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I27" s="10" t="n">
         <v>666</v>
       </c>
     </row>
@@ -1640,14 +1724,17 @@
         <v>11.1</v>
       </c>
       <c r="F28" s="10" t="n">
+        <v>289.203945945946</v>
+      </c>
+      <c r="G28" s="10" t="n">
         <v>8.470000000000001</v>
       </c>
-      <c r="G28" s="10" t="inlineStr">
+      <c r="H28" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H28" s="10" t="n">
+      <c r="I28" s="10" t="n">
         <v>30492</v>
       </c>
     </row>
@@ -1670,14 +1757,17 @@
         <v>1.23</v>
       </c>
       <c r="F29" s="10" t="n">
+        <v>289.203945945946</v>
+      </c>
+      <c r="G29" s="10" t="n">
         <v>3.3</v>
       </c>
-      <c r="G29" s="10" t="inlineStr">
+      <c r="H29" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H29" s="10" t="n">
+      <c r="I29" s="10" t="n">
         <v>104068800</v>
       </c>
     </row>
@@ -1700,14 +1790,17 @@
         <v>1.23</v>
       </c>
       <c r="F30" s="10" t="n">
+        <v>289.203945945946</v>
+      </c>
+      <c r="G30" s="10" t="n">
         <v>4.34</v>
       </c>
-      <c r="G30" s="10" t="inlineStr">
+      <c r="H30" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H30" s="10" t="n">
+      <c r="I30" s="10" t="n">
         <v>374976</v>
       </c>
     </row>
@@ -1730,14 +1823,17 @@
         <v>33.2</v>
       </c>
       <c r="F31" s="10" t="n">
+        <v>286.3405405405405</v>
+      </c>
+      <c r="G31" s="10" t="n">
         <v>20.5</v>
       </c>
-      <c r="G31" s="10" t="inlineStr">
+      <c r="H31" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H31" s="10" t="n">
+      <c r="I31" s="10" t="n">
         <v>73800</v>
       </c>
     </row>
@@ -1760,14 +1856,17 @@
         <v>33.2</v>
       </c>
       <c r="F32" s="10" t="n">
+        <v>286.3405405405405</v>
+      </c>
+      <c r="G32" s="10" t="n">
         <v>4.6</v>
       </c>
-      <c r="G32" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H32" s="10" t="n">
+      <c r="H32" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I32" s="10" t="n">
         <v>276</v>
       </c>
     </row>
@@ -1790,14 +1889,17 @@
         <v>7.38</v>
       </c>
       <c r="F33" s="10" t="n">
+        <v>286.3405405405405</v>
+      </c>
+      <c r="G33" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G33" s="10" t="inlineStr">
+      <c r="H33" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H33" s="10" t="n">
+      <c r="I33" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -1820,14 +1922,17 @@
         <v>52.9</v>
       </c>
       <c r="F34" s="10" t="n">
+        <v>283.4771351351351</v>
+      </c>
+      <c r="G34" s="10" t="n">
         <v>16.1</v>
       </c>
-      <c r="G34" s="10" t="inlineStr">
+      <c r="H34" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H34" s="10" t="n">
+      <c r="I34" s="10" t="n">
         <v>1391040</v>
       </c>
     </row>
@@ -1850,14 +1955,17 @@
         <v>52.9</v>
       </c>
       <c r="F35" s="10" t="n">
+        <v>283.4771351351351</v>
+      </c>
+      <c r="G35" s="10" t="n">
         <v>4.7</v>
       </c>
-      <c r="G35" s="10" t="inlineStr">
+      <c r="H35" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H35" s="10" t="n">
+      <c r="I35" s="10" t="n">
         <v>16920</v>
       </c>
     </row>
@@ -1880,14 +1988,17 @@
         <v>12.3</v>
       </c>
       <c r="F36" s="10" t="n">
+        <v>283.4771351351351</v>
+      </c>
+      <c r="G36" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G36" s="10" t="inlineStr">
+      <c r="H36" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H36" s="10" t="n">
+      <c r="I36" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -1910,14 +2021,17 @@
         <v>1.23</v>
       </c>
       <c r="F37" s="10" t="n">
+        <v>280.6137297297298</v>
+      </c>
+      <c r="G37" s="10" t="n">
         <v>8.720000000000001</v>
       </c>
-      <c r="G37" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H37" s="10" t="n">
+      <c r="H37" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I37" s="10" t="n">
         <v>523.2</v>
       </c>
     </row>
@@ -1940,14 +2054,17 @@
         <v>1.23</v>
       </c>
       <c r="F38" s="10" t="n">
+        <v>280.6137297297298</v>
+      </c>
+      <c r="G38" s="10" t="n">
         <v>3.6</v>
       </c>
-      <c r="G38" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H38" s="10" t="n">
+      <c r="H38" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I38" s="10" t="n">
         <v>216</v>
       </c>
     </row>
@@ -1970,14 +2087,17 @@
         <v>2.46</v>
       </c>
       <c r="F39" s="10" t="n">
+        <v>280.6137297297298</v>
+      </c>
+      <c r="G39" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G39" s="10" t="inlineStr">
+      <c r="H39" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H39" s="10" t="n">
+      <c r="I39" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -2000,14 +2120,17 @@
         <v>2.46</v>
       </c>
       <c r="F40" s="10" t="n">
+        <v>277.7503243243243</v>
+      </c>
+      <c r="G40" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="G40" s="10" t="inlineStr">
+      <c r="H40" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H40" s="10" t="n">
+      <c r="I40" s="10" t="n">
         <v>189216000</v>
       </c>
     </row>
@@ -2030,14 +2153,17 @@
         <v>2.46</v>
       </c>
       <c r="F41" s="10" t="n">
+        <v>277.7503243243243</v>
+      </c>
+      <c r="G41" s="10" t="n">
         <v>91</v>
       </c>
-      <c r="G41" s="10" t="inlineStr">
+      <c r="H41" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H41" s="10" t="n">
+      <c r="I41" s="10" t="n">
         <v>7862400</v>
       </c>
     </row>
@@ -2060,14 +2186,17 @@
         <v>2.46</v>
       </c>
       <c r="F42" s="10" t="n">
+        <v>274.8869189189189</v>
+      </c>
+      <c r="G42" s="10" t="n">
         <v>4.28</v>
       </c>
-      <c r="G42" s="10" t="inlineStr">
+      <c r="H42" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H42" s="10" t="n">
+      <c r="I42" s="10" t="n">
         <v>369792</v>
       </c>
     </row>
@@ -2090,14 +2219,17 @@
         <v>2.46</v>
       </c>
       <c r="F43" s="10" t="n">
+        <v>274.8869189189189</v>
+      </c>
+      <c r="G43" s="10" t="n">
         <v>51.5</v>
       </c>
-      <c r="G43" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H43" s="10" t="n">
+      <c r="H43" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I43" s="10" t="n">
         <v>3090</v>
       </c>
     </row>
@@ -2113,11 +2245,12 @@
       <c r="E44" s="10" t="n">
         <v>1230.27</v>
       </c>
-      <c r="F44" s="10" t="n">
+      <c r="F44" s="10" t="inlineStr"/>
+      <c r="G44" s="10" t="n">
         <v>-1</v>
       </c>
-      <c r="G44" s="10" t="inlineStr"/>
-      <c r="H44" s="10" t="n">
+      <c r="H44" s="10" t="inlineStr"/>
+      <c r="I44" s="10" t="n">
         <v>-1</v>
       </c>
     </row>
@@ -2132,7 +2265,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2148,6 +2281,7 @@
     <col width="16" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
+    <col width="16" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2178,15 +2312,20 @@
       </c>
       <c r="F1" s="9" t="inlineStr">
         <is>
+          <t>Recoil_E(MeV)</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
           <t>t1/2</t>
         </is>
       </c>
-      <c r="G1" s="9" t="inlineStr">
+      <c r="H1" s="9" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="H1" s="9" t="inlineStr">
+      <c r="I1" s="9" t="inlineStr">
         <is>
           <t>t1/2(s)</t>
         </is>
@@ -2211,14 +2350,17 @@
         <v>1.63</v>
       </c>
       <c r="F2" s="10" t="n">
+        <v>245.1891891891892</v>
+      </c>
+      <c r="G2" s="10" t="n">
         <v>58</v>
       </c>
-      <c r="G2" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I2" s="10" t="n">
         <v>3480</v>
       </c>
     </row>
@@ -2241,14 +2383,17 @@
         <v>1.63</v>
       </c>
       <c r="F3" s="10" t="n">
+        <v>245.1891891891892</v>
+      </c>
+      <c r="G3" s="10" t="n">
         <v>39.6</v>
       </c>
-      <c r="G3" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H3" s="10" t="n">
+      <c r="H3" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I3" s="10" t="n">
         <v>2376</v>
       </c>
     </row>
@@ -2271,14 +2416,17 @@
         <v>132</v>
       </c>
       <c r="F4" s="10" t="n">
+        <v>242.9189189189189</v>
+      </c>
+      <c r="G4" s="10" t="n">
         <v>32.4</v>
       </c>
-      <c r="G4" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H4" s="10" t="n">
+      <c r="H4" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I4" s="10" t="n">
         <v>1944</v>
       </c>
     </row>
@@ -2301,14 +2449,17 @@
         <v>132</v>
       </c>
       <c r="F5" s="10" t="n">
+        <v>242.9189189189189</v>
+      </c>
+      <c r="G5" s="10" t="n">
         <v>50.4</v>
       </c>
-      <c r="G5" s="10" t="inlineStr">
+      <c r="H5" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H5" s="10" t="n">
+      <c r="I5" s="10" t="n">
         <v>50.4</v>
       </c>
     </row>
@@ -2331,14 +2482,17 @@
         <v>75.7</v>
       </c>
       <c r="F6" s="10" t="n">
+        <v>242.9189189189189</v>
+      </c>
+      <c r="G6" s="10" t="n">
         <v>6.5</v>
       </c>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="H6" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H6" s="10" t="n">
+      <c r="I6" s="10" t="n">
         <v>23400</v>
       </c>
     </row>
@@ -2361,14 +2515,17 @@
         <v>10.6</v>
       </c>
       <c r="F7" s="10" t="n">
+        <v>242.9189189189189</v>
+      </c>
+      <c r="G7" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G7" s="10" t="inlineStr">
+      <c r="H7" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H7" s="10" t="n">
+      <c r="I7" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -2391,14 +2548,17 @@
         <v>10.6</v>
       </c>
       <c r="F8" s="10" t="n">
+        <v>242.9189189189189</v>
+      </c>
+      <c r="G8" s="10" t="n">
         <v>44.3</v>
       </c>
-      <c r="G8" s="10" t="inlineStr">
+      <c r="H8" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H8" s="10" t="n">
+      <c r="I8" s="10" t="n">
         <v>44.3</v>
       </c>
     </row>
@@ -2421,14 +2581,17 @@
         <v>160</v>
       </c>
       <c r="F9" s="10" t="n">
+        <v>240.6486486486486</v>
+      </c>
+      <c r="G9" s="10" t="n">
         <v>6.2</v>
       </c>
-      <c r="G9" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H9" s="10" t="n">
+      <c r="H9" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I9" s="10" t="n">
         <v>372</v>
       </c>
     </row>
@@ -2451,14 +2614,17 @@
         <v>160</v>
       </c>
       <c r="F10" s="10" t="n">
+        <v>240.6486486486486</v>
+      </c>
+      <c r="G10" s="10" t="n">
         <v>5.2</v>
       </c>
-      <c r="G10" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H10" s="10" t="n">
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I10" s="10" t="n">
         <v>312</v>
       </c>
     </row>
@@ -2481,14 +2647,17 @@
         <v>210</v>
       </c>
       <c r="F11" s="10" t="n">
+        <v>240.6486486486486</v>
+      </c>
+      <c r="G11" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G11" s="10" t="inlineStr">
+      <c r="H11" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H11" s="10" t="n">
+      <c r="I11" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -2511,14 +2680,17 @@
         <v>10.6</v>
       </c>
       <c r="F12" s="10" t="n">
+        <v>240.6486486486486</v>
+      </c>
+      <c r="G12" s="10" t="n">
         <v>23.96</v>
       </c>
-      <c r="G12" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H12" s="10" t="n">
+      <c r="H12" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I12" s="10" t="n">
         <v>1437.6</v>
       </c>
     </row>
@@ -2541,14 +2713,17 @@
         <v>10.6</v>
       </c>
       <c r="F13" s="10" t="n">
+        <v>240.6486486486486</v>
+      </c>
+      <c r="G13" s="10" t="n">
         <v>8.279999999999999</v>
       </c>
-      <c r="G13" s="10" t="inlineStr">
+      <c r="H13" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H13" s="10" t="n">
+      <c r="I13" s="10" t="n">
         <v>715392</v>
       </c>
     </row>
@@ -2571,14 +2746,17 @@
         <v>0.8129999999999999</v>
       </c>
       <c r="F14" s="10" t="n">
+        <v>240.6486486486486</v>
+      </c>
+      <c r="G14" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G14" s="10" t="inlineStr">
+      <c r="H14" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H14" s="10" t="n">
+      <c r="I14" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -2601,14 +2779,17 @@
         <v>2.44</v>
       </c>
       <c r="F15" s="10" t="n">
+        <v>238.3783783783784</v>
+      </c>
+      <c r="G15" s="10" t="n">
         <v>5.07</v>
       </c>
-      <c r="G15" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H15" s="10" t="n">
+      <c r="H15" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I15" s="10" t="n">
         <v>304.2</v>
       </c>
     </row>
@@ -2631,14 +2812,17 @@
         <v>2.44</v>
       </c>
       <c r="F16" s="10" t="n">
+        <v>238.3783783783784</v>
+      </c>
+      <c r="G16" s="10" t="n">
         <v>48</v>
       </c>
-      <c r="G16" s="10" t="inlineStr">
+      <c r="H16" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H16" s="10" t="n">
+      <c r="I16" s="10" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2661,14 +2845,17 @@
         <v>86.2</v>
       </c>
       <c r="F17" s="10" t="n">
+        <v>236.1081081081081</v>
+      </c>
+      <c r="G17" s="10" t="n">
         <v>69.2</v>
       </c>
-      <c r="G17" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H17" s="10" t="n">
+      <c r="H17" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I17" s="10" t="n">
         <v>4152</v>
       </c>
     </row>
@@ -2691,14 +2878,17 @@
         <v>86.2</v>
       </c>
       <c r="F18" s="10" t="n">
+        <v>236.1081081081081</v>
+      </c>
+      <c r="G18" s="10" t="n">
         <v>33.5</v>
       </c>
-      <c r="G18" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H18" s="10" t="n">
+      <c r="H18" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I18" s="10" t="n">
         <v>2010</v>
       </c>
     </row>
@@ -2721,14 +2911,17 @@
         <v>24.4</v>
       </c>
       <c r="F19" s="10" t="n">
+        <v>236.1081081081081</v>
+      </c>
+      <c r="G19" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G19" s="10" t="inlineStr">
+      <c r="H19" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H19" s="10" t="n">
+      <c r="I19" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -2751,14 +2944,17 @@
         <v>69.09999999999999</v>
       </c>
       <c r="F20" s="10" t="n">
+        <v>233.8378378378378</v>
+      </c>
+      <c r="G20" s="10" t="n">
         <v>65.7</v>
       </c>
-      <c r="G20" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H20" s="10" t="n">
+      <c r="H20" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I20" s="10" t="n">
         <v>3942</v>
       </c>
     </row>
@@ -2781,14 +2977,17 @@
         <v>13</v>
       </c>
       <c r="F21" s="10" t="n">
+        <v>233.8378378378378</v>
+      </c>
+      <c r="G21" s="10" t="n">
         <v>16.991</v>
       </c>
-      <c r="G21" s="10" t="inlineStr">
+      <c r="H21" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H21" s="10" t="n">
+      <c r="I21" s="10" t="n">
         <v>1468022.4</v>
       </c>
     </row>
@@ -2811,14 +3010,17 @@
         <v>10.6</v>
       </c>
       <c r="F22" s="10" t="n">
+        <v>229.2972972972973</v>
+      </c>
+      <c r="G22" s="10" t="n">
         <v>3.3</v>
       </c>
-      <c r="G22" s="10" t="inlineStr">
+      <c r="H22" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H22" s="10" t="n">
+      <c r="I22" s="10" t="n">
         <v>104068800</v>
       </c>
     </row>
@@ -2841,14 +3043,17 @@
         <v>10.6</v>
       </c>
       <c r="F23" s="10" t="n">
+        <v>229.2972972972973</v>
+      </c>
+      <c r="G23" s="10" t="n">
         <v>4.34</v>
       </c>
-      <c r="G23" s="10" t="inlineStr">
+      <c r="H23" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H23" s="10" t="n">
+      <c r="I23" s="10" t="n">
         <v>374976</v>
       </c>
     </row>
@@ -2871,14 +3076,17 @@
         <v>0.8129999999999999</v>
       </c>
       <c r="F24" s="10" t="n">
+        <v>229.2972972972973</v>
+      </c>
+      <c r="G24" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G24" s="10" t="inlineStr">
+      <c r="H24" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H24" s="10" t="n">
+      <c r="I24" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -2901,14 +3109,17 @@
         <v>4.88</v>
       </c>
       <c r="F25" s="10" t="n">
+        <v>227.027027027027</v>
+      </c>
+      <c r="G25" s="10" t="n">
         <v>20.5</v>
       </c>
-      <c r="G25" s="10" t="inlineStr">
+      <c r="H25" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H25" s="10" t="n">
+      <c r="I25" s="10" t="n">
         <v>73800</v>
       </c>
     </row>
@@ -2931,14 +3142,17 @@
         <v>4.88</v>
       </c>
       <c r="F26" s="10" t="n">
+        <v>227.027027027027</v>
+      </c>
+      <c r="G26" s="10" t="n">
         <v>4.6</v>
       </c>
-      <c r="G26" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H26" s="10" t="n">
+      <c r="H26" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I26" s="10" t="n">
         <v>276</v>
       </c>
     </row>
@@ -2961,14 +3175,17 @@
         <v>0.8129999999999999</v>
       </c>
       <c r="F27" s="10" t="n">
+        <v>222.4864864864865</v>
+      </c>
+      <c r="G27" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="G27" s="10" t="inlineStr">
+      <c r="H27" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H27" s="10" t="n">
+      <c r="I27" s="10" t="n">
         <v>189216000</v>
       </c>
     </row>
@@ -2984,11 +3201,12 @@
       <c r="E28" s="10" t="n">
         <v>813.499</v>
       </c>
-      <c r="F28" s="10" t="n">
+      <c r="F28" s="10" t="inlineStr"/>
+      <c r="G28" s="10" t="n">
         <v>-1</v>
       </c>
-      <c r="G28" s="10" t="inlineStr"/>
-      <c r="H28" s="10" t="n">
+      <c r="H28" s="10" t="inlineStr"/>
+      <c r="I28" s="10" t="n">
         <v>-1</v>
       </c>
     </row>
@@ -3003,7 +3221,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3019,6 +3237,7 @@
     <col width="16" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
+    <col width="16" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3049,15 +3268,20 @@
       </c>
       <c r="F1" s="9" t="inlineStr">
         <is>
+          <t>Recoil_E(MeV)</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
           <t>t1/2</t>
         </is>
       </c>
-      <c r="G1" s="9" t="inlineStr">
+      <c r="H1" s="9" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="H1" s="9" t="inlineStr">
+      <c r="I1" s="9" t="inlineStr">
         <is>
           <t>t1/2(s)</t>
         </is>
@@ -3082,14 +3306,17 @@
         <v>37.4</v>
       </c>
       <c r="F2" s="10" t="n">
+        <v>264.0740720720721</v>
+      </c>
+      <c r="G2" s="10" t="n">
         <v>32.4</v>
       </c>
-      <c r="G2" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I2" s="10" t="n">
         <v>1944</v>
       </c>
     </row>
@@ -3112,14 +3339,17 @@
         <v>37.4</v>
       </c>
       <c r="F3" s="10" t="n">
+        <v>264.0740720720721</v>
+      </c>
+      <c r="G3" s="10" t="n">
         <v>50.4</v>
       </c>
-      <c r="G3" s="10" t="inlineStr">
+      <c r="H3" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H3" s="10" t="n">
+      <c r="I3" s="10" t="n">
         <v>50.4</v>
       </c>
     </row>
@@ -3142,14 +3372,17 @@
         <v>21.7</v>
       </c>
       <c r="F4" s="10" t="n">
+        <v>264.0740720720721</v>
+      </c>
+      <c r="G4" s="10" t="n">
         <v>6.5</v>
       </c>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="H4" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H4" s="10" t="n">
+      <c r="I4" s="10" t="n">
         <v>23400</v>
       </c>
     </row>
@@ -3172,14 +3405,17 @@
         <v>1.97</v>
       </c>
       <c r="F5" s="10" t="n">
+        <v>264.0740720720721</v>
+      </c>
+      <c r="G5" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G5" s="10" t="inlineStr">
+      <c r="H5" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H5" s="10" t="n">
+      <c r="I5" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -3202,14 +3438,17 @@
         <v>1.97</v>
       </c>
       <c r="F6" s="10" t="n">
+        <v>264.0740720720721</v>
+      </c>
+      <c r="G6" s="10" t="n">
         <v>44.3</v>
       </c>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="H6" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H6" s="10" t="n">
+      <c r="I6" s="10" t="n">
         <v>44.3</v>
       </c>
     </row>
@@ -3232,14 +3471,17 @@
         <v>179</v>
       </c>
       <c r="F7" s="10" t="n">
+        <v>261.6060900900901</v>
+      </c>
+      <c r="G7" s="10" t="n">
         <v>6.2</v>
       </c>
-      <c r="G7" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H7" s="10" t="n">
+      <c r="H7" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I7" s="10" t="n">
         <v>372</v>
       </c>
     </row>
@@ -3262,14 +3504,17 @@
         <v>179</v>
       </c>
       <c r="F8" s="10" t="n">
+        <v>261.6060900900901</v>
+      </c>
+      <c r="G8" s="10" t="n">
         <v>5.2</v>
       </c>
-      <c r="G8" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H8" s="10" t="n">
+      <c r="H8" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I8" s="10" t="n">
         <v>312</v>
       </c>
     </row>
@@ -3292,14 +3537,17 @@
         <v>303</v>
       </c>
       <c r="F9" s="10" t="n">
+        <v>261.6060900900901</v>
+      </c>
+      <c r="G9" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G9" s="10" t="inlineStr">
+      <c r="H9" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H9" s="10" t="n">
+      <c r="I9" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -3322,14 +3570,17 @@
         <v>33.5</v>
       </c>
       <c r="F10" s="10" t="n">
+        <v>261.6060900900901</v>
+      </c>
+      <c r="G10" s="10" t="n">
         <v>23.96</v>
       </c>
-      <c r="G10" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H10" s="10" t="n">
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I10" s="10" t="n">
         <v>1437.6</v>
       </c>
     </row>
@@ -3352,14 +3603,17 @@
         <v>33.5</v>
       </c>
       <c r="F11" s="10" t="n">
+        <v>261.6060900900901</v>
+      </c>
+      <c r="G11" s="10" t="n">
         <v>8.279999999999999</v>
       </c>
-      <c r="G11" s="10" t="inlineStr">
+      <c r="H11" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H11" s="10" t="n">
+      <c r="I11" s="10" t="n">
         <v>715392</v>
       </c>
     </row>
@@ -3382,14 +3636,17 @@
         <v>15.8</v>
       </c>
       <c r="F12" s="10" t="n">
+        <v>259.1381081081082</v>
+      </c>
+      <c r="G12" s="10" t="n">
         <v>5.07</v>
       </c>
-      <c r="G12" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H12" s="10" t="n">
+      <c r="H12" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I12" s="10" t="n">
         <v>304.2</v>
       </c>
     </row>
@@ -3412,14 +3669,17 @@
         <v>15.8</v>
       </c>
       <c r="F13" s="10" t="n">
+        <v>259.1381081081082</v>
+      </c>
+      <c r="G13" s="10" t="n">
         <v>48</v>
       </c>
-      <c r="G13" s="10" t="inlineStr">
+      <c r="H13" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H13" s="10" t="n">
+      <c r="I13" s="10" t="n">
         <v>48</v>
       </c>
     </row>
@@ -3442,14 +3702,17 @@
         <v>38.4</v>
       </c>
       <c r="F14" s="10" t="n">
+        <v>259.1381081081082</v>
+      </c>
+      <c r="G14" s="10" t="n">
         <v>55.5</v>
       </c>
-      <c r="G14" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H14" s="10" t="n">
+      <c r="H14" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I14" s="10" t="n">
         <v>3330</v>
       </c>
     </row>
@@ -3472,14 +3735,17 @@
         <v>9.85</v>
       </c>
       <c r="F15" s="10" t="n">
+        <v>259.1381081081082</v>
+      </c>
+      <c r="G15" s="10" t="n">
         <v>41.29</v>
       </c>
-      <c r="G15" s="10" t="inlineStr">
+      <c r="H15" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H15" s="10" t="n">
+      <c r="I15" s="10" t="n">
         <v>3567456</v>
       </c>
     </row>
@@ -3502,14 +3768,17 @@
         <v>9.85</v>
       </c>
       <c r="F16" s="10" t="n">
+        <v>259.1381081081082</v>
+      </c>
+      <c r="G16" s="10" t="n">
         <v>7.23</v>
       </c>
-      <c r="G16" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H16" s="10" t="n">
+      <c r="H16" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I16" s="10" t="n">
         <v>433.8</v>
       </c>
     </row>
@@ -3532,14 +3801,17 @@
         <v>50.2</v>
       </c>
       <c r="F17" s="10" t="n">
+        <v>256.6701261261261</v>
+      </c>
+      <c r="G17" s="10" t="n">
         <v>69.2</v>
       </c>
-      <c r="G17" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H17" s="10" t="n">
+      <c r="H17" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I17" s="10" t="n">
         <v>4152</v>
       </c>
     </row>
@@ -3562,14 +3834,17 @@
         <v>50.2</v>
       </c>
       <c r="F18" s="10" t="n">
+        <v>256.6701261261261</v>
+      </c>
+      <c r="G18" s="10" t="n">
         <v>33.5</v>
       </c>
-      <c r="G18" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H18" s="10" t="n">
+      <c r="H18" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I18" s="10" t="n">
         <v>2010</v>
       </c>
     </row>
@@ -3592,14 +3867,17 @@
         <v>15.8</v>
       </c>
       <c r="F19" s="10" t="n">
+        <v>256.6701261261261</v>
+      </c>
+      <c r="G19" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G19" s="10" t="inlineStr">
+      <c r="H19" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H19" s="10" t="n">
+      <c r="I19" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -3622,14 +3900,17 @@
         <v>163</v>
       </c>
       <c r="F20" s="10" t="n">
+        <v>254.2021441441442</v>
+      </c>
+      <c r="G20" s="10" t="n">
         <v>65.7</v>
       </c>
-      <c r="G20" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H20" s="10" t="n">
+      <c r="H20" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I20" s="10" t="n">
         <v>3942</v>
       </c>
     </row>
@@ -3652,14 +3933,17 @@
         <v>57.1</v>
       </c>
       <c r="F21" s="10" t="n">
+        <v>254.2021441441442</v>
+      </c>
+      <c r="G21" s="10" t="n">
         <v>16.991</v>
       </c>
-      <c r="G21" s="10" t="inlineStr">
+      <c r="H21" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H21" s="10" t="n">
+      <c r="I21" s="10" t="n">
         <v>1468022.4</v>
       </c>
     </row>
@@ -3682,14 +3966,17 @@
         <v>1.97</v>
       </c>
       <c r="F22" s="10" t="n">
+        <v>254.2021441441442</v>
+      </c>
+      <c r="G22" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G22" s="10" t="inlineStr">
+      <c r="H22" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H22" s="10" t="n">
+      <c r="I22" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -3712,14 +3999,17 @@
         <v>1.97</v>
       </c>
       <c r="F23" s="10" t="n">
+        <v>254.2021441441442</v>
+      </c>
+      <c r="G23" s="10" t="n">
         <v>56.114</v>
       </c>
-      <c r="G23" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H23" s="10" t="n">
+      <c r="H23" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I23" s="10" t="n">
         <v>3366.84</v>
       </c>
     </row>
@@ -3742,14 +4032,17 @@
         <v>10.8</v>
       </c>
       <c r="F24" s="10" t="n">
+        <v>251.7341621621622</v>
+      </c>
+      <c r="G24" s="10" t="n">
         <v>12.9</v>
       </c>
-      <c r="G24" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H24" s="10" t="n">
+      <c r="H24" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I24" s="10" t="n">
         <v>774</v>
       </c>
     </row>
@@ -3772,14 +4065,17 @@
         <v>10.8</v>
       </c>
       <c r="F25" s="10" t="n">
+        <v>251.7341621621622</v>
+      </c>
+      <c r="G25" s="10" t="n">
         <v>7.7</v>
       </c>
-      <c r="G25" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H25" s="10" t="n">
+      <c r="H25" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I25" s="10" t="n">
         <v>462</v>
       </c>
     </row>
@@ -3802,14 +4098,17 @@
         <v>5.91</v>
       </c>
       <c r="F26" s="10" t="n">
+        <v>251.7341621621622</v>
+      </c>
+      <c r="G26" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G26" s="10" t="inlineStr">
+      <c r="H26" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H26" s="10" t="n">
+      <c r="I26" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -3832,14 +4131,17 @@
         <v>1.97</v>
       </c>
       <c r="F27" s="10" t="n">
+        <v>251.7341621621622</v>
+      </c>
+      <c r="G27" s="10" t="n">
         <v>207.3</v>
       </c>
-      <c r="G27" s="10" t="inlineStr">
+      <c r="H27" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H27" s="10" t="n">
+      <c r="I27" s="10" t="n">
         <v>17910720</v>
       </c>
     </row>
@@ -3862,14 +4164,17 @@
         <v>1.97</v>
       </c>
       <c r="F28" s="10" t="n">
+        <v>251.7341621621622</v>
+      </c>
+      <c r="G28" s="10" t="n">
         <v>3.742</v>
       </c>
-      <c r="G28" s="10" t="inlineStr">
+      <c r="H28" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H28" s="10" t="n">
+      <c r="I28" s="10" t="n">
         <v>118007712</v>
       </c>
     </row>
@@ -3892,14 +4197,17 @@
         <v>10.8</v>
       </c>
       <c r="F29" s="10" t="n">
+        <v>249.2661801801802</v>
+      </c>
+      <c r="G29" s="10" t="n">
         <v>3.3</v>
       </c>
-      <c r="G29" s="10" t="inlineStr">
+      <c r="H29" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H29" s="10" t="n">
+      <c r="I29" s="10" t="n">
         <v>104068800</v>
       </c>
     </row>
@@ -3922,14 +4230,17 @@
         <v>10.8</v>
       </c>
       <c r="F30" s="10" t="n">
+        <v>249.2661801801802</v>
+      </c>
+      <c r="G30" s="10" t="n">
         <v>4.34</v>
       </c>
-      <c r="G30" s="10" t="inlineStr">
+      <c r="H30" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H30" s="10" t="n">
+      <c r="I30" s="10" t="n">
         <v>374976</v>
       </c>
     </row>
@@ -3952,14 +4263,17 @@
         <v>1.97</v>
       </c>
       <c r="F31" s="10" t="n">
+        <v>249.2661801801802</v>
+      </c>
+      <c r="G31" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G31" s="10" t="inlineStr">
+      <c r="H31" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H31" s="10" t="n">
+      <c r="I31" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -3982,14 +4296,17 @@
         <v>20.7</v>
       </c>
       <c r="F32" s="10" t="n">
+        <v>246.7981981981982</v>
+      </c>
+      <c r="G32" s="10" t="n">
         <v>20.5</v>
       </c>
-      <c r="G32" s="10" t="inlineStr">
+      <c r="H32" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H32" s="10" t="n">
+      <c r="I32" s="10" t="n">
         <v>73800</v>
       </c>
     </row>
@@ -4012,14 +4329,17 @@
         <v>20.7</v>
       </c>
       <c r="F33" s="10" t="n">
+        <v>246.7981981981982</v>
+      </c>
+      <c r="G33" s="10" t="n">
         <v>4.6</v>
       </c>
-      <c r="G33" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H33" s="10" t="n">
+      <c r="H33" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I33" s="10" t="n">
         <v>276</v>
       </c>
     </row>
@@ -4042,14 +4362,17 @@
         <v>1.97</v>
       </c>
       <c r="F34" s="10" t="n">
+        <v>246.7981981981982</v>
+      </c>
+      <c r="G34" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G34" s="10" t="inlineStr">
+      <c r="H34" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H34" s="10" t="n">
+      <c r="I34" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -4072,14 +4395,17 @@
         <v>0.985</v>
       </c>
       <c r="F35" s="10" t="n">
+        <v>244.3302162162163</v>
+      </c>
+      <c r="G35" s="10" t="n">
         <v>16.1</v>
       </c>
-      <c r="G35" s="10" t="inlineStr">
+      <c r="H35" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H35" s="10" t="n">
+      <c r="I35" s="10" t="n">
         <v>1391040</v>
       </c>
     </row>
@@ -4102,14 +4428,17 @@
         <v>0.985</v>
       </c>
       <c r="F36" s="10" t="n">
+        <v>244.3302162162163</v>
+      </c>
+      <c r="G36" s="10" t="n">
         <v>4.7</v>
       </c>
-      <c r="G36" s="10" t="inlineStr">
+      <c r="H36" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H36" s="10" t="n">
+      <c r="I36" s="10" t="n">
         <v>16920</v>
       </c>
     </row>
@@ -4125,11 +4454,12 @@
       <c r="E37" s="10" t="n">
         <v>984.693</v>
       </c>
-      <c r="F37" s="10" t="n">
+      <c r="F37" s="10" t="inlineStr"/>
+      <c r="G37" s="10" t="n">
         <v>-1</v>
       </c>
-      <c r="G37" s="10" t="inlineStr"/>
-      <c r="H37" s="10" t="n">
+      <c r="H37" s="10" t="inlineStr"/>
+      <c r="I37" s="10" t="n">
         <v>-1</v>
       </c>
     </row>
@@ -4144,7 +4474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4160,6 +4490,7 @@
     <col width="16" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
+    <col width="16" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4190,15 +4521,20 @@
       </c>
       <c r="F1" s="9" t="inlineStr">
         <is>
+          <t>Recoil_E(MeV)</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
           <t>t1/2</t>
         </is>
       </c>
-      <c r="G1" s="9" t="inlineStr">
+      <c r="H1" s="9" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="H1" s="9" t="inlineStr">
+      <c r="I1" s="9" t="inlineStr">
         <is>
           <t>t1/2(s)</t>
         </is>
@@ -4223,14 +4559,17 @@
         <v>10.1</v>
       </c>
       <c r="F2" s="10" t="n">
+        <v>285.2292252252252</v>
+      </c>
+      <c r="G2" s="10" t="n">
         <v>32.4</v>
       </c>
-      <c r="G2" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I2" s="10" t="n">
         <v>1944</v>
       </c>
     </row>
@@ -4253,14 +4592,17 @@
         <v>10.1</v>
       </c>
       <c r="F3" s="10" t="n">
+        <v>285.2292252252252</v>
+      </c>
+      <c r="G3" s="10" t="n">
         <v>50.4</v>
       </c>
-      <c r="G3" s="10" t="inlineStr">
+      <c r="H3" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H3" s="10" t="n">
+      <c r="I3" s="10" t="n">
         <v>50.4</v>
       </c>
     </row>
@@ -4283,14 +4625,17 @@
         <v>4.49</v>
       </c>
       <c r="F4" s="10" t="n">
+        <v>285.2292252252252</v>
+      </c>
+      <c r="G4" s="10" t="n">
         <v>6.5</v>
       </c>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="H4" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H4" s="10" t="n">
+      <c r="I4" s="10" t="n">
         <v>23400</v>
       </c>
     </row>
@@ -4313,14 +4658,17 @@
         <v>1.12</v>
       </c>
       <c r="F5" s="10" t="n">
+        <v>285.2292252252252</v>
+      </c>
+      <c r="G5" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G5" s="10" t="inlineStr">
+      <c r="H5" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H5" s="10" t="n">
+      <c r="I5" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -4343,14 +4691,17 @@
         <v>1.12</v>
       </c>
       <c r="F6" s="10" t="n">
+        <v>285.2292252252252</v>
+      </c>
+      <c r="G6" s="10" t="n">
         <v>44.3</v>
       </c>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="H6" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H6" s="10" t="n">
+      <c r="I6" s="10" t="n">
         <v>44.3</v>
       </c>
     </row>
@@ -4373,14 +4724,17 @@
         <v>117</v>
       </c>
       <c r="F7" s="10" t="n">
+        <v>282.5635315315315</v>
+      </c>
+      <c r="G7" s="10" t="n">
         <v>6.2</v>
       </c>
-      <c r="G7" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H7" s="10" t="n">
+      <c r="H7" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I7" s="10" t="n">
         <v>372</v>
       </c>
     </row>
@@ -4403,14 +4757,17 @@
         <v>117</v>
       </c>
       <c r="F8" s="10" t="n">
+        <v>282.5635315315315</v>
+      </c>
+      <c r="G8" s="10" t="n">
         <v>5.2</v>
       </c>
-      <c r="G8" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H8" s="10" t="n">
+      <c r="H8" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I8" s="10" t="n">
         <v>312</v>
       </c>
     </row>
@@ -4433,14 +4790,17 @@
         <v>192</v>
       </c>
       <c r="F9" s="10" t="n">
+        <v>282.5635315315315</v>
+      </c>
+      <c r="G9" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G9" s="10" t="inlineStr">
+      <c r="H9" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H9" s="10" t="n">
+      <c r="I9" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -4463,14 +4823,17 @@
         <v>41.5</v>
       </c>
       <c r="F10" s="10" t="n">
+        <v>282.5635315315315</v>
+      </c>
+      <c r="G10" s="10" t="n">
         <v>23.96</v>
       </c>
-      <c r="G10" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H10" s="10" t="n">
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I10" s="10" t="n">
         <v>1437.6</v>
       </c>
     </row>
@@ -4493,14 +4856,17 @@
         <v>41.5</v>
       </c>
       <c r="F11" s="10" t="n">
+        <v>282.5635315315315</v>
+      </c>
+      <c r="G11" s="10" t="n">
         <v>8.279999999999999</v>
       </c>
-      <c r="G11" s="10" t="inlineStr">
+      <c r="H11" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H11" s="10" t="n">
+      <c r="I11" s="10" t="n">
         <v>715392</v>
       </c>
     </row>
@@ -4523,14 +4889,17 @@
         <v>60.6</v>
       </c>
       <c r="F12" s="10" t="n">
+        <v>279.8978378378378</v>
+      </c>
+      <c r="G12" s="10" t="n">
         <v>5.07</v>
       </c>
-      <c r="G12" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H12" s="10" t="n">
+      <c r="H12" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I12" s="10" t="n">
         <v>304.2</v>
       </c>
     </row>
@@ -4553,14 +4922,17 @@
         <v>60.6</v>
       </c>
       <c r="F13" s="10" t="n">
+        <v>279.8978378378378</v>
+      </c>
+      <c r="G13" s="10" t="n">
         <v>48</v>
       </c>
-      <c r="G13" s="10" t="inlineStr">
+      <c r="H13" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H13" s="10" t="n">
+      <c r="I13" s="10" t="n">
         <v>48</v>
       </c>
     </row>
@@ -4583,14 +4955,17 @@
         <v>197</v>
       </c>
       <c r="F14" s="10" t="n">
+        <v>279.8978378378378</v>
+      </c>
+      <c r="G14" s="10" t="n">
         <v>55.5</v>
       </c>
-      <c r="G14" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H14" s="10" t="n">
+      <c r="H14" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I14" s="10" t="n">
         <v>3330</v>
       </c>
     </row>
@@ -4613,14 +4988,17 @@
         <v>40.4</v>
       </c>
       <c r="F15" s="10" t="n">
+        <v>279.8978378378378</v>
+      </c>
+      <c r="G15" s="10" t="n">
         <v>41.29</v>
       </c>
-      <c r="G15" s="10" t="inlineStr">
+      <c r="H15" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H15" s="10" t="n">
+      <c r="I15" s="10" t="n">
         <v>3567456</v>
       </c>
     </row>
@@ -4643,14 +5021,17 @@
         <v>40.4</v>
       </c>
       <c r="F16" s="10" t="n">
+        <v>279.8978378378378</v>
+      </c>
+      <c r="G16" s="10" t="n">
         <v>7.23</v>
       </c>
-      <c r="G16" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H16" s="10" t="n">
+      <c r="H16" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I16" s="10" t="n">
         <v>433.8</v>
       </c>
     </row>
@@ -4673,14 +5054,17 @@
         <v>2.24</v>
       </c>
       <c r="F17" s="10" t="n">
+        <v>279.8978378378378</v>
+      </c>
+      <c r="G17" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G17" s="10" t="inlineStr">
+      <c r="H17" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H17" s="10" t="n">
+      <c r="I17" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -4703,14 +5087,17 @@
         <v>19.1</v>
       </c>
       <c r="F18" s="10" t="n">
+        <v>277.2321441441442</v>
+      </c>
+      <c r="G18" s="10" t="n">
         <v>69.2</v>
       </c>
-      <c r="G18" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H18" s="10" t="n">
+      <c r="H18" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I18" s="10" t="n">
         <v>4152</v>
       </c>
     </row>
@@ -4733,14 +5120,17 @@
         <v>19.1</v>
       </c>
       <c r="F19" s="10" t="n">
+        <v>277.2321441441442</v>
+      </c>
+      <c r="G19" s="10" t="n">
         <v>33.5</v>
       </c>
-      <c r="G19" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H19" s="10" t="n">
+      <c r="H19" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I19" s="10" t="n">
         <v>2010</v>
       </c>
     </row>
@@ -4763,14 +5153,17 @@
         <v>5.61</v>
       </c>
       <c r="F20" s="10" t="n">
+        <v>277.2321441441442</v>
+      </c>
+      <c r="G20" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G20" s="10" t="inlineStr">
+      <c r="H20" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H20" s="10" t="n">
+      <c r="I20" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -4793,14 +5186,17 @@
         <v>158</v>
       </c>
       <c r="F21" s="10" t="n">
+        <v>274.5664504504505</v>
+      </c>
+      <c r="G21" s="10" t="n">
         <v>65.7</v>
       </c>
-      <c r="G21" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H21" s="10" t="n">
+      <c r="H21" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I21" s="10" t="n">
         <v>3942</v>
       </c>
     </row>
@@ -4823,14 +5219,17 @@
         <v>74</v>
       </c>
       <c r="F22" s="10" t="n">
+        <v>274.5664504504505</v>
+      </c>
+      <c r="G22" s="10" t="n">
         <v>16.991</v>
       </c>
-      <c r="G22" s="10" t="inlineStr">
+      <c r="H22" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H22" s="10" t="n">
+      <c r="I22" s="10" t="n">
         <v>1468022.4</v>
       </c>
     </row>
@@ -4853,14 +5252,17 @@
         <v>3.36</v>
       </c>
       <c r="F23" s="10" t="n">
+        <v>274.5664504504505</v>
+      </c>
+      <c r="G23" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G23" s="10" t="inlineStr">
+      <c r="H23" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H23" s="10" t="n">
+      <c r="I23" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -4883,14 +5285,17 @@
         <v>3.36</v>
       </c>
       <c r="F24" s="10" t="n">
+        <v>274.5664504504505</v>
+      </c>
+      <c r="G24" s="10" t="n">
         <v>56.114</v>
       </c>
-      <c r="G24" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H24" s="10" t="n">
+      <c r="H24" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I24" s="10" t="n">
         <v>3366.84</v>
       </c>
     </row>
@@ -4913,14 +5318,17 @@
         <v>85.2</v>
       </c>
       <c r="F25" s="10" t="n">
+        <v>271.9007567567568</v>
+      </c>
+      <c r="G25" s="10" t="n">
         <v>12.9</v>
       </c>
-      <c r="G25" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H25" s="10" t="n">
+      <c r="H25" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I25" s="10" t="n">
         <v>774</v>
       </c>
     </row>
@@ -4943,14 +5351,17 @@
         <v>85.2</v>
       </c>
       <c r="F26" s="10" t="n">
+        <v>271.9007567567568</v>
+      </c>
+      <c r="G26" s="10" t="n">
         <v>7.7</v>
       </c>
-      <c r="G26" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H26" s="10" t="n">
+      <c r="H26" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I26" s="10" t="n">
         <v>462</v>
       </c>
     </row>
@@ -4973,14 +5384,17 @@
         <v>40.4</v>
       </c>
       <c r="F27" s="10" t="n">
+        <v>271.9007567567568</v>
+      </c>
+      <c r="G27" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G27" s="10" t="inlineStr">
+      <c r="H27" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H27" s="10" t="n">
+      <c r="I27" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -5003,14 +5417,17 @@
         <v>4.49</v>
       </c>
       <c r="F28" s="10" t="n">
+        <v>269.2350630630631</v>
+      </c>
+      <c r="G28" s="10" t="n">
         <v>3.3</v>
       </c>
-      <c r="G28" s="10" t="inlineStr">
+      <c r="H28" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H28" s="10" t="n">
+      <c r="I28" s="10" t="n">
         <v>104068800</v>
       </c>
     </row>
@@ -5033,14 +5450,17 @@
         <v>4.49</v>
       </c>
       <c r="F29" s="10" t="n">
+        <v>269.2350630630631</v>
+      </c>
+      <c r="G29" s="10" t="n">
         <v>4.34</v>
       </c>
-      <c r="G29" s="10" t="inlineStr">
+      <c r="H29" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H29" s="10" t="n">
+      <c r="I29" s="10" t="n">
         <v>374976</v>
       </c>
     </row>
@@ -5063,14 +5483,17 @@
         <v>41.5</v>
       </c>
       <c r="F30" s="10" t="n">
+        <v>266.5693693693694</v>
+      </c>
+      <c r="G30" s="10" t="n">
         <v>20.5</v>
       </c>
-      <c r="G30" s="10" t="inlineStr">
+      <c r="H30" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H30" s="10" t="n">
+      <c r="I30" s="10" t="n">
         <v>73800</v>
       </c>
     </row>
@@ -5093,14 +5516,17 @@
         <v>41.5</v>
       </c>
       <c r="F31" s="10" t="n">
+        <v>266.5693693693694</v>
+      </c>
+      <c r="G31" s="10" t="n">
         <v>4.6</v>
       </c>
-      <c r="G31" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H31" s="10" t="n">
+      <c r="H31" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I31" s="10" t="n">
         <v>276</v>
       </c>
     </row>
@@ -5123,14 +5549,17 @@
         <v>4.49</v>
       </c>
       <c r="F32" s="10" t="n">
+        <v>266.5693693693694</v>
+      </c>
+      <c r="G32" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G32" s="10" t="inlineStr">
+      <c r="H32" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H32" s="10" t="n">
+      <c r="I32" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -5153,14 +5582,17 @@
         <v>12.3</v>
       </c>
       <c r="F33" s="10" t="n">
+        <v>263.9036756756757</v>
+      </c>
+      <c r="G33" s="10" t="n">
         <v>16.1</v>
       </c>
-      <c r="G33" s="10" t="inlineStr">
+      <c r="H33" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H33" s="10" t="n">
+      <c r="I33" s="10" t="n">
         <v>1391040</v>
       </c>
     </row>
@@ -5183,14 +5615,17 @@
         <v>12.3</v>
       </c>
       <c r="F34" s="10" t="n">
+        <v>263.9036756756757</v>
+      </c>
+      <c r="G34" s="10" t="n">
         <v>4.7</v>
       </c>
-      <c r="G34" s="10" t="inlineStr">
+      <c r="H34" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H34" s="10" t="n">
+      <c r="I34" s="10" t="n">
         <v>16920</v>
       </c>
     </row>
@@ -5213,14 +5648,17 @@
         <v>2.24</v>
       </c>
       <c r="F35" s="10" t="n">
+        <v>263.9036756756757</v>
+      </c>
+      <c r="G35" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G35" s="10" t="inlineStr">
+      <c r="H35" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H35" s="10" t="n">
+      <c r="I35" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -5243,14 +5681,17 @@
         <v>3.36</v>
       </c>
       <c r="F36" s="10" t="n">
+        <v>258.5722882882883</v>
+      </c>
+      <c r="G36" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="G36" s="10" t="inlineStr">
+      <c r="H36" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H36" s="10" t="n">
+      <c r="I36" s="10" t="n">
         <v>189216000</v>
       </c>
     </row>
@@ -5273,14 +5714,17 @@
         <v>3.36</v>
       </c>
       <c r="F37" s="10" t="n">
+        <v>258.5722882882883</v>
+      </c>
+      <c r="G37" s="10" t="n">
         <v>91</v>
       </c>
-      <c r="G37" s="10" t="inlineStr">
+      <c r="H37" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H37" s="10" t="n">
+      <c r="I37" s="10" t="n">
         <v>7862400</v>
       </c>
     </row>
@@ -5303,14 +5747,17 @@
         <v>1.12</v>
       </c>
       <c r="F38" s="10" t="n">
+        <v>250.5752072072072</v>
+      </c>
+      <c r="G38" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="G38" s="10" t="inlineStr">
+      <c r="H38" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H38" s="10" t="n">
+      <c r="I38" s="10" t="n">
         <v>126144000</v>
       </c>
     </row>
@@ -5333,14 +5780,17 @@
         <v>1.12</v>
       </c>
       <c r="F39" s="10" t="n">
+        <v>250.5752072072072</v>
+      </c>
+      <c r="G39" s="10" t="n">
         <v>6.263</v>
       </c>
-      <c r="G39" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H39" s="10" t="n">
+      <c r="H39" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I39" s="10" t="n">
         <v>375.78</v>
       </c>
     </row>
@@ -5356,11 +5806,12 @@
       <c r="E40" s="10" t="n">
         <v>1121.6</v>
       </c>
-      <c r="F40" s="10" t="n">
+      <c r="F40" s="10" t="inlineStr"/>
+      <c r="G40" s="10" t="n">
         <v>-1</v>
       </c>
-      <c r="G40" s="10" t="inlineStr"/>
-      <c r="H40" s="10" t="n">
+      <c r="H40" s="10" t="inlineStr"/>
+      <c r="I40" s="10" t="n">
         <v>-1</v>
       </c>
     </row>
@@ -5375,7 +5826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5391,6 +5842,7 @@
     <col width="16" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
+    <col width="16" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5421,15 +5873,20 @@
       </c>
       <c r="F1" s="9" t="inlineStr">
         <is>
+          <t>Recoil_E(MeV)</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
           <t>t1/2</t>
         </is>
       </c>
-      <c r="G1" s="9" t="inlineStr">
+      <c r="H1" s="9" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="H1" s="9" t="inlineStr">
+      <c r="I1" s="9" t="inlineStr">
         <is>
           <t>t1/2(s)</t>
         </is>
@@ -5454,14 +5911,17 @@
         <v>13.6</v>
       </c>
       <c r="F2" s="10" t="n">
+        <v>223.0997837837838</v>
+      </c>
+      <c r="G2" s="10" t="n">
         <v>58</v>
       </c>
-      <c r="G2" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I2" s="10" t="n">
         <v>3480</v>
       </c>
     </row>
@@ -5484,14 +5944,17 @@
         <v>13.6</v>
       </c>
       <c r="F3" s="10" t="n">
+        <v>223.0997837837838</v>
+      </c>
+      <c r="G3" s="10" t="n">
         <v>39.6</v>
       </c>
-      <c r="G3" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H3" s="10" t="n">
+      <c r="H3" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I3" s="10" t="n">
         <v>2376</v>
       </c>
     </row>
@@ -5514,14 +5977,17 @@
         <v>4.13</v>
       </c>
       <c r="F4" s="10" t="n">
+        <v>223.0997837837838</v>
+      </c>
+      <c r="G4" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G4" s="10" t="inlineStr">
+      <c r="H4" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H4" s="10" t="n">
+      <c r="I4" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -5544,14 +6010,17 @@
         <v>250</v>
       </c>
       <c r="F5" s="10" t="n">
+        <v>221.034045045045</v>
+      </c>
+      <c r="G5" s="10" t="n">
         <v>32.4</v>
       </c>
-      <c r="G5" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H5" s="10" t="n">
+      <c r="H5" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I5" s="10" t="n">
         <v>1944</v>
       </c>
     </row>
@@ -5574,14 +6043,17 @@
         <v>250</v>
       </c>
       <c r="F6" s="10" t="n">
+        <v>221.034045045045</v>
+      </c>
+      <c r="G6" s="10" t="n">
         <v>50.4</v>
       </c>
-      <c r="G6" s="10" t="inlineStr">
+      <c r="H6" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H6" s="10" t="n">
+      <c r="I6" s="10" t="n">
         <v>50.4</v>
       </c>
     </row>
@@ -5604,14 +6076,17 @@
         <v>127</v>
       </c>
       <c r="F7" s="10" t="n">
+        <v>221.034045045045</v>
+      </c>
+      <c r="G7" s="10" t="n">
         <v>6.5</v>
       </c>
-      <c r="G7" s="10" t="inlineStr">
+      <c r="H7" s="10" t="inlineStr">
         <is>
           <t>h</t>
         </is>
       </c>
-      <c r="H7" s="10" t="n">
+      <c r="I7" s="10" t="n">
         <v>23400</v>
       </c>
     </row>
@@ -5634,14 +6109,17 @@
         <v>6.49</v>
       </c>
       <c r="F8" s="10" t="n">
+        <v>221.034045045045</v>
+      </c>
+      <c r="G8" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G8" s="10" t="inlineStr">
+      <c r="H8" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H8" s="10" t="n">
+      <c r="I8" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -5664,14 +6142,17 @@
         <v>6.49</v>
       </c>
       <c r="F9" s="10" t="n">
+        <v>221.034045045045</v>
+      </c>
+      <c r="G9" s="10" t="n">
         <v>44.3</v>
       </c>
-      <c r="G9" s="10" t="inlineStr">
+      <c r="H9" s="10" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="H9" s="10" t="n">
+      <c r="I9" s="10" t="n">
         <v>44.3</v>
       </c>
     </row>
@@ -5694,14 +6175,17 @@
         <v>34.2</v>
       </c>
       <c r="F10" s="10" t="n">
+        <v>218.9683063063063</v>
+      </c>
+      <c r="G10" s="10" t="n">
         <v>6.2</v>
       </c>
-      <c r="G10" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H10" s="10" t="n">
+      <c r="H10" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I10" s="10" t="n">
         <v>372</v>
       </c>
     </row>
@@ -5724,14 +6208,17 @@
         <v>34.2</v>
       </c>
       <c r="F11" s="10" t="n">
+        <v>218.9683063063063</v>
+      </c>
+      <c r="G11" s="10" t="n">
         <v>5.2</v>
       </c>
-      <c r="G11" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H11" s="10" t="n">
+      <c r="H11" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I11" s="10" t="n">
         <v>312</v>
       </c>
     </row>
@@ -5754,14 +6241,17 @@
         <v>30.1</v>
       </c>
       <c r="F12" s="10" t="n">
+        <v>218.9683063063063</v>
+      </c>
+      <c r="G12" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G12" s="10" t="inlineStr">
+      <c r="H12" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H12" s="10" t="n">
+      <c r="I12" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -5784,14 +6274,17 @@
         <v>1.18</v>
       </c>
       <c r="F13" s="10" t="n">
+        <v>218.9683063063063</v>
+      </c>
+      <c r="G13" s="10" t="n">
         <v>23.96</v>
       </c>
-      <c r="G13" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H13" s="10" t="n">
+      <c r="H13" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I13" s="10" t="n">
         <v>1437.6</v>
       </c>
     </row>
@@ -5814,14 +6307,17 @@
         <v>1.18</v>
       </c>
       <c r="F14" s="10" t="n">
+        <v>218.9683063063063</v>
+      </c>
+      <c r="G14" s="10" t="n">
         <v>8.279999999999999</v>
       </c>
-      <c r="G14" s="10" t="inlineStr">
+      <c r="H14" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H14" s="10" t="n">
+      <c r="I14" s="10" t="n">
         <v>715392</v>
       </c>
     </row>
@@ -5844,14 +6340,17 @@
         <v>8.85</v>
       </c>
       <c r="F15" s="10" t="n">
+        <v>216.9025675675676</v>
+      </c>
+      <c r="G15" s="10" t="n">
         <v>41.29</v>
       </c>
-      <c r="G15" s="10" t="inlineStr">
+      <c r="H15" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H15" s="10" t="n">
+      <c r="I15" s="10" t="n">
         <v>3567456</v>
       </c>
     </row>
@@ -5874,14 +6373,17 @@
         <v>8.85</v>
       </c>
       <c r="F16" s="10" t="n">
+        <v>216.9025675675676</v>
+      </c>
+      <c r="G16" s="10" t="n">
         <v>7.23</v>
       </c>
-      <c r="G16" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H16" s="10" t="n">
+      <c r="H16" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I16" s="10" t="n">
         <v>433.8</v>
       </c>
     </row>
@@ -5904,14 +6406,17 @@
         <v>2.36</v>
       </c>
       <c r="F17" s="10" t="n">
+        <v>216.9025675675676</v>
+      </c>
+      <c r="G17" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G17" s="10" t="inlineStr">
+      <c r="H17" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H17" s="10" t="n">
+      <c r="I17" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -5934,14 +6439,17 @@
         <v>78.5</v>
       </c>
       <c r="F18" s="10" t="n">
+        <v>214.8368288288288</v>
+      </c>
+      <c r="G18" s="10" t="n">
         <v>69.2</v>
       </c>
-      <c r="G18" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H18" s="10" t="n">
+      <c r="H18" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I18" s="10" t="n">
         <v>4152</v>
       </c>
     </row>
@@ -5964,14 +6472,17 @@
         <v>78.5</v>
       </c>
       <c r="F19" s="10" t="n">
+        <v>214.8368288288288</v>
+      </c>
+      <c r="G19" s="10" t="n">
         <v>33.5</v>
       </c>
-      <c r="G19" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H19" s="10" t="n">
+      <c r="H19" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I19" s="10" t="n">
         <v>2010</v>
       </c>
     </row>
@@ -5994,14 +6505,17 @@
         <v>21.2</v>
       </c>
       <c r="F20" s="10" t="n">
+        <v>214.8368288288288</v>
+      </c>
+      <c r="G20" s="10" t="n">
         <v>14000000000</v>
       </c>
-      <c r="G20" s="10" t="inlineStr">
+      <c r="H20" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H20" s="10" t="n">
+      <c r="I20" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
     </row>
@@ -6024,14 +6538,17 @@
         <v>6.49</v>
       </c>
       <c r="F21" s="10" t="n">
+        <v>212.7710900900901</v>
+      </c>
+      <c r="G21" s="10" t="n">
         <v>65.7</v>
       </c>
-      <c r="G21" s="10" t="inlineStr">
-        <is>
-          <t>m</t>
-        </is>
-      </c>
-      <c r="H21" s="10" t="n">
+      <c r="H21" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="I21" s="10" t="n">
         <v>3942</v>
       </c>
     </row>
@@ -6054,14 +6571,17 @@
         <v>2.36</v>
       </c>
       <c r="F22" s="10" t="n">
+        <v>212.7710900900901</v>
+      </c>
+      <c r="G22" s="10" t="n">
         <v>16.991</v>
       </c>
-      <c r="G22" s="10" t="inlineStr">
+      <c r="H22" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H22" s="10" t="n">
+      <c r="I22" s="10" t="n">
         <v>1468022.4</v>
       </c>
     </row>
@@ -6084,14 +6604,17 @@
         <v>1.18</v>
       </c>
       <c r="F23" s="10" t="n">
+        <v>210.7053513513513</v>
+      </c>
+      <c r="G23" s="10" t="n">
         <v>207.3</v>
       </c>
-      <c r="G23" s="10" t="inlineStr">
+      <c r="H23" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H23" s="10" t="n">
+      <c r="I23" s="10" t="n">
         <v>17910720</v>
       </c>
     </row>
@@ -6114,14 +6637,17 @@
         <v>1.18</v>
       </c>
       <c r="F24" s="10" t="n">
+        <v>210.7053513513513</v>
+      </c>
+      <c r="G24" s="10" t="n">
         <v>3.742</v>
       </c>
-      <c r="G24" s="10" t="inlineStr">
+      <c r="H24" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H24" s="10" t="n">
+      <c r="I24" s="10" t="n">
         <v>118007712</v>
       </c>
     </row>
@@ -6144,14 +6670,17 @@
         <v>2.36</v>
       </c>
       <c r="F25" s="10" t="n">
+        <v>208.6396126126126</v>
+      </c>
+      <c r="G25" s="10" t="n">
         <v>3.3</v>
       </c>
-      <c r="G25" s="10" t="inlineStr">
+      <c r="H25" s="10" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="H25" s="10" t="n">
+      <c r="I25" s="10" t="n">
         <v>104068800</v>
       </c>
     </row>
@@ -6174,14 +6703,17 @@
         <v>2.36</v>
       </c>
       <c r="F26" s="10" t="n">
+        <v>208.6396126126126</v>
+      </c>
+      <c r="G26" s="10" t="n">
         <v>4.34</v>
       </c>
-      <c r="G26" s="10" t="inlineStr">
+      <c r="H26" s="10" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="H26" s="10" t="n">
+      <c r="I26" s="10" t="n">
         <v>374976</v>
       </c>
     </row>
@@ -6197,11 +6729,12 @@
       <c r="E27" s="10" t="n">
         <v>590.221</v>
       </c>
-      <c r="F27" s="10" t="n">
+      <c r="F27" s="10" t="inlineStr"/>
+      <c r="G27" s="10" t="n">
         <v>-1</v>
       </c>
-      <c r="G27" s="10" t="inlineStr"/>
-      <c r="H27" s="10" t="n">
+      <c r="H27" s="10" t="inlineStr"/>
+      <c r="I27" s="10" t="n">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add function to calculate production rate
</commit_message>
<xml_diff>
--- a/example/DoesCal.xlsx
+++ b/example/DoesCal.xlsx
@@ -504,7 +504,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -753,7 +753,7 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>g/atoms</t>
+          <t>g</t>
         </is>
       </c>
       <c r="E8" s="1" t="inlineStr">
@@ -781,7 +781,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -798,6 +798,7 @@
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -846,6 +847,11 @@
           <t>t1/2(s)</t>
         </is>
       </c>
+      <c r="J1" s="9" t="inlineStr">
+        <is>
+          <t>Prodx_Rate(pps)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
@@ -879,6 +885,9 @@
       <c r="I2" s="10" t="n">
         <v>372</v>
       </c>
+      <c r="J2" s="10" t="n">
+        <v>734.2822571020887</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="n">
@@ -912,6 +921,9 @@
       <c r="I3" s="10" t="n">
         <v>312</v>
       </c>
+      <c r="J3" s="10" t="n">
+        <v>734.2822571020887</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
@@ -945,6 +957,9 @@
       <c r="I4" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J4" s="10" t="n">
+        <v>1133.977771435984</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="n">
@@ -978,6 +993,9 @@
       <c r="I5" s="10" t="n">
         <v>1437.6</v>
       </c>
+      <c r="J5" s="10" t="n">
+        <v>155.718478661305</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="n">
@@ -1011,6 +1029,9 @@
       <c r="I6" s="10" t="n">
         <v>715392</v>
       </c>
+      <c r="J6" s="10" t="n">
+        <v>155.718478661305</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n">
@@ -1044,6 +1065,9 @@
       <c r="I7" s="10" t="n">
         <v>304.2</v>
       </c>
+      <c r="J7" s="10" t="n">
+        <v>1313.026893241666</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="n">
@@ -1077,6 +1101,9 @@
       <c r="I8" s="10" t="n">
         <v>48</v>
       </c>
+      <c r="J8" s="10" t="n">
+        <v>1313.026893241666</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n">
@@ -1110,6 +1137,9 @@
       <c r="I9" s="10" t="n">
         <v>3330</v>
       </c>
+      <c r="J9" s="10" t="n">
+        <v>5787.446361395772</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n">
@@ -1143,6 +1173,9 @@
       <c r="I10" s="10" t="n">
         <v>3567456</v>
       </c>
+      <c r="J10" s="10" t="n">
+        <v>1246.109544688027</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="n">
@@ -1176,6 +1209,9 @@
       <c r="I11" s="10" t="n">
         <v>433.8</v>
       </c>
+      <c r="J11" s="10" t="n">
+        <v>1246.109544688027</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n">
@@ -1209,6 +1245,9 @@
       <c r="I12" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J12" s="10" t="n">
+        <v>66.736490854845</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="n">
@@ -1242,6 +1281,9 @@
       <c r="I13" s="10" t="n">
         <v>108</v>
       </c>
+      <c r="J13" s="10" t="n">
+        <v>88.98198780646</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="n">
@@ -1275,6 +1317,9 @@
       <c r="I14" s="10" t="n">
         <v>3462</v>
       </c>
+      <c r="J14" s="10" t="n">
+        <v>935.0343027630045</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="n">
@@ -1308,6 +1353,9 @@
       <c r="I15" s="10" t="n">
         <v>4152</v>
       </c>
+      <c r="J15" s="10" t="n">
+        <v>377.9925904786613</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="n">
@@ -1341,6 +1389,9 @@
       <c r="I16" s="10" t="n">
         <v>2010</v>
       </c>
+      <c r="J16" s="10" t="n">
+        <v>377.9925904786613</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="n">
@@ -1374,6 +1425,9 @@
       <c r="I17" s="10" t="n">
         <v>3942</v>
       </c>
+      <c r="J17" s="10" t="n">
+        <v>1535.481862757816</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="n">
@@ -1407,6 +1461,9 @@
       <c r="I18" s="10" t="n">
         <v>1468022.4</v>
       </c>
+      <c r="J18" s="10" t="n">
+        <v>779.4966818004931</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="n">
@@ -1440,6 +1497,9 @@
       <c r="I19" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J19" s="10" t="n">
+        <v>88.98198780646</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="n">
@@ -1473,6 +1533,9 @@
       <c r="I20" s="10" t="n">
         <v>3366.84</v>
       </c>
+      <c r="J20" s="10" t="n">
+        <v>88.98198780646</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="n">
@@ -1506,6 +1569,9 @@
       <c r="I21" s="10" t="n">
         <v>3390940.8</v>
       </c>
+      <c r="J21" s="10" t="n">
+        <v>22.245496951615</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -1539,6 +1605,9 @@
       <c r="I22" s="10" t="n">
         <v>774</v>
       </c>
+      <c r="J22" s="10" t="n">
+        <v>2839.465871059801</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="n">
@@ -1572,6 +1641,9 @@
       <c r="I23" s="10" t="n">
         <v>462</v>
       </c>
+      <c r="J23" s="10" t="n">
+        <v>2839.465871059801</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="n">
@@ -1605,6 +1677,9 @@
       <c r="I24" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J24" s="10" t="n">
+        <v>2441.578933713842</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="n">
@@ -1638,6 +1713,9 @@
       <c r="I25" s="10" t="n">
         <v>17910720</v>
       </c>
+      <c r="J25" s="10" t="n">
+        <v>311.0752419250227</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="n">
@@ -1671,6 +1749,9 @@
       <c r="I26" s="10" t="n">
         <v>118007712</v>
       </c>
+      <c r="J26" s="10" t="n">
+        <v>311.0752419250227</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="10" t="n">
@@ -1704,6 +1785,9 @@
       <c r="I27" s="10" t="n">
         <v>666</v>
       </c>
+      <c r="J27" s="10" t="n">
+        <v>88.98198780646</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="10" t="n">
@@ -1737,6 +1821,9 @@
       <c r="I28" s="10" t="n">
         <v>30492</v>
       </c>
+      <c r="J28" s="10" t="n">
+        <v>200.7520456609159</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="10" t="n">
@@ -1770,6 +1857,9 @@
       <c r="I29" s="10" t="n">
         <v>104068800</v>
       </c>
+      <c r="J29" s="10" t="n">
+        <v>22.245496951615</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="n">
@@ -1803,6 +1893,9 @@
       <c r="I30" s="10" t="n">
         <v>374976</v>
       </c>
+      <c r="J30" s="10" t="n">
+        <v>22.245496951615</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="10" t="n">
@@ -1836,6 +1929,9 @@
       <c r="I31" s="10" t="n">
         <v>73800</v>
       </c>
+      <c r="J31" s="10" t="n">
+        <v>600.4475599948113</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="10" t="n">
@@ -1869,6 +1965,9 @@
       <c r="I32" s="10" t="n">
         <v>276</v>
       </c>
+      <c r="J32" s="10" t="n">
+        <v>600.4475599948113</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="n">
@@ -1902,6 +2001,9 @@
       <c r="I33" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J33" s="10" t="n">
+        <v>133.47298170969</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="10" t="n">
@@ -1935,6 +2037,9 @@
       <c r="I34" s="10" t="n">
         <v>1391040</v>
       </c>
+      <c r="J34" s="10" t="n">
+        <v>956.7372266182383</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="10" t="n">
@@ -1968,6 +2073,9 @@
       <c r="I35" s="10" t="n">
         <v>16920</v>
       </c>
+      <c r="J35" s="10" t="n">
+        <v>956.7372266182383</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="n">
@@ -2001,6 +2109,9 @@
       <c r="I36" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J36" s="10" t="n">
+        <v>222.45496951615</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="10" t="n">
@@ -2034,6 +2145,9 @@
       <c r="I37" s="10" t="n">
         <v>523.2</v>
       </c>
+      <c r="J37" s="10" t="n">
+        <v>22.245496951615</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="10" t="n">
@@ -2067,6 +2181,9 @@
       <c r="I38" s="10" t="n">
         <v>216</v>
       </c>
+      <c r="J38" s="10" t="n">
+        <v>22.245496951615</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="10" t="n">
@@ -2100,6 +2217,9 @@
       <c r="I39" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J39" s="10" t="n">
+        <v>44.49099390323</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="10" t="n">
@@ -2133,6 +2253,9 @@
       <c r="I40" s="10" t="n">
         <v>189216000</v>
       </c>
+      <c r="J40" s="10" t="n">
+        <v>44.49099390323</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="10" t="n">
@@ -2166,6 +2289,9 @@
       <c r="I41" s="10" t="n">
         <v>7862400</v>
       </c>
+      <c r="J41" s="10" t="n">
+        <v>44.49099390323</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="10" t="n">
@@ -2199,6 +2325,9 @@
       <c r="I42" s="10" t="n">
         <v>369792</v>
       </c>
+      <c r="J42" s="10" t="n">
+        <v>44.49099390323</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="10" t="n">
@@ -2231,6 +2360,9 @@
       </c>
       <c r="I43" s="10" t="n">
         <v>3090</v>
+      </c>
+      <c r="J43" s="10" t="n">
+        <v>44.49099390323</v>
       </c>
     </row>
     <row r="44">
@@ -2252,6 +2384,9 @@
       <c r="H44" s="10" t="inlineStr"/>
       <c r="I44" s="10" t="n">
         <v>-1</v>
+      </c>
+      <c r="J44" s="10" t="n">
+        <v>22250.38010948243</v>
       </c>
     </row>
   </sheetData>
@@ -2265,7 +2400,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2282,6 +2417,7 @@
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2330,6 +2466,11 @@
           <t>t1/2(s)</t>
         </is>
       </c>
+      <c r="J1" s="9" t="inlineStr">
+        <is>
+          <t>Prodx_Rate(pps)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
@@ -2363,6 +2504,9 @@
       <c r="I2" s="10" t="n">
         <v>3480</v>
       </c>
+      <c r="J2" s="10" t="n">
+        <v>29.47980490335971</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="n">
@@ -2396,6 +2540,9 @@
       <c r="I3" s="10" t="n">
         <v>2376</v>
       </c>
+      <c r="J3" s="10" t="n">
+        <v>29.47980490335971</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
@@ -2429,6 +2576,9 @@
       <c r="I4" s="10" t="n">
         <v>1944</v>
       </c>
+      <c r="J4" s="10" t="n">
+        <v>2387.321624075756</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="n">
@@ -2462,6 +2612,9 @@
       <c r="I5" s="10" t="n">
         <v>50.4</v>
       </c>
+      <c r="J5" s="10" t="n">
+        <v>2387.321624075756</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="n">
@@ -2495,6 +2648,9 @@
       <c r="I6" s="10" t="n">
         <v>23400</v>
       </c>
+      <c r="J6" s="10" t="n">
+        <v>1369.092779867688</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n">
@@ -2528,6 +2684,9 @@
       <c r="I7" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J7" s="10" t="n">
+        <v>191.709160721235</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="n">
@@ -2561,6 +2720,9 @@
       <c r="I8" s="10" t="n">
         <v>44.3</v>
       </c>
+      <c r="J8" s="10" t="n">
+        <v>191.709160721235</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n">
@@ -2594,6 +2756,9 @@
       <c r="I9" s="10" t="n">
         <v>372</v>
       </c>
+      <c r="J9" s="10" t="n">
+        <v>2893.723180697886</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n">
@@ -2627,6 +2792,9 @@
       <c r="I10" s="10" t="n">
         <v>312</v>
       </c>
+      <c r="J10" s="10" t="n">
+        <v>2893.723180697886</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="n">
@@ -2660,6 +2828,9 @@
       <c r="I11" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J11" s="10" t="n">
+        <v>3798.011674665975</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n">
@@ -2693,6 +2864,9 @@
       <c r="I12" s="10" t="n">
         <v>1437.6</v>
       </c>
+      <c r="J12" s="10" t="n">
+        <v>191.709160721235</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="n">
@@ -2726,6 +2900,9 @@
       <c r="I13" s="10" t="n">
         <v>715392</v>
       </c>
+      <c r="J13" s="10" t="n">
+        <v>191.709160721235</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="n">
@@ -2759,6 +2936,9 @@
       <c r="I14" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J14" s="10" t="n">
+        <v>14.70373091192113</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="n">
@@ -2792,6 +2972,9 @@
       <c r="I15" s="10" t="n">
         <v>304.2</v>
       </c>
+      <c r="J15" s="10" t="n">
+        <v>44.12927850564276</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="n">
@@ -2825,6 +3008,9 @@
       <c r="I16" s="10" t="n">
         <v>48</v>
       </c>
+      <c r="J16" s="10" t="n">
+        <v>44.12927850564276</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="n">
@@ -2858,6 +3044,9 @@
       <c r="I17" s="10" t="n">
         <v>4152</v>
       </c>
+      <c r="J17" s="10" t="n">
+        <v>1558.993363600986</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="n">
@@ -2891,6 +3080,9 @@
       <c r="I18" s="10" t="n">
         <v>2010</v>
       </c>
+      <c r="J18" s="10" t="n">
+        <v>1558.993363600986</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="n">
@@ -2924,6 +3116,9 @@
       <c r="I19" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J19" s="10" t="n">
+        <v>441.2927850564276</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="n">
@@ -2957,6 +3152,9 @@
       <c r="I20" s="10" t="n">
         <v>3942</v>
       </c>
+      <c r="J20" s="10" t="n">
+        <v>1249.726698663899</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="n">
@@ -2990,6 +3188,9 @@
       <c r="I21" s="10" t="n">
         <v>1468022.4</v>
       </c>
+      <c r="J21" s="10" t="n">
+        <v>235.1150084317032</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -3023,6 +3224,9 @@
       <c r="I22" s="10" t="n">
         <v>104068800</v>
       </c>
+      <c r="J22" s="10" t="n">
+        <v>191.709160721235</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="n">
@@ -3056,6 +3260,9 @@
       <c r="I23" s="10" t="n">
         <v>374976</v>
       </c>
+      <c r="J23" s="10" t="n">
+        <v>191.709160721235</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="n">
@@ -3089,6 +3296,9 @@
       <c r="I24" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J24" s="10" t="n">
+        <v>14.70373091192113</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="n">
@@ -3122,6 +3332,9 @@
       <c r="I25" s="10" t="n">
         <v>73800</v>
       </c>
+      <c r="J25" s="10" t="n">
+        <v>88.25855701128552</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="n">
@@ -3155,6 +3368,9 @@
       <c r="I26" s="10" t="n">
         <v>276</v>
       </c>
+      <c r="J26" s="10" t="n">
+        <v>88.25855701128552</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="10" t="n">
@@ -3187,6 +3403,9 @@
       </c>
       <c r="I27" s="10" t="n">
         <v>189216000</v>
+      </c>
+      <c r="J27" s="10" t="n">
+        <v>14.70373091192113</v>
       </c>
     </row>
     <row r="28">
@@ -3208,6 +3427,9 @@
       <c r="H28" s="10" t="inlineStr"/>
       <c r="I28" s="10" t="n">
         <v>-1</v>
+      </c>
+      <c r="J28" s="10" t="n">
+        <v>14712.75571109093</v>
       </c>
     </row>
   </sheetData>
@@ -3221,7 +3443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3238,6 +3460,7 @@
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3286,6 +3509,11 @@
           <t>t1/2(s)</t>
         </is>
       </c>
+      <c r="J1" s="9" t="inlineStr">
+        <is>
+          <t>Prodx_Rate(pps)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
@@ -3319,6 +3547,9 @@
       <c r="I2" s="10" t="n">
         <v>1944</v>
       </c>
+      <c r="J2" s="10" t="n">
+        <v>676.4077934881309</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="n">
@@ -3352,6 +3583,9 @@
       <c r="I3" s="10" t="n">
         <v>50.4</v>
       </c>
+      <c r="J3" s="10" t="n">
+        <v>676.4077934881309</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
@@ -3385,6 +3619,9 @@
       <c r="I4" s="10" t="n">
         <v>23400</v>
       </c>
+      <c r="J4" s="10" t="n">
+        <v>392.4612063821507</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="n">
@@ -3418,6 +3655,9 @@
       <c r="I5" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J5" s="10" t="n">
+        <v>35.62896666234272</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="n">
@@ -3451,6 +3691,9 @@
       <c r="I6" s="10" t="n">
         <v>44.3</v>
       </c>
+      <c r="J6" s="10" t="n">
+        <v>35.62896666234272</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n">
@@ -3484,6 +3727,9 @@
       <c r="I7" s="10" t="n">
         <v>372</v>
       </c>
+      <c r="J7" s="10" t="n">
+        <v>3237.35280840576</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="n">
@@ -3517,6 +3763,9 @@
       <c r="I8" s="10" t="n">
         <v>312</v>
       </c>
+      <c r="J8" s="10" t="n">
+        <v>3237.35280840576</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n">
@@ -3550,6 +3799,9 @@
       <c r="I9" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J9" s="10" t="n">
+        <v>5479.988273446622</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n">
@@ -3583,6 +3835,9 @@
       <c r="I10" s="10" t="n">
         <v>1437.6</v>
       </c>
+      <c r="J10" s="10" t="n">
+        <v>605.87329095862</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="n">
@@ -3616,6 +3871,9 @@
       <c r="I11" s="10" t="n">
         <v>715392</v>
       </c>
+      <c r="J11" s="10" t="n">
+        <v>605.87329095862</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n">
@@ -3649,6 +3907,9 @@
       <c r="I12" s="10" t="n">
         <v>304.2</v>
       </c>
+      <c r="J12" s="10" t="n">
+        <v>285.7551640939163</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="n">
@@ -3682,6 +3943,9 @@
       <c r="I13" s="10" t="n">
         <v>48</v>
       </c>
+      <c r="J13" s="10" t="n">
+        <v>285.7551640939163</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="n">
@@ -3715,6 +3979,9 @@
       <c r="I14" s="10" t="n">
         <v>3330</v>
       </c>
+      <c r="J14" s="10" t="n">
+        <v>694.4935633674926</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="n">
@@ -3748,6 +4015,9 @@
       <c r="I15" s="10" t="n">
         <v>3567456</v>
       </c>
+      <c r="J15" s="10" t="n">
+        <v>178.1448333117136</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="n">
@@ -3781,6 +4051,9 @@
       <c r="I16" s="10" t="n">
         <v>433.8</v>
       </c>
+      <c r="J16" s="10" t="n">
+        <v>178.1448333117136</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="n">
@@ -3814,6 +4087,9 @@
       <c r="I17" s="10" t="n">
         <v>4152</v>
       </c>
+      <c r="J17" s="10" t="n">
+        <v>907.9056479439618</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="n">
@@ -3847,6 +4123,9 @@
       <c r="I18" s="10" t="n">
         <v>2010</v>
       </c>
+      <c r="J18" s="10" t="n">
+        <v>907.9056479439618</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="n">
@@ -3880,6 +4159,9 @@
       <c r="I19" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J19" s="10" t="n">
+        <v>285.7551640939163</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="n">
@@ -3913,6 +4195,9 @@
       <c r="I20" s="10" t="n">
         <v>3942</v>
       </c>
+      <c r="J20" s="10" t="n">
+        <v>2947.980490335971</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="n">
@@ -3946,6 +4231,9 @@
       <c r="I21" s="10" t="n">
         <v>1468022.4</v>
       </c>
+      <c r="J21" s="10" t="n">
+        <v>1032.697460111558</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -3979,6 +4267,9 @@
       <c r="I22" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J22" s="10" t="n">
+        <v>35.62896666234272</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="n">
@@ -4012,6 +4303,9 @@
       <c r="I23" s="10" t="n">
         <v>3366.84</v>
       </c>
+      <c r="J23" s="10" t="n">
+        <v>35.62896666234272</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="n">
@@ -4045,6 +4339,9 @@
       <c r="I24" s="10" t="n">
         <v>774</v>
       </c>
+      <c r="J24" s="10" t="n">
+        <v>195.3263146971073</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="n">
@@ -4078,6 +4375,9 @@
       <c r="I25" s="10" t="n">
         <v>462</v>
       </c>
+      <c r="J25" s="10" t="n">
+        <v>195.3263146971073</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="n">
@@ -4111,6 +4411,9 @@
       <c r="I26" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J26" s="10" t="n">
+        <v>106.8868999870282</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="10" t="n">
@@ -4144,6 +4447,9 @@
       <c r="I27" s="10" t="n">
         <v>17910720</v>
       </c>
+      <c r="J27" s="10" t="n">
+        <v>35.62896666234272</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="10" t="n">
@@ -4177,6 +4483,9 @@
       <c r="I28" s="10" t="n">
         <v>118007712</v>
       </c>
+      <c r="J28" s="10" t="n">
+        <v>35.62896666234272</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="10" t="n">
@@ -4210,6 +4519,9 @@
       <c r="I29" s="10" t="n">
         <v>104068800</v>
       </c>
+      <c r="J29" s="10" t="n">
+        <v>195.3263146971073</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="n">
@@ -4243,6 +4555,9 @@
       <c r="I30" s="10" t="n">
         <v>374976</v>
       </c>
+      <c r="J30" s="10" t="n">
+        <v>195.3263146971073</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="10" t="n">
@@ -4276,6 +4591,9 @@
       <c r="I31" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J31" s="10" t="n">
+        <v>35.62896666234272</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="10" t="n">
@@ -4309,6 +4627,9 @@
       <c r="I32" s="10" t="n">
         <v>73800</v>
       </c>
+      <c r="J32" s="10" t="n">
+        <v>374.375436502789</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="n">
@@ -4342,6 +4663,9 @@
       <c r="I33" s="10" t="n">
         <v>276</v>
       </c>
+      <c r="J33" s="10" t="n">
+        <v>374.375436502789</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="10" t="n">
@@ -4375,6 +4699,9 @@
       <c r="I34" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J34" s="10" t="n">
+        <v>35.62896666234272</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="10" t="n">
@@ -4408,6 +4735,9 @@
       <c r="I35" s="10" t="n">
         <v>1391040</v>
       </c>
+      <c r="J35" s="10" t="n">
+        <v>17.81448333117136</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="n">
@@ -4440,6 +4770,9 @@
       </c>
       <c r="I36" s="10" t="n">
         <v>16920</v>
+      </c>
+      <c r="J36" s="10" t="n">
+        <v>17.81448333117136</v>
       </c>
     </row>
     <row r="37">
@@ -4461,6 +4794,9 @@
       <c r="H37" s="10" t="inlineStr"/>
       <c r="I37" s="10" t="n">
         <v>-1</v>
+      </c>
+      <c r="J37" s="10" t="n">
+        <v>17808.9309998184</v>
       </c>
     </row>
   </sheetData>
@@ -4474,7 +4810,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4491,6 +4827,7 @@
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4539,6 +4876,11 @@
           <t>t1/2(s)</t>
         </is>
       </c>
+      <c r="J1" s="9" t="inlineStr">
+        <is>
+          <t>Prodx_Rate(pps)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
@@ -4572,6 +4914,9 @@
       <c r="I2" s="10" t="n">
         <v>1944</v>
       </c>
+      <c r="J2" s="10" t="n">
+        <v>182.6662757815541</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="n">
@@ -4605,6 +4950,9 @@
       <c r="I3" s="10" t="n">
         <v>50.4</v>
       </c>
+      <c r="J3" s="10" t="n">
+        <v>182.6662757815541</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
@@ -4638,6 +4986,9 @@
       <c r="I4" s="10" t="n">
         <v>23400</v>
       </c>
+      <c r="J4" s="10" t="n">
+        <v>81.20510675833441</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="n">
@@ -4671,6 +5022,9 @@
       <c r="I5" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J5" s="10" t="n">
+        <v>20.25606226488521</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="n">
@@ -4704,6 +5058,9 @@
       <c r="I6" s="10" t="n">
         <v>44.3</v>
       </c>
+      <c r="J6" s="10" t="n">
+        <v>20.25606226488521</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n">
@@ -4737,6 +5094,9 @@
       <c r="I7" s="10" t="n">
         <v>372</v>
       </c>
+      <c r="J7" s="10" t="n">
+        <v>2116.03507588533</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="n">
@@ -4770,6 +5130,9 @@
       <c r="I8" s="10" t="n">
         <v>312</v>
       </c>
+      <c r="J8" s="10" t="n">
+        <v>2116.03507588533</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n">
@@ -4803,6 +5166,9 @@
       <c r="I9" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J9" s="10" t="n">
+        <v>3472.467816837463</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n">
@@ -4836,6 +5202,9 @@
       <c r="I10" s="10" t="n">
         <v>1437.6</v>
       </c>
+      <c r="J10" s="10" t="n">
+        <v>750.5594499935142</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="n">
@@ -4869,6 +5238,9 @@
       <c r="I11" s="10" t="n">
         <v>715392</v>
       </c>
+      <c r="J11" s="10" t="n">
+        <v>750.5594499935142</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n">
@@ -4902,6 +5274,9 @@
       <c r="I12" s="10" t="n">
         <v>304.2</v>
       </c>
+      <c r="J12" s="10" t="n">
+        <v>1095.997654689324</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="n">
@@ -4935,6 +5310,9 @@
       <c r="I13" s="10" t="n">
         <v>48</v>
       </c>
+      <c r="J13" s="10" t="n">
+        <v>1095.997654689324</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="n">
@@ -4968,6 +5346,9 @@
       <c r="I14" s="10" t="n">
         <v>3330</v>
       </c>
+      <c r="J14" s="10" t="n">
+        <v>3562.896666234272</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="n">
@@ -5001,6 +5382,9 @@
       <c r="I15" s="10" t="n">
         <v>3567456</v>
       </c>
+      <c r="J15" s="10" t="n">
+        <v>730.6651031262163</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="n">
@@ -5034,6 +5418,9 @@
       <c r="I16" s="10" t="n">
         <v>433.8</v>
       </c>
+      <c r="J16" s="10" t="n">
+        <v>730.6651031262163</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="n">
@@ -5067,6 +5454,9 @@
       <c r="I17" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J17" s="10" t="n">
+        <v>40.51212452977042</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="n">
@@ -5100,6 +5490,9 @@
       <c r="I18" s="10" t="n">
         <v>4152</v>
       </c>
+      <c r="J18" s="10" t="n">
+        <v>345.4382046958102</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="n">
@@ -5133,6 +5526,9 @@
       <c r="I19" s="10" t="n">
         <v>2010</v>
       </c>
+      <c r="J19" s="10" t="n">
+        <v>345.4382046958102</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="n">
@@ -5166,6 +5562,9 @@
       <c r="I20" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J20" s="10" t="n">
+        <v>101.4611690232197</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="n">
@@ -5199,6 +5598,9 @@
       <c r="I21" s="10" t="n">
         <v>3942</v>
       </c>
+      <c r="J21" s="10" t="n">
+        <v>2857.551640939163</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -5232,6 +5634,9 @@
       <c r="I22" s="10" t="n">
         <v>1468022.4</v>
       </c>
+      <c r="J22" s="10" t="n">
+        <v>1338.346971072772</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="n">
@@ -5265,6 +5670,9 @@
       <c r="I23" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J23" s="10" t="n">
+        <v>60.7681867946556</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="n">
@@ -5298,6 +5706,9 @@
       <c r="I24" s="10" t="n">
         <v>3366.84</v>
       </c>
+      <c r="J24" s="10" t="n">
+        <v>60.7681867946556</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="n">
@@ -5331,6 +5742,9 @@
       <c r="I25" s="10" t="n">
         <v>774</v>
       </c>
+      <c r="J25" s="10" t="n">
+        <v>1540.907593721624</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="n">
@@ -5364,6 +5778,9 @@
       <c r="I26" s="10" t="n">
         <v>462</v>
       </c>
+      <c r="J26" s="10" t="n">
+        <v>1540.907593721624</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="10" t="n">
@@ -5397,6 +5814,9 @@
       <c r="I27" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J27" s="10" t="n">
+        <v>730.6651031262163</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="10" t="n">
@@ -5430,6 +5850,9 @@
       <c r="I28" s="10" t="n">
         <v>104068800</v>
       </c>
+      <c r="J28" s="10" t="n">
+        <v>81.20510675833441</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="10" t="n">
@@ -5463,6 +5886,9 @@
       <c r="I29" s="10" t="n">
         <v>374976</v>
       </c>
+      <c r="J29" s="10" t="n">
+        <v>81.20510675833441</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="n">
@@ -5496,6 +5922,9 @@
       <c r="I30" s="10" t="n">
         <v>73800</v>
       </c>
+      <c r="J30" s="10" t="n">
+        <v>750.5594499935142</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="10" t="n">
@@ -5529,6 +5958,9 @@
       <c r="I31" s="10" t="n">
         <v>276</v>
       </c>
+      <c r="J31" s="10" t="n">
+        <v>750.5594499935142</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="10" t="n">
@@ -5562,6 +5994,9 @@
       <c r="I32" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J32" s="10" t="n">
+        <v>81.20510675833441</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="n">
@@ -5595,6 +6030,9 @@
       <c r="I33" s="10" t="n">
         <v>1391040</v>
       </c>
+      <c r="J33" s="10" t="n">
+        <v>222.45496951615</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="10" t="n">
@@ -5628,6 +6066,9 @@
       <c r="I34" s="10" t="n">
         <v>16920</v>
       </c>
+      <c r="J34" s="10" t="n">
+        <v>222.45496951615</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="10" t="n">
@@ -5661,6 +6102,9 @@
       <c r="I35" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J35" s="10" t="n">
+        <v>40.51212452977042</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="n">
@@ -5694,6 +6138,9 @@
       <c r="I36" s="10" t="n">
         <v>189216000</v>
       </c>
+      <c r="J36" s="10" t="n">
+        <v>60.7681867946556</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="10" t="n">
@@ -5727,6 +6174,9 @@
       <c r="I37" s="10" t="n">
         <v>7862400</v>
       </c>
+      <c r="J37" s="10" t="n">
+        <v>60.7681867946556</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="10" t="n">
@@ -5760,6 +6210,9 @@
       <c r="I38" s="10" t="n">
         <v>126144000</v>
       </c>
+      <c r="J38" s="10" t="n">
+        <v>20.25606226488521</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="10" t="n">
@@ -5792,6 +6245,9 @@
       </c>
       <c r="I39" s="10" t="n">
         <v>375.78</v>
+      </c>
+      <c r="J39" s="10" t="n">
+        <v>20.25606226488521</v>
       </c>
     </row>
     <row r="40">
@@ -5813,6 +6269,9 @@
       <c r="H40" s="10" t="inlineStr"/>
       <c r="I40" s="10" t="n">
         <v>-1</v>
+      </c>
+      <c r="J40" s="10" t="n">
+        <v>20284.99949669218</v>
       </c>
     </row>
   </sheetData>
@@ -5826,7 +6285,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5843,6 +6302,7 @@
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5891,6 +6351,11 @@
           <t>t1/2(s)</t>
         </is>
       </c>
+      <c r="J1" s="9" t="inlineStr">
+        <is>
+          <t>Prodx_Rate(pps)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
@@ -5924,6 +6389,9 @@
       <c r="I2" s="10" t="n">
         <v>3480</v>
       </c>
+      <c r="J2" s="10" t="n">
+        <v>245.9664703593203</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="n">
@@ -5957,6 +6425,9 @@
       <c r="I3" s="10" t="n">
         <v>2376</v>
       </c>
+      <c r="J3" s="10" t="n">
+        <v>245.9664703593203</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
@@ -5990,6 +6461,9 @@
       <c r="I4" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J4" s="10" t="n">
+        <v>74.69422960176418</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="n">
@@ -6023,6 +6497,9 @@
       <c r="I5" s="10" t="n">
         <v>1944</v>
       </c>
+      <c r="J5" s="10" t="n">
+        <v>4521.442469840447</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="n">
@@ -6056,6 +6533,9 @@
       <c r="I6" s="10" t="n">
         <v>50.4</v>
       </c>
+      <c r="J6" s="10" t="n">
+        <v>4521.442469840447</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n">
@@ -6089,6 +6569,9 @@
       <c r="I7" s="10" t="n">
         <v>23400</v>
       </c>
+      <c r="J7" s="10" t="n">
+        <v>2296.892774678947</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="n">
@@ -6122,6 +6605,9 @@
       <c r="I8" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J8" s="10" t="n">
+        <v>117.376646517058</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n">
@@ -6155,6 +6641,9 @@
       <c r="I9" s="10" t="n">
         <v>44.3</v>
       </c>
+      <c r="J9" s="10" t="n">
+        <v>117.376646517058</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n">
@@ -6188,6 +6677,9 @@
       <c r="I10" s="10" t="n">
         <v>372</v>
       </c>
+      <c r="J10" s="10" t="n">
+        <v>618.5333298741731</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="n">
@@ -6221,6 +6713,9 @@
       <c r="I11" s="10" t="n">
         <v>312</v>
       </c>
+      <c r="J11" s="10" t="n">
+        <v>618.5333298741731</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n">
@@ -6254,6 +6749,9 @@
       <c r="I12" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J12" s="10" t="n">
+        <v>544.3816733687898</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="n">
@@ -6287,6 +6785,9 @@
       <c r="I13" s="10" t="n">
         <v>1437.6</v>
       </c>
+      <c r="J13" s="10" t="n">
+        <v>21.3412084576469</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="n">
@@ -6320,6 +6821,9 @@
       <c r="I14" s="10" t="n">
         <v>715392</v>
       </c>
+      <c r="J14" s="10" t="n">
+        <v>21.3412084576469</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="n">
@@ -6353,6 +6857,9 @@
       <c r="I15" s="10" t="n">
         <v>3567456</v>
       </c>
+      <c r="J15" s="10" t="n">
+        <v>160.0590634323518</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="n">
@@ -6386,6 +6893,9 @@
       <c r="I16" s="10" t="n">
         <v>433.8</v>
       </c>
+      <c r="J16" s="10" t="n">
+        <v>160.0590634323518</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="n">
@@ -6419,6 +6929,9 @@
       <c r="I17" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J17" s="10" t="n">
+        <v>42.68241691529381</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="n">
@@ -6452,6 +6965,9 @@
       <c r="I18" s="10" t="n">
         <v>4152</v>
       </c>
+      <c r="J18" s="10" t="n">
+        <v>1419.7329355299</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="n">
@@ -6485,6 +7001,9 @@
       <c r="I19" s="10" t="n">
         <v>2010</v>
       </c>
+      <c r="J19" s="10" t="n">
+        <v>1419.7329355299</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="n">
@@ -6518,6 +7037,9 @@
       <c r="I20" s="10" t="n">
         <v>4.41504e+17</v>
       </c>
+      <c r="J20" s="10" t="n">
+        <v>383.4183214424699</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="n">
@@ -6551,6 +7073,9 @@
       <c r="I21" s="10" t="n">
         <v>3942</v>
       </c>
+      <c r="J21" s="10" t="n">
+        <v>117.376646517058</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -6584,6 +7109,9 @@
       <c r="I22" s="10" t="n">
         <v>1468022.4</v>
       </c>
+      <c r="J22" s="10" t="n">
+        <v>42.68241691529381</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="n">
@@ -6617,6 +7145,9 @@
       <c r="I23" s="10" t="n">
         <v>17910720</v>
       </c>
+      <c r="J23" s="10" t="n">
+        <v>21.3412084576469</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="n">
@@ -6650,6 +7181,9 @@
       <c r="I24" s="10" t="n">
         <v>118007712</v>
       </c>
+      <c r="J24" s="10" t="n">
+        <v>21.3412084576469</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="n">
@@ -6683,6 +7217,9 @@
       <c r="I25" s="10" t="n">
         <v>104068800</v>
       </c>
+      <c r="J25" s="10" t="n">
+        <v>42.68241691529381</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="n">
@@ -6715,6 +7252,9 @@
       </c>
       <c r="I26" s="10" t="n">
         <v>374976</v>
+      </c>
+      <c r="J26" s="10" t="n">
+        <v>42.68241691529381</v>
       </c>
     </row>
     <row r="27">
@@ -6737,6 +7277,9 @@
       <c r="I27" s="10" t="n">
         <v>-1</v>
       </c>
+      <c r="J27" s="10" t="n">
+        <v>10674.60118396679</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add function to summarize all production A(Bq) at cd = 0s in a new sheet Summary
</commit_message>
<xml_diff>
--- a/example/DoesCal.xlsx
+++ b/example/DoesCal.xlsx
@@ -12,6 +12,7 @@
     <sheet name="6um_362MeV" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="3um_391MeV" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="12um_303MeV" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Summary" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
@@ -781,7 +782,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -799,6 +800,8 @@
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
     <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="16" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -852,6 +855,16 @@
           <t>Prodx_Rate(pps)</t>
         </is>
       </c>
+      <c r="K1" s="9" t="inlineStr">
+        <is>
+          <t>Stop_Ratio</t>
+        </is>
+      </c>
+      <c r="L1" s="9" t="inlineStr">
+        <is>
+          <t>Prodx_A(Bq)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
@@ -888,6 +901,12 @@
       <c r="J2" s="10" t="n">
         <v>734.2822571020887</v>
       </c>
+      <c r="K2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="10" t="n">
+        <v>733.3842327669173</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="n">
@@ -924,6 +943,12 @@
       <c r="J3" s="10" t="n">
         <v>734.2822571020887</v>
       </c>
+      <c r="K3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <v>734.034983621253</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
@@ -960,6 +985,12 @@
       <c r="J4" s="10" t="n">
         <v>1133.977771435984</v>
       </c>
+      <c r="K4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="10" t="n">
+        <v>6.420737979432899e-12</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="n">
@@ -996,6 +1027,12 @@
       <c r="J5" s="10" t="n">
         <v>155.718478661305</v>
       </c>
+      <c r="K5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10" t="n">
+        <v>128.2604822863538</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="n">
@@ -1032,6 +1069,12 @@
       <c r="J6" s="10" t="n">
         <v>155.718478661305</v>
       </c>
+      <c r="K6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="10" t="n">
+        <v>0.5420942074056223</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n">
@@ -1068,6 +1111,12 @@
       <c r="J7" s="10" t="n">
         <v>1313.026893241666</v>
       </c>
+      <c r="K7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="10" t="n">
+        <v>1312.66669224367</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="n">
@@ -1104,6 +1153,12 @@
       <c r="J8" s="10" t="n">
         <v>1313.026893241666</v>
       </c>
+      <c r="K8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="10" t="n">
+        <v>1313.026893241666</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n">
@@ -1140,6 +1195,12 @@
       <c r="J9" s="10" t="n">
         <v>5787.446361395772</v>
       </c>
+      <c r="K9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="10" t="n">
+        <v>3051.432784206843</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n">
@@ -1176,6 +1237,12 @@
       <c r="J10" s="10" t="n">
         <v>1246.109544688027</v>
       </c>
+      <c r="K10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="10" t="n">
+        <v>0.8711270220538968</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="n">
@@ -1212,6 +1279,12 @@
       <c r="J11" s="10" t="n">
         <v>1246.109544688027</v>
       </c>
+      <c r="K11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="10" t="n">
+        <v>1242.147563230566</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n">
@@ -1248,6 +1321,12 @@
       <c r="J12" s="10" t="n">
         <v>66.736490854845</v>
       </c>
+      <c r="K12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>3.778711825216491e-13</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="n">
@@ -1284,6 +1363,12 @@
       <c r="J13" s="10" t="n">
         <v>88.98198780646</v>
       </c>
+      <c r="K13" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="10" t="n">
+        <v>88.98198779819772</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="n">
@@ -1320,6 +1405,12 @@
       <c r="J14" s="10" t="n">
         <v>935.0343027630045</v>
       </c>
+      <c r="K14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="10" t="n">
+        <v>480.1881212201769</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="n">
@@ -1356,6 +1447,12 @@
       <c r="J15" s="10" t="n">
         <v>377.9925904786613</v>
       </c>
+      <c r="K15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="10" t="n">
+        <v>170.7256476207904</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="n">
@@ -1392,6 +1489,12 @@
       <c r="J16" s="10" t="n">
         <v>377.9925904786613</v>
       </c>
+      <c r="K16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="10" t="n">
+        <v>268.7380314146083</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="n">
@@ -1428,6 +1531,12 @@
       <c r="J17" s="10" t="n">
         <v>1535.481862757816</v>
       </c>
+      <c r="K17" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="10" t="n">
+        <v>720.0459638588325</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="n">
@@ -1464,6 +1573,12 @@
       <c r="J18" s="10" t="n">
         <v>779.4966818004931</v>
       </c>
+      <c r="K18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="10" t="n">
+        <v>1.323574372876981</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="n">
@@ -1500,6 +1615,12 @@
       <c r="J19" s="10" t="n">
         <v>88.98198780646</v>
       </c>
+      <c r="K19" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="10" t="n">
+        <v>5.038282433621988e-13</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="n">
@@ -1536,6 +1657,12 @@
       <c r="J20" s="10" t="n">
         <v>88.98198780646</v>
       </c>
+      <c r="K20" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="10" t="n">
+        <v>46.56951825726176</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="n">
@@ -1572,6 +1699,12 @@
       <c r="J21" s="10" t="n">
         <v>22.245496951615</v>
       </c>
+      <c r="K21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="10" t="n">
+        <v>0.01636054959816941</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -1608,6 +1741,12 @@
       <c r="J22" s="10" t="n">
         <v>2839.465871059801</v>
       </c>
+      <c r="K22" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" s="10" t="n">
+        <v>2726.383621523662</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="n">
@@ -1644,6 +1783,12 @@
       <c r="J23" s="10" t="n">
         <v>2839.465871059801</v>
       </c>
+      <c r="K23" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="10" t="n">
+        <v>2826.641193619373</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="n">
@@ -1680,6 +1825,12 @@
       <c r="J24" s="10" t="n">
         <v>2441.578933713842</v>
       </c>
+      <c r="K24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" s="10" t="n">
+        <v>1.382455545810912e-11</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="n">
@@ -1716,6 +1867,12 @@
       <c r="J25" s="10" t="n">
         <v>311.0752419250227</v>
       </c>
+      <c r="K25" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" s="10" t="n">
+        <v>0.04332692746524298</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="n">
@@ -1752,6 +1909,12 @@
       <c r="J26" s="10" t="n">
         <v>311.0752419250227</v>
       </c>
+      <c r="K26" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" s="10" t="n">
+        <v>0.006576369433904025</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="10" t="n">
@@ -1788,6 +1951,12 @@
       <c r="J27" s="10" t="n">
         <v>88.98198780646</v>
       </c>
+      <c r="K27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" s="10" t="n">
+        <v>86.88083107180485</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="10" t="n">
@@ -1824,6 +1993,12 @@
       <c r="J28" s="10" t="n">
         <v>200.7520456609159</v>
       </c>
+      <c r="K28" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" s="10" t="n">
+        <v>15.771185516272</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="10" t="n">
@@ -1860,6 +2035,12 @@
       <c r="J29" s="10" t="n">
         <v>22.245496951615</v>
       </c>
+      <c r="K29" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="10" t="n">
+        <v>0.0005332760691358341</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="n">
@@ -1896,6 +2077,12 @@
       <c r="J30" s="10" t="n">
         <v>22.245496951615</v>
       </c>
+      <c r="K30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="10" t="n">
+        <v>0.1475130514320869</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="10" t="n">
@@ -1932,6 +2119,12 @@
       <c r="J31" s="10" t="n">
         <v>600.4475599948113</v>
       </c>
+      <c r="K31" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" s="10" t="n">
+        <v>19.95880342549659</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="10" t="n">
@@ -1968,6 +2161,12 @@
       <c r="J32" s="10" t="n">
         <v>600.4475599948113</v>
       </c>
+      <c r="K32" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" s="10" t="n">
+        <v>600.3763024892601</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="n">
@@ -2004,6 +2203,12 @@
       <c r="J33" s="10" t="n">
         <v>133.47298170969</v>
       </c>
+      <c r="K33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" s="10" t="n">
+        <v>7.557423650432982e-13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="10" t="n">
@@ -2040,6 +2245,12 @@
       <c r="J34" s="10" t="n">
         <v>956.7372266182383</v>
       </c>
+      <c r="K34" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" s="10" t="n">
+        <v>1.714349633378636</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="10" t="n">
@@ -2076,6 +2287,12 @@
       <c r="J35" s="10" t="n">
         <v>956.7372266182383</v>
       </c>
+      <c r="K35" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" s="10" t="n">
+        <v>131.1606979483483</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="n">
@@ -2112,6 +2329,12 @@
       <c r="J36" s="10" t="n">
         <v>222.45496951615</v>
       </c>
+      <c r="K36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" s="10" t="n">
+        <v>1.259570608405497e-12</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="10" t="n">
@@ -2148,6 +2371,12 @@
       <c r="J37" s="10" t="n">
         <v>22.245496951615</v>
       </c>
+      <c r="K37" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L37" s="10" t="n">
+        <v>22.05653489069024</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="10" t="n">
@@ -2184,6 +2413,12 @@
       <c r="J38" s="10" t="n">
         <v>22.245496951615</v>
       </c>
+      <c r="K38" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L38" s="10" t="n">
+        <v>22.2452825930475</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="10" t="n">
@@ -2220,6 +2455,12 @@
       <c r="J39" s="10" t="n">
         <v>44.49099390323</v>
       </c>
+      <c r="K39" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L39" s="10" t="n">
+        <v>2.519141216810994e-13</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="10" t="n">
@@ -2256,6 +2497,12 @@
       <c r="J40" s="10" t="n">
         <v>44.49099390323</v>
       </c>
+      <c r="K40" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L40" s="10" t="n">
+        <v>0.0005866068400912797</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="10" t="n">
@@ -2292,6 +2539,12 @@
       <c r="J41" s="10" t="n">
         <v>44.49099390323</v>
       </c>
+      <c r="K41" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L41" s="10" t="n">
+        <v>0.01411509507135675</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="10" t="n">
@@ -2328,6 +2581,12 @@
       <c r="J42" s="10" t="n">
         <v>44.49099390323</v>
       </c>
+      <c r="K42" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L42" s="10" t="n">
+        <v>0.2991480473667453</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="10" t="n">
@@ -2363,6 +2622,12 @@
       </c>
       <c r="J43" s="10" t="n">
         <v>44.49099390323</v>
+      </c>
+      <c r="K43" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L43" s="10" t="n">
+        <v>24.64686592336117</v>
       </c>
     </row>
     <row r="44">
@@ -2378,16 +2643,12 @@
         <v>1230.27</v>
       </c>
       <c r="F44" s="10" t="inlineStr"/>
-      <c r="G44" s="10" t="n">
-        <v>-1</v>
-      </c>
+      <c r="G44" s="10" t="inlineStr"/>
       <c r="H44" s="10" t="inlineStr"/>
-      <c r="I44" s="10" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J44" s="10" t="n">
-        <v>22250.38010948243</v>
-      </c>
+      <c r="I44" s="10" t="inlineStr"/>
+      <c r="J44" s="10" t="inlineStr"/>
+      <c r="K44" s="10" t="inlineStr"/>
+      <c r="L44" s="10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2400,7 +2661,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2418,6 +2679,8 @@
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
     <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="16" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2471,6 +2734,16 @@
           <t>Prodx_Rate(pps)</t>
         </is>
       </c>
+      <c r="K1" s="9" t="inlineStr">
+        <is>
+          <t>Stop_Ratio</t>
+        </is>
+      </c>
+      <c r="L1" s="9" t="inlineStr">
+        <is>
+          <t>Prodx_A(Bq)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
@@ -2507,6 +2780,12 @@
       <c r="J2" s="10" t="n">
         <v>29.47980490335971</v>
       </c>
+      <c r="K2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="10" t="n">
+        <v>15.08584168635466</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="n">
@@ -2543,6 +2822,12 @@
       <c r="J3" s="10" t="n">
         <v>29.47980490335971</v>
       </c>
+      <c r="K3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <v>19.16370833124201</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
@@ -2579,6 +2864,12 @@
       <c r="J4" s="10" t="n">
         <v>2387.321624075756</v>
       </c>
+      <c r="K4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="10" t="n">
+        <v>1725.766029116671</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="n">
@@ -2615,6 +2906,12 @@
       <c r="J5" s="10" t="n">
         <v>2387.321624075756</v>
       </c>
+      <c r="K5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10" t="n">
+        <v>2387.321624075756</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="n">
@@ -2651,6 +2948,12 @@
       <c r="J6" s="10" t="n">
         <v>1369.092779867688</v>
       </c>
+      <c r="K6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="10" t="n">
+        <v>138.4545370616962</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n">
@@ -2687,6 +2990,12 @@
       <c r="J7" s="10" t="n">
         <v>191.709160721235</v>
       </c>
+      <c r="K7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="10" t="n">
+        <v>1.085483613747827e-12</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="n">
@@ -2723,6 +3032,12 @@
       <c r="J8" s="10" t="n">
         <v>191.709160721235</v>
       </c>
+      <c r="K8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="10" t="n">
+        <v>191.709160721235</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n">
@@ -2759,6 +3074,12 @@
       <c r="J9" s="10" t="n">
         <v>2893.723180697886</v>
       </c>
+      <c r="K9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="10" t="n">
+        <v>2890.184168539575</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n">
@@ -2795,6 +3116,12 @@
       <c r="J10" s="10" t="n">
         <v>2893.723180697886</v>
       </c>
+      <c r="K10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="10" t="n">
+        <v>2892.74870392612</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="n">
@@ -2831,6 +3158,12 @@
       <c r="J11" s="10" t="n">
         <v>3798.011674665975</v>
       </c>
+      <c r="K11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="10" t="n">
+        <v>2.15048640459475e-11</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n">
@@ -2867,6 +3200,12 @@
       <c r="J12" s="10" t="n">
         <v>191.709160721235</v>
       </c>
+      <c r="K12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>157.9048910842452</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="n">
@@ -2903,6 +3242,12 @@
       <c r="J13" s="10" t="n">
         <v>191.709160721235</v>
       </c>
+      <c r="K13" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="10" t="n">
+        <v>0.6673865968059928</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="n">
@@ -2939,6 +3284,12 @@
       <c r="J14" s="10" t="n">
         <v>14.70373091192113</v>
       </c>
+      <c r="K14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="10" t="n">
+        <v>8.325454509216819e-14</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="n">
@@ -2975,6 +3326,12 @@
       <c r="J15" s="10" t="n">
         <v>44.12927850564276</v>
       </c>
+      <c r="K15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="10" t="n">
+        <v>44.1171725767845</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="n">
@@ -3011,6 +3368,12 @@
       <c r="J16" s="10" t="n">
         <v>44.12927850564276</v>
       </c>
+      <c r="K16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="10" t="n">
+        <v>44.12927850564276</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="n">
@@ -3047,6 +3410,12 @@
       <c r="J17" s="10" t="n">
         <v>1558.993363600986</v>
       </c>
+      <c r="K17" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="10" t="n">
+        <v>704.141187794839</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="n">
@@ -3083,6 +3452,12 @@
       <c r="J18" s="10" t="n">
         <v>1558.993363600986</v>
       </c>
+      <c r="K18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="10" t="n">
+        <v>1108.383651097571</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="n">
@@ -3119,6 +3494,12 @@
       <c r="J19" s="10" t="n">
         <v>441.2927850564276</v>
       </c>
+      <c r="K19" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="10" t="n">
+        <v>2.498660393910091e-12</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="n">
@@ -3155,6 +3536,12 @@
       <c r="J20" s="10" t="n">
         <v>1249.726698663899</v>
       </c>
+      <c r="K20" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="10" t="n">
+        <v>586.0444770629599</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="n">
@@ -3191,6 +3578,12 @@
       <c r="J21" s="10" t="n">
         <v>235.1150084317032</v>
       </c>
+      <c r="K21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="10" t="n">
+        <v>0.3992219686171868</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -3227,6 +3620,12 @@
       <c r="J22" s="10" t="n">
         <v>191.709160721235</v>
       </c>
+      <c r="K22" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" s="10" t="n">
+        <v>0.004595712465723449</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="n">
@@ -3263,6 +3662,12 @@
       <c r="J23" s="10" t="n">
         <v>191.709160721235</v>
       </c>
+      <c r="K23" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="10" t="n">
+        <v>1.27125068713831</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="n">
@@ -3299,6 +3704,12 @@
       <c r="J24" s="10" t="n">
         <v>14.70373091192113</v>
       </c>
+      <c r="K24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" s="10" t="n">
+        <v>8.325454509216819e-14</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="n">
@@ -3335,6 +3746,12 @@
       <c r="J25" s="10" t="n">
         <v>88.25855701128552</v>
       </c>
+      <c r="K25" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" s="10" t="n">
+        <v>2.933703636036848</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="n">
@@ -3371,6 +3788,12 @@
       <c r="J26" s="10" t="n">
         <v>88.25855701128552</v>
       </c>
+      <c r="K26" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" s="10" t="n">
+        <v>88.24808301649365</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="10" t="n">
@@ -3406,6 +3829,12 @@
       </c>
       <c r="J27" s="10" t="n">
         <v>14.70373091192113</v>
+      </c>
+      <c r="K27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" s="10" t="n">
+        <v>0.0001938664069082156</v>
       </c>
     </row>
     <row r="28">
@@ -3421,16 +3850,12 @@
         <v>813.499</v>
       </c>
       <c r="F28" s="10" t="inlineStr"/>
-      <c r="G28" s="10" t="n">
-        <v>-1</v>
-      </c>
+      <c r="G28" s="10" t="inlineStr"/>
       <c r="H28" s="10" t="inlineStr"/>
-      <c r="I28" s="10" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J28" s="10" t="n">
-        <v>14712.75571109093</v>
-      </c>
+      <c r="I28" s="10" t="inlineStr"/>
+      <c r="J28" s="10" t="inlineStr"/>
+      <c r="K28" s="10" t="inlineStr"/>
+      <c r="L28" s="10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3443,7 +3868,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3461,6 +3886,8 @@
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
     <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="16" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3514,6 +3941,16 @@
           <t>Prodx_Rate(pps)</t>
         </is>
       </c>
+      <c r="K1" s="9" t="inlineStr">
+        <is>
+          <t>Stop_Ratio</t>
+        </is>
+      </c>
+      <c r="L1" s="9" t="inlineStr">
+        <is>
+          <t>Prodx_A(Bq)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
@@ -3550,6 +3987,12 @@
       <c r="J2" s="10" t="n">
         <v>676.4077934881309</v>
       </c>
+      <c r="K2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="10" t="n">
+        <v>488.9670415830567</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="n">
@@ -3586,6 +4029,12 @@
       <c r="J3" s="10" t="n">
         <v>676.4077934881309</v>
       </c>
+      <c r="K3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <v>676.4077934881309</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
@@ -3622,6 +4071,12 @@
       <c r="J4" s="10" t="n">
         <v>392.4612063821507</v>
       </c>
+      <c r="K4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="10" t="n">
+        <v>39.68908129773853</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="n">
@@ -3658,6 +4113,12 @@
       <c r="J5" s="10" t="n">
         <v>35.62896666234272</v>
       </c>
+      <c r="K5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10" t="n">
+        <v>2.017361055738885e-13</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="n">
@@ -3694,6 +4155,12 @@
       <c r="J6" s="10" t="n">
         <v>35.62896666234272</v>
       </c>
+      <c r="K6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="10" t="n">
+        <v>35.62896666234272</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n">
@@ -3730,6 +4197,12 @@
       <c r="J7" s="10" t="n">
         <v>3237.35280840576</v>
       </c>
+      <c r="K7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="10" t="n">
+        <v>3233.39353855365</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="n">
@@ -3766,6 +4239,12 @@
       <c r="J8" s="10" t="n">
         <v>3237.35280840576</v>
       </c>
+      <c r="K8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="10" t="n">
+        <v>3236.262612517346</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n">
@@ -3802,6 +4281,12 @@
       <c r="J9" s="10" t="n">
         <v>5479.988273446622</v>
       </c>
+      <c r="K9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="10" t="n">
+        <v>3.102844669486712e-11</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n">
@@ -3838,6 +4323,12 @@
       <c r="J10" s="10" t="n">
         <v>605.87329095862</v>
       </c>
+      <c r="K10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="10" t="n">
+        <v>499.0390425775672</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="n">
@@ -3874,6 +4365,12 @@
       <c r="J11" s="10" t="n">
         <v>605.87329095862</v>
       </c>
+      <c r="K11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="10" t="n">
+        <v>2.109193489905732</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n">
@@ -3910,6 +4407,12 @@
       <c r="J12" s="10" t="n">
         <v>285.7551640939163</v>
       </c>
+      <c r="K12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>285.6767732431128</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="n">
@@ -3946,6 +4449,12 @@
       <c r="J13" s="10" t="n">
         <v>285.7551640939163</v>
       </c>
+      <c r="K13" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="10" t="n">
+        <v>285.7551640939163</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="n">
@@ -3982,6 +4491,12 @@
       <c r="J14" s="10" t="n">
         <v>694.4935633674926</v>
       </c>
+      <c r="K14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="10" t="n">
+        <v>366.1719341048212</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="n">
@@ -4018,6 +4533,12 @@
       <c r="J15" s="10" t="n">
         <v>178.1448333117136</v>
       </c>
+      <c r="K15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="10" t="n">
+        <v>0.1245370271005934</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="n">
@@ -4054,6 +4575,12 @@
       <c r="J16" s="10" t="n">
         <v>178.1448333117136</v>
       </c>
+      <c r="K16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="10" t="n">
+        <v>177.5784252223669</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="n">
@@ -4090,6 +4617,12 @@
       <c r="J17" s="10" t="n">
         <v>907.9056479439618</v>
       </c>
+      <c r="K17" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="10" t="n">
+        <v>410.0683019408459</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="n">
@@ -4126,6 +4659,12 @@
       <c r="J18" s="10" t="n">
         <v>907.9056479439618</v>
       </c>
+      <c r="K18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="10" t="n">
+        <v>645.4856065556621</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="n">
@@ -4162,6 +4701,12 @@
       <c r="J19" s="10" t="n">
         <v>285.7551640939163</v>
       </c>
+      <c r="K19" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="10" t="n">
+        <v>1.617985009171289e-12</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="n">
@@ -4198,6 +4743,12 @@
       <c r="J20" s="10" t="n">
         <v>2947.980490335971</v>
       </c>
+      <c r="K20" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="10" t="n">
+        <v>1382.420401754884</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="n">
@@ -4234,6 +4785,12 @@
       <c r="J21" s="10" t="n">
         <v>1032.697460111558</v>
       </c>
+      <c r="K21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="10" t="n">
+        <v>1.75350572369549</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -4270,6 +4827,12 @@
       <c r="J22" s="10" t="n">
         <v>35.62896666234272</v>
       </c>
+      <c r="K22" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" s="10" t="n">
+        <v>2.017361055738885e-13</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="n">
@@ -4306,6 +4869,12 @@
       <c r="J23" s="10" t="n">
         <v>35.62896666234272</v>
       </c>
+      <c r="K23" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="10" t="n">
+        <v>18.64673800138327</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="n">
@@ -4342,6 +4911,12 @@
       <c r="J24" s="10" t="n">
         <v>195.3263146971073</v>
       </c>
+      <c r="K24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" s="10" t="n">
+        <v>187.5474083595894</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="n">
@@ -4378,6 +4953,12 @@
       <c r="J25" s="10" t="n">
         <v>195.3263146971073</v>
       </c>
+      <c r="K25" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" s="10" t="n">
+        <v>194.4441075865556</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="n">
@@ -4414,6 +4995,12 @@
       <c r="J26" s="10" t="n">
         <v>106.8868999870282</v>
       </c>
+      <c r="K26" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" s="10" t="n">
+        <v>6.052083167216657e-13</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="10" t="n">
@@ -4450,6 +5037,12 @@
       <c r="J27" s="10" t="n">
         <v>35.62896666234272</v>
       </c>
+      <c r="K27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" s="10" t="n">
+        <v>0.004962444599216784</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="10" t="n">
@@ -4486,6 +5079,12 @@
       <c r="J28" s="10" t="n">
         <v>35.62896666234272</v>
       </c>
+      <c r="K28" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" s="10" t="n">
+        <v>0.0007532237084180774</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="10" t="n">
@@ -4522,6 +5121,12 @@
       <c r="J29" s="10" t="n">
         <v>195.3263146971073</v>
       </c>
+      <c r="K29" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="10" t="n">
+        <v>0.004682424021680493</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="n">
@@ -4558,6 +5163,12 @@
       <c r="J30" s="10" t="n">
         <v>195.3263146971073</v>
       </c>
+      <c r="K30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="10" t="n">
+        <v>1.295236549159788</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="10" t="n">
@@ -4594,6 +5205,12 @@
       <c r="J31" s="10" t="n">
         <v>35.62896666234272</v>
       </c>
+      <c r="K31" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" s="10" t="n">
+        <v>2.017361055738885e-13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="10" t="n">
@@ -4630,6 +5247,12 @@
       <c r="J32" s="10" t="n">
         <v>374.375436502789</v>
       </c>
+      <c r="K32" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" s="10" t="n">
+        <v>12.44419370204155</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="n">
@@ -4666,6 +5289,12 @@
       <c r="J33" s="10" t="n">
         <v>374.375436502789</v>
       </c>
+      <c r="K33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" s="10" t="n">
+        <v>374.3310078773399</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="10" t="n">
@@ -4702,6 +5331,12 @@
       <c r="J34" s="10" t="n">
         <v>35.62896666234272</v>
       </c>
+      <c r="K34" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" s="10" t="n">
+        <v>2.017361055738885e-13</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="10" t="n">
@@ -4738,6 +5373,12 @@
       <c r="J35" s="10" t="n">
         <v>17.81448333117136</v>
       </c>
+      <c r="K35" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" s="10" t="n">
+        <v>0.03192125498824115</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="n">
@@ -4773,6 +5414,12 @@
       </c>
       <c r="J36" s="10" t="n">
         <v>17.81448333117136</v>
+      </c>
+      <c r="K36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" s="10" t="n">
+        <v>2.442217154614803</v>
       </c>
     </row>
     <row r="37">
@@ -4788,16 +5435,12 @@
         <v>984.693</v>
       </c>
       <c r="F37" s="10" t="inlineStr"/>
-      <c r="G37" s="10" t="n">
-        <v>-1</v>
-      </c>
+      <c r="G37" s="10" t="inlineStr"/>
       <c r="H37" s="10" t="inlineStr"/>
-      <c r="I37" s="10" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J37" s="10" t="n">
-        <v>17808.9309998184</v>
-      </c>
+      <c r="I37" s="10" t="inlineStr"/>
+      <c r="J37" s="10" t="inlineStr"/>
+      <c r="K37" s="10" t="inlineStr"/>
+      <c r="L37" s="10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4810,7 +5453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4828,6 +5471,8 @@
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
     <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="16" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4881,6 +5526,16 @@
           <t>Prodx_Rate(pps)</t>
         </is>
       </c>
+      <c r="K1" s="9" t="inlineStr">
+        <is>
+          <t>Stop_Ratio</t>
+        </is>
+      </c>
+      <c r="L1" s="9" t="inlineStr">
+        <is>
+          <t>Prodx_A(Bq)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
@@ -4917,6 +5572,12 @@
       <c r="J2" s="10" t="n">
         <v>182.6662757815541</v>
       </c>
+      <c r="K2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="10" t="n">
+        <v>132.0472491975635</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="n">
@@ -4953,6 +5614,12 @@
       <c r="J3" s="10" t="n">
         <v>182.6662757815541</v>
       </c>
+      <c r="K3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <v>182.6662757815541</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
@@ -4989,6 +5656,12 @@
       <c r="J4" s="10" t="n">
         <v>81.20510675833441</v>
       </c>
+      <c r="K4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="10" t="n">
+        <v>8.212164747780921</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="n">
@@ -5025,6 +5698,12 @@
       <c r="J5" s="10" t="n">
         <v>20.25606226488521</v>
       </c>
+      <c r="K5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10" t="n">
+        <v>1.146926082450534e-13</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="n">
@@ -5061,6 +5740,12 @@
       <c r="J6" s="10" t="n">
         <v>20.25606226488521</v>
       </c>
+      <c r="K6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="10" t="n">
+        <v>20.25606226488521</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n">
@@ -5097,6 +5782,12 @@
       <c r="J7" s="10" t="n">
         <v>2116.03507588533</v>
       </c>
+      <c r="K7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="10" t="n">
+        <v>2113.447173244565</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="n">
@@ -5133,6 +5824,12 @@
       <c r="J8" s="10" t="n">
         <v>2116.03507588533</v>
       </c>
+      <c r="K8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="10" t="n">
+        <v>2115.322489745976</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n">
@@ -5169,6 +5866,12 @@
       <c r="J9" s="10" t="n">
         <v>3472.467816837463</v>
       </c>
+      <c r="K9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="10" t="n">
+        <v>1.966158998486629e-11</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n">
@@ -5205,6 +5908,12 @@
       <c r="J10" s="10" t="n">
         <v>750.5594499935142</v>
       </c>
+      <c r="K10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="10" t="n">
+        <v>618.2125452826577</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="n">
@@ -5241,6 +5950,12 @@
       <c r="J11" s="10" t="n">
         <v>750.5594499935142</v>
       </c>
+      <c r="K11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="10" t="n">
+        <v>2.61288148749516</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n">
@@ -5277,6 +5992,12 @@
       <c r="J12" s="10" t="n">
         <v>1095.997654689324</v>
       </c>
+      <c r="K12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>1095.696991046369</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="n">
@@ -5313,6 +6034,12 @@
       <c r="J13" s="10" t="n">
         <v>1095.997654689324</v>
       </c>
+      <c r="K13" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="10" t="n">
+        <v>1095.997654689324</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="n">
@@ -5349,6 +6076,12 @@
       <c r="J14" s="10" t="n">
         <v>3562.896666234272</v>
       </c>
+      <c r="K14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="10" t="n">
+        <v>1878.538307777338</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="n">
@@ -5385,6 +6118,12 @@
       <c r="J15" s="10" t="n">
         <v>730.6651031262163</v>
       </c>
+      <c r="K15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="10" t="n">
+        <v>0.51079146140751</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="n">
@@ -5421,6 +6160,12 @@
       <c r="J16" s="10" t="n">
         <v>730.6651031262163</v>
       </c>
+      <c r="K16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="10" t="n">
+        <v>728.3419674095049</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="n">
@@ -5457,6 +6202,12 @@
       <c r="J17" s="10" t="n">
         <v>40.51212452977042</v>
       </c>
+      <c r="K17" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="10" t="n">
+        <v>2.293852164901068e-13</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="n">
@@ -5493,6 +6244,12 @@
       <c r="J18" s="10" t="n">
         <v>345.4382046958102</v>
       </c>
+      <c r="K18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="10" t="n">
+        <v>156.0220033280908</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="n">
@@ -5529,6 +6286,12 @@
       <c r="J19" s="10" t="n">
         <v>345.4382046958102</v>
       </c>
+      <c r="K19" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="10" t="n">
+        <v>245.5931291875129</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="n">
@@ -5565,6 +6328,12 @@
       <c r="J20" s="10" t="n">
         <v>101.4611690232197</v>
       </c>
+      <c r="K20" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="10" t="n">
+        <v>5.744870823703124e-13</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="n">
@@ -5601,6 +6370,12 @@
       <c r="J21" s="10" t="n">
         <v>2857.551640939163</v>
       </c>
+      <c r="K21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="10" t="n">
+        <v>1340.014867958722</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -5637,6 +6412,12 @@
       <c r="J22" s="10" t="n">
         <v>1338.346971072772</v>
       </c>
+      <c r="K22" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" s="10" t="n">
+        <v>2.272494282897832</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="n">
@@ -5673,6 +6454,12 @@
       <c r="J23" s="10" t="n">
         <v>60.7681867946556</v>
       </c>
+      <c r="K23" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="10" t="n">
+        <v>3.440778247351601e-13</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="n">
@@ -5709,6 +6496,12 @@
       <c r="J24" s="10" t="n">
         <v>60.7681867946556</v>
       </c>
+      <c r="K24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" s="10" t="n">
+        <v>31.80357344398364</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="n">
@@ -5745,6 +6538,12 @@
       <c r="J25" s="10" t="n">
         <v>1540.907593721624</v>
       </c>
+      <c r="K25" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" s="10" t="n">
+        <v>1479.540665947872</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="n">
@@ -5781,6 +6580,12 @@
       <c r="J26" s="10" t="n">
         <v>1540.907593721624</v>
       </c>
+      <c r="K26" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" s="10" t="n">
+        <v>1533.947959849494</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="10" t="n">
@@ -5817,6 +6622,12 @@
       <c r="J27" s="10" t="n">
         <v>730.6651031262163</v>
       </c>
+      <c r="K27" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" s="10" t="n">
+        <v>4.137126225982283e-12</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="10" t="n">
@@ -5853,6 +6664,12 @@
       <c r="J28" s="10" t="n">
         <v>81.20510675833441</v>
       </c>
+      <c r="K28" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" s="10" t="n">
+        <v>0.001946674431235686</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="10" t="n">
@@ -5889,6 +6706,12 @@
       <c r="J29" s="10" t="n">
         <v>81.20510675833441</v>
       </c>
+      <c r="K29" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="10" t="n">
+        <v>0.5384826023821708</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="n">
@@ -5925,6 +6748,12 @@
       <c r="J30" s="10" t="n">
         <v>750.5594499935142</v>
       </c>
+      <c r="K30" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L30" s="10" t="n">
+        <v>24.94850428187074</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="10" t="n">
@@ -5961,6 +6790,12 @@
       <c r="J31" s="10" t="n">
         <v>750.5594499935142</v>
       </c>
+      <c r="K31" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L31" s="10" t="n">
+        <v>750.4703781115753</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="10" t="n">
@@ -5997,6 +6832,12 @@
       <c r="J32" s="10" t="n">
         <v>81.20510675833441</v>
       </c>
+      <c r="K32" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L32" s="10" t="n">
+        <v>4.597944741252585e-13</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="n">
@@ -6033,6 +6874,12 @@
       <c r="J33" s="10" t="n">
         <v>222.45496951615</v>
       </c>
+      <c r="K33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" s="10" t="n">
+        <v>0.3986105952846358</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="10" t="n">
@@ -6069,6 +6916,12 @@
       <c r="J34" s="10" t="n">
         <v>222.45496951615</v>
       </c>
+      <c r="K34" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L34" s="10" t="n">
+        <v>30.49672182920008</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="10" t="n">
@@ -6105,6 +6958,12 @@
       <c r="J35" s="10" t="n">
         <v>40.51212452977042</v>
       </c>
+      <c r="K35" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L35" s="10" t="n">
+        <v>2.293852164901068e-13</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="n">
@@ -6141,6 +7000,12 @@
       <c r="J36" s="10" t="n">
         <v>60.7681867946556</v>
       </c>
+      <c r="K36" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" s="10" t="n">
+        <v>0.00080121909866126</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="10" t="n">
@@ -6177,6 +7042,12 @@
       <c r="J37" s="10" t="n">
         <v>60.7681867946556</v>
       </c>
+      <c r="K37" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L37" s="10" t="n">
+        <v>0.01927915424380434</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="10" t="n">
@@ -6213,6 +7084,12 @@
       <c r="J38" s="10" t="n">
         <v>20.25606226488521</v>
       </c>
+      <c r="K38" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L38" s="10" t="n">
+        <v>0.0004006082288352761</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="10" t="n">
@@ -6248,6 +7125,12 @@
       </c>
       <c r="J39" s="10" t="n">
         <v>20.25606226488521</v>
+      </c>
+      <c r="K39" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L39" s="10" t="n">
+        <v>20.22956030998986</v>
       </c>
     </row>
     <row r="40">
@@ -6263,16 +7146,12 @@
         <v>1121.6</v>
       </c>
       <c r="F40" s="10" t="inlineStr"/>
-      <c r="G40" s="10" t="n">
-        <v>-1</v>
-      </c>
+      <c r="G40" s="10" t="inlineStr"/>
       <c r="H40" s="10" t="inlineStr"/>
-      <c r="I40" s="10" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J40" s="10" t="n">
-        <v>20284.99949669218</v>
-      </c>
+      <c r="I40" s="10" t="inlineStr"/>
+      <c r="J40" s="10" t="inlineStr"/>
+      <c r="K40" s="10" t="inlineStr"/>
+      <c r="L40" s="10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6285,7 +7164,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6303,6 +7182,8 @@
     <col width="16" customWidth="1" min="8" max="8"/>
     <col width="16" customWidth="1" min="9" max="9"/>
     <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="16" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6356,6 +7237,16 @@
           <t>Prodx_Rate(pps)</t>
         </is>
       </c>
+      <c r="K1" s="9" t="inlineStr">
+        <is>
+          <t>Stop_Ratio</t>
+        </is>
+      </c>
+      <c r="L1" s="9" t="inlineStr">
+        <is>
+          <t>Prodx_A(Bq)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
@@ -6392,6 +7283,12 @@
       <c r="J2" s="10" t="n">
         <v>245.9664703593203</v>
       </c>
+      <c r="K2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="10" t="n">
+        <v>125.869599346272</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="10" t="n">
@@ -6428,6 +7325,12 @@
       <c r="J3" s="10" t="n">
         <v>245.9664703593203</v>
       </c>
+      <c r="K3" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <v>159.893517364964</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
@@ -6464,6 +7367,12 @@
       <c r="J4" s="10" t="n">
         <v>74.69422960176418</v>
       </c>
+      <c r="K4" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="10" t="n">
+        <v>4.229289929036343e-13</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="n">
@@ -6500,6 +7409,12 @@
       <c r="J5" s="10" t="n">
         <v>4521.442469840447</v>
       </c>
+      <c r="K5" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10" t="n">
+        <v>3268.496267266422</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="n">
@@ -6536,6 +7451,12 @@
       <c r="J6" s="10" t="n">
         <v>4521.442469840447</v>
       </c>
+      <c r="K6" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="10" t="n">
+        <v>4521.442469840447</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="n">
@@ -6572,6 +7493,12 @@
       <c r="J7" s="10" t="n">
         <v>2296.892774678947</v>
       </c>
+      <c r="K7" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="10" t="n">
+        <v>232.2817200374559</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="n">
@@ -6608,6 +7535,12 @@
       <c r="J8" s="10" t="n">
         <v>117.376646517058</v>
       </c>
+      <c r="K8" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="10" t="n">
+        <v>6.646027031342825e-13</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n">
@@ -6644,6 +7577,12 @@
       <c r="J9" s="10" t="n">
         <v>117.376646517058</v>
       </c>
+      <c r="K9" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="10" t="n">
+        <v>117.376646517058</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="n">
@@ -6680,6 +7619,12 @@
       <c r="J10" s="10" t="n">
         <v>618.5333298741731</v>
       </c>
+      <c r="K10" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="10" t="n">
+        <v>617.7768660253341</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="n">
@@ -6716,6 +7661,12 @@
       <c r="J11" s="10" t="n">
         <v>618.5333298741731</v>
       </c>
+      <c r="K11" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="10" t="n">
+        <v>618.325035464208</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n">
@@ -6752,6 +7703,12 @@
       <c r="J12" s="10" t="n">
         <v>544.3816733687898</v>
       </c>
+      <c r="K12" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>3.08236384658581e-12</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="n">
@@ -6788,6 +7745,12 @@
       <c r="J13" s="10" t="n">
         <v>21.3412084576469</v>
       </c>
+      <c r="K13" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="10" t="n">
+        <v>17.57809164900086</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="n">
@@ -6824,6 +7787,12 @@
       <c r="J14" s="10" t="n">
         <v>21.3412084576469</v>
       </c>
+      <c r="K14" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="10" t="n">
+        <v>0.07429397964444065</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="n">
@@ -6860,6 +7829,12 @@
       <c r="J15" s="10" t="n">
         <v>160.0590634323518</v>
       </c>
+      <c r="K15" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="10" t="n">
+        <v>0.111893674095457</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="n">
@@ -6896,6 +7871,12 @@
       <c r="J16" s="10" t="n">
         <v>160.0590634323518</v>
       </c>
+      <c r="K16" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="10" t="n">
+        <v>159.5501587023296</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="n">
@@ -6932,6 +7913,12 @@
       <c r="J17" s="10" t="n">
         <v>42.68241691529381</v>
       </c>
+      <c r="K17" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="10" t="n">
+        <v>2.416737102306481e-13</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="n">
@@ -6968,6 +7955,12 @@
       <c r="J18" s="10" t="n">
         <v>1419.7329355299</v>
       </c>
+      <c r="K18" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L18" s="10" t="n">
+        <v>641.2422649871793</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="n">
@@ -7004,6 +7997,12 @@
       <c r="J19" s="10" t="n">
         <v>1419.7329355299</v>
       </c>
+      <c r="K19" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" s="10" t="n">
+        <v>1009.374902681663</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="n">
@@ -7040,6 +8039,12 @@
       <c r="J20" s="10" t="n">
         <v>383.4183214424699</v>
       </c>
+      <c r="K20" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L20" s="10" t="n">
+        <v>2.170967227495653e-12</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="n">
@@ -7076,6 +8081,12 @@
       <c r="J21" s="10" t="n">
         <v>117.376646517058</v>
       </c>
+      <c r="K21" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" s="10" t="n">
+        <v>55.0423828674184</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
@@ -7112,6 +8123,12 @@
       <c r="J22" s="10" t="n">
         <v>42.68241691529381</v>
       </c>
+      <c r="K22" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" s="10" t="n">
+        <v>0.07247414199512005</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="n">
@@ -7148,6 +8165,12 @@
       <c r="J23" s="10" t="n">
         <v>21.3412084576469</v>
       </c>
+      <c r="K23" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="10" t="n">
+        <v>0.002972428744708529</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="n">
@@ -7184,6 +8207,12 @@
       <c r="J24" s="10" t="n">
         <v>21.3412084576469</v>
       </c>
+      <c r="K24" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" s="10" t="n">
+        <v>0.0004511695309306248</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="n">
@@ -7220,6 +8249,12 @@
       <c r="J25" s="10" t="n">
         <v>42.68241691529381</v>
       </c>
+      <c r="K25" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" s="10" t="n">
+        <v>0.001023196360293145</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="n">
@@ -7255,6 +8290,12 @@
       </c>
       <c r="J26" s="10" t="n">
         <v>42.68241691529381</v>
+      </c>
+      <c r="K26" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" s="10" t="n">
+        <v>0.283033171853435</v>
       </c>
     </row>
     <row r="27">
@@ -7270,15 +8311,1495 @@
         <v>590.221</v>
       </c>
       <c r="F27" s="10" t="inlineStr"/>
+      <c r="G27" s="10" t="inlineStr"/>
+      <c r="H27" s="10" t="inlineStr"/>
+      <c r="I27" s="10" t="inlineStr"/>
+      <c r="J27" s="10" t="inlineStr"/>
+      <c r="K27" s="10" t="inlineStr"/>
+      <c r="L27" s="10" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="14" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B1" s="9" t="inlineStr">
+        <is>
+          <t>isotope</t>
+        </is>
+      </c>
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>A(Bq)@0um</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>A(Bq)@3um</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
+        <is>
+          <t>A(Bq)@6um</t>
+        </is>
+      </c>
+      <c r="F1" s="9" t="inlineStr">
+        <is>
+          <t>A(Bq)@9um</t>
+        </is>
+      </c>
+      <c r="G1" s="9" t="inlineStr">
+        <is>
+          <t>A(Bq)@12um</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="10" t="n">
+        <v>108</v>
+      </c>
+      <c r="B2" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="10" t="n">
+        <v>108</v>
+      </c>
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="10" t="n">
+        <v>15.09</v>
+      </c>
+      <c r="G3" s="10" t="n">
+        <v>125.87</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="10" t="n">
+        <v>108</v>
+      </c>
+      <c r="B4" s="10" t="inlineStr">
+        <is>
+          <t>In isomer</t>
+        </is>
+      </c>
+      <c r="C4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10" t="n">
+        <v>19.16</v>
+      </c>
+      <c r="G4" s="10" t="n">
+        <v>159.89</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="B5" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="C5" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>Ag isomer</t>
+        </is>
+      </c>
+      <c r="C6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10" t="n">
+        <v>20.26</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>35.63</v>
+      </c>
+      <c r="F6" s="10" t="n">
+        <v>191.71</v>
+      </c>
+      <c r="G6" s="10" t="n">
+        <v>117.38</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="B7" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="C7" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10" t="n">
+        <v>8.210000000000001</v>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>39.69</v>
+      </c>
+      <c r="F7" s="10" t="n">
+        <v>138.45</v>
+      </c>
+      <c r="G7" s="10" t="n">
+        <v>232.28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="B8" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="C8" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10" t="n">
+        <v>132.05</v>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>488.97</v>
+      </c>
+      <c r="F8" s="10" t="n">
+        <v>1725.77</v>
+      </c>
+      <c r="G8" s="10" t="n">
+        <v>3268.5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="n">
+        <v>107</v>
+      </c>
+      <c r="B9" s="10" t="inlineStr">
+        <is>
+          <t>In isomer</t>
+        </is>
+      </c>
+      <c r="C9" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10" t="n">
+        <v>182.67</v>
+      </c>
+      <c r="E9" s="10" t="n">
+        <v>676.41</v>
+      </c>
+      <c r="F9" s="10" t="n">
+        <v>2387.32</v>
+      </c>
+      <c r="G9" s="10" t="n">
+        <v>4521.44</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="B10" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="C10" s="10" t="n">
+        <v>128.26</v>
+      </c>
+      <c r="D10" s="10" t="n">
+        <v>618.21</v>
+      </c>
+      <c r="E10" s="10" t="n">
+        <v>499.04</v>
+      </c>
+      <c r="F10" s="10" t="n">
+        <v>157.9</v>
+      </c>
+      <c r="G10" s="10" t="n">
+        <v>17.58</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="B11" s="10" t="inlineStr">
+        <is>
+          <t>Ag isomer</t>
+        </is>
+      </c>
+      <c r="C11" s="10" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="D11" s="10" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="B12" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="C13" s="10" t="n">
+        <v>733.38</v>
+      </c>
+      <c r="D13" s="10" t="n">
+        <v>2113.45</v>
+      </c>
+      <c r="E13" s="10" t="n">
+        <v>3233.39</v>
+      </c>
+      <c r="F13" s="10" t="n">
+        <v>2890.18</v>
+      </c>
+      <c r="G13" s="10" t="n">
+        <v>617.78</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t>In isomer</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="n">
+        <v>734.03</v>
+      </c>
+      <c r="D14" s="10" t="n">
+        <v>2115.32</v>
+      </c>
+      <c r="E14" s="10" t="n">
+        <v>3236.26</v>
+      </c>
+      <c r="F14" s="10" t="n">
+        <v>2892.75</v>
+      </c>
+      <c r="G14" s="10" t="n">
+        <v>618.33</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="n">
+        <v>106</v>
+      </c>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="C16" s="10" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="D16" s="10" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E16" s="10" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="F16" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="10" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="B17" s="10" t="inlineStr">
+        <is>
+          <t>Ag isomer</t>
+        </is>
+      </c>
+      <c r="C17" s="10" t="n">
+        <v>1242.15</v>
+      </c>
+      <c r="D17" s="10" t="n">
+        <v>728.34</v>
+      </c>
+      <c r="E17" s="10" t="n">
+        <v>177.58</v>
+      </c>
+      <c r="F17" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10" t="n">
+        <v>159.55</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="B18" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="C18" s="10" t="n">
+        <v>3051.43</v>
+      </c>
+      <c r="D18" s="10" t="n">
+        <v>1878.54</v>
+      </c>
+      <c r="E18" s="10" t="n">
+        <v>366.17</v>
+      </c>
+      <c r="F18" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="B19" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="C19" s="10" t="n">
+        <v>1312.67</v>
+      </c>
+      <c r="D19" s="10" t="n">
+        <v>1095.7</v>
+      </c>
+      <c r="E19" s="10" t="n">
+        <v>285.68</v>
+      </c>
+      <c r="F19" s="10" t="n">
+        <v>44.12</v>
+      </c>
+      <c r="G19" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="B20" s="10" t="inlineStr">
+        <is>
+          <t>In isomer</t>
+        </is>
+      </c>
+      <c r="C20" s="10" t="n">
+        <v>1313.03</v>
+      </c>
+      <c r="D20" s="10" t="n">
+        <v>1096</v>
+      </c>
+      <c r="E20" s="10" t="n">
+        <v>285.76</v>
+      </c>
+      <c r="F20" s="10" t="n">
+        <v>44.13</v>
+      </c>
+      <c r="G20" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="n">
+        <v>105</v>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="C21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="C22" s="10" t="n">
+        <v>170.73</v>
+      </c>
+      <c r="D22" s="10" t="n">
+        <v>156.02</v>
+      </c>
+      <c r="E22" s="10" t="n">
+        <v>410.07</v>
+      </c>
+      <c r="F22" s="10" t="n">
+        <v>704.14</v>
+      </c>
+      <c r="G22" s="10" t="n">
+        <v>641.24</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="B23" s="10" t="inlineStr">
+        <is>
+          <t>Ag isomer</t>
+        </is>
+      </c>
+      <c r="C23" s="10" t="n">
+        <v>268.74</v>
+      </c>
+      <c r="D23" s="10" t="n">
+        <v>245.59</v>
+      </c>
+      <c r="E23" s="10" t="n">
+        <v>645.49</v>
+      </c>
+      <c r="F23" s="10" t="n">
+        <v>1108.38</v>
+      </c>
+      <c r="G23" s="10" t="n">
+        <v>1009.37</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="B24" s="10" t="inlineStr">
+        <is>
+          <t>Cd</t>
+        </is>
+      </c>
+      <c r="C24" s="10" t="n">
+        <v>480.19</v>
+      </c>
+      <c r="D24" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="B25" s="10" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="C25" s="10" t="n">
+        <v>88.98</v>
+      </c>
+      <c r="D25" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="10" t="n">
+        <v>104</v>
+      </c>
+      <c r="B26" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="C26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="B27" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="C27" s="10" t="n">
+        <v>720.05</v>
+      </c>
+      <c r="D27" s="10" t="n">
+        <v>1340.01</v>
+      </c>
+      <c r="E27" s="10" t="n">
+        <v>1382.42</v>
+      </c>
+      <c r="F27" s="10" t="n">
+        <v>586.04</v>
+      </c>
       <c r="G27" s="10" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H27" s="10" t="inlineStr"/>
-      <c r="I27" s="10" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J27" s="10" t="n">
-        <v>10674.60118396679</v>
+        <v>55.04</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="B28" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="C28" s="10" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="D28" s="10" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="E28" s="10" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="F28" s="10" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G28" s="10" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="B29" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="C29" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="B30" s="10" t="inlineStr">
+        <is>
+          <t>Rh isomer</t>
+        </is>
+      </c>
+      <c r="C30" s="10" t="n">
+        <v>46.57</v>
+      </c>
+      <c r="D30" s="10" t="n">
+        <v>31.8</v>
+      </c>
+      <c r="E30" s="10" t="n">
+        <v>18.65</v>
+      </c>
+      <c r="F30" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="10" t="n">
+        <v>103</v>
+      </c>
+      <c r="B31" s="10" t="inlineStr">
+        <is>
+          <t>Ru</t>
+        </is>
+      </c>
+      <c r="C31" s="10" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D31" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="10" t="n">
+        <v>102</v>
+      </c>
+      <c r="B32" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="C32" s="10" t="n">
+        <v>2726.38</v>
+      </c>
+      <c r="D32" s="10" t="n">
+        <v>1479.54</v>
+      </c>
+      <c r="E32" s="10" t="n">
+        <v>187.55</v>
+      </c>
+      <c r="F32" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="10" t="n">
+        <v>102</v>
+      </c>
+      <c r="B33" s="10" t="inlineStr">
+        <is>
+          <t>Ag isomer</t>
+        </is>
+      </c>
+      <c r="C33" s="10" t="n">
+        <v>2826.64</v>
+      </c>
+      <c r="D33" s="10" t="n">
+        <v>1533.95</v>
+      </c>
+      <c r="E33" s="10" t="n">
+        <v>194.44</v>
+      </c>
+      <c r="F33" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="10" t="n">
+        <v>102</v>
+      </c>
+      <c r="B34" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="C34" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="10" t="n">
+        <v>102</v>
+      </c>
+      <c r="B35" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="C35" s="10" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="D35" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="10" t="n">
+        <v>102</v>
+      </c>
+      <c r="B36" s="10" t="inlineStr">
+        <is>
+          <t>Rh isomer</t>
+        </is>
+      </c>
+      <c r="C36" s="10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D36" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="10" t="n">
+        <v>101</v>
+      </c>
+      <c r="B37" s="10" t="inlineStr">
+        <is>
+          <t>Ag</t>
+        </is>
+      </c>
+      <c r="C37" s="10" t="n">
+        <v>86.88</v>
+      </c>
+      <c r="D37" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="10" t="n">
+        <v>101</v>
+      </c>
+      <c r="B38" s="10" t="inlineStr">
+        <is>
+          <t>Pd</t>
+        </is>
+      </c>
+      <c r="C38" s="10" t="n">
+        <v>15.77</v>
+      </c>
+      <c r="D38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="10" t="n">
+        <v>101</v>
+      </c>
+      <c r="B39" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="C39" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="10" t="n">
+        <v>101</v>
+      </c>
+      <c r="B40" s="10" t="inlineStr">
+        <is>
+          <t>Rh isomer</t>
+        </is>
+      </c>
+      <c r="C40" s="10" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="D40" s="10" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="E40" s="10" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="F40" s="10" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="G40" s="10" t="n">
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="10" t="n">
+        <v>101</v>
+      </c>
+      <c r="B41" s="10" t="inlineStr">
+        <is>
+          <t>Ru</t>
+        </is>
+      </c>
+      <c r="C41" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="B42" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="C42" s="10" t="n">
+        <v>19.96</v>
+      </c>
+      <c r="D42" s="10" t="n">
+        <v>24.95</v>
+      </c>
+      <c r="E42" s="10" t="n">
+        <v>12.44</v>
+      </c>
+      <c r="F42" s="10" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="G42" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="B43" s="10" t="inlineStr">
+        <is>
+          <t>Rh isomer</t>
+        </is>
+      </c>
+      <c r="C43" s="10" t="n">
+        <v>600.38</v>
+      </c>
+      <c r="D43" s="10" t="n">
+        <v>750.47</v>
+      </c>
+      <c r="E43" s="10" t="n">
+        <v>374.33</v>
+      </c>
+      <c r="F43" s="10" t="n">
+        <v>88.25</v>
+      </c>
+      <c r="G43" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="B44" s="10" t="inlineStr">
+        <is>
+          <t>Ru</t>
+        </is>
+      </c>
+      <c r="C44" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="10" t="n">
+        <v>99</v>
+      </c>
+      <c r="B45" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="C45" s="10" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="D45" s="10" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E45" s="10" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="F45" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="10" t="n">
+        <v>99</v>
+      </c>
+      <c r="B46" s="10" t="inlineStr">
+        <is>
+          <t>Rh isomer</t>
+        </is>
+      </c>
+      <c r="C46" s="10" t="n">
+        <v>131.16</v>
+      </c>
+      <c r="D46" s="10" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="E46" s="10" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="F46" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="10" t="n">
+        <v>99</v>
+      </c>
+      <c r="B47" s="10" t="inlineStr">
+        <is>
+          <t>Ru</t>
+        </is>
+      </c>
+      <c r="C47" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="10" t="n">
+        <v>98</v>
+      </c>
+      <c r="B48" s="10" t="inlineStr">
+        <is>
+          <t>Rh</t>
+        </is>
+      </c>
+      <c r="C48" s="10" t="n">
+        <v>22.06</v>
+      </c>
+      <c r="D48" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="10" t="n">
+        <v>98</v>
+      </c>
+      <c r="B49" s="10" t="inlineStr">
+        <is>
+          <t>Rh isomer</t>
+        </is>
+      </c>
+      <c r="C49" s="10" t="n">
+        <v>22.25</v>
+      </c>
+      <c r="D49" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="10" t="n">
+        <v>98</v>
+      </c>
+      <c r="B50" s="10" t="inlineStr">
+        <is>
+          <t>Ru</t>
+        </is>
+      </c>
+      <c r="C50" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="10" t="n">
+        <v>98</v>
+      </c>
+      <c r="B51" s="10" t="inlineStr">
+        <is>
+          <t>Tc</t>
+        </is>
+      </c>
+      <c r="C51" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="10" t="n">
+        <v>97</v>
+      </c>
+      <c r="B52" s="10" t="inlineStr">
+        <is>
+          <t>Tc</t>
+        </is>
+      </c>
+      <c r="C52" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="10" t="n">
+        <v>97</v>
+      </c>
+      <c r="B53" s="10" t="inlineStr">
+        <is>
+          <t>Tc isomer</t>
+        </is>
+      </c>
+      <c r="C53" s="10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D53" s="10" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E53" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F53" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="10" t="n">
+        <v>96</v>
+      </c>
+      <c r="B54" s="10" t="inlineStr">
+        <is>
+          <t>Tc</t>
+        </is>
+      </c>
+      <c r="C54" s="10" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D54" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="10" t="n">
+        <v>96</v>
+      </c>
+      <c r="B55" s="10" t="inlineStr">
+        <is>
+          <t>Tc isomer</t>
+        </is>
+      </c>
+      <c r="C55" s="10" t="n">
+        <v>24.65</v>
+      </c>
+      <c r="D55" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="10" t="n">
+        <v>94</v>
+      </c>
+      <c r="B56" s="10" t="inlineStr">
+        <is>
+          <t>Nb</t>
+        </is>
+      </c>
+      <c r="C56" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="10" t="n">
+        <v>94</v>
+      </c>
+      <c r="B57" s="10" t="inlineStr">
+        <is>
+          <t>Nb isomer</t>
+        </is>
+      </c>
+      <c r="C57" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="10" t="n">
+        <v>20.23</v>
+      </c>
+      <c r="E57" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F57" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" s="10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="10" t="inlineStr"/>
+      <c r="B58" s="10" t="inlineStr"/>
+      <c r="C58" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on Does Parameters PDF file Reader
</commit_message>
<xml_diff>
--- a/example/DoesCal.xlsx
+++ b/example/DoesCal.xlsx
@@ -12,7 +12,7 @@
     <sheet name="6um_362MeV" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="3um_391MeV" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="12um_303MeV" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Summary" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Summary_A" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
@@ -8329,7 +8329,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8344,6 +8344,7 @@
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8382,6 +8383,11 @@
           <t>A(Bq)@12um</t>
         </is>
       </c>
+      <c r="H1" s="9" t="inlineStr">
+        <is>
+          <t>A(Bq)@cd = 0s</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
@@ -8389,7 +8395,7 @@
       </c>
       <c r="B2" s="10" t="inlineStr">
         <is>
-          <t>Cd</t>
+          <t>In</t>
         </is>
       </c>
       <c r="C2" s="10" t="n">
@@ -8402,10 +8408,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="10" t="n">
-        <v>0</v>
+        <v>15.09</v>
       </c>
       <c r="G2" s="10" t="n">
-        <v>0</v>
+        <v>125.87</v>
+      </c>
+      <c r="H2" s="10" t="n">
+        <v>140.96</v>
       </c>
     </row>
     <row r="3">
@@ -8414,7 +8423,7 @@
       </c>
       <c r="B3" s="10" t="inlineStr">
         <is>
-          <t>In</t>
+          <t>In isomer</t>
         </is>
       </c>
       <c r="C3" s="10" t="n">
@@ -8427,35 +8436,41 @@
         <v>0</v>
       </c>
       <c r="F3" s="10" t="n">
-        <v>15.09</v>
+        <v>19.16</v>
       </c>
       <c r="G3" s="10" t="n">
-        <v>125.87</v>
+        <v>159.89</v>
+      </c>
+      <c r="H3" s="10" t="n">
+        <v>179.05</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="10" t="inlineStr">
         <is>
-          <t>In isomer</t>
+          <t>Ag isomer</t>
         </is>
       </c>
       <c r="C4" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="10" t="n">
-        <v>0</v>
+        <v>20.26</v>
       </c>
       <c r="E4" s="10" t="n">
-        <v>0</v>
+        <v>35.63</v>
       </c>
       <c r="F4" s="10" t="n">
-        <v>19.16</v>
+        <v>191.71</v>
       </c>
       <c r="G4" s="10" t="n">
-        <v>159.89</v>
+        <v>117.38</v>
+      </c>
+      <c r="H4" s="10" t="n">
+        <v>364.98</v>
       </c>
     </row>
     <row r="5">
@@ -8464,23 +8479,26 @@
       </c>
       <c r="B5" s="10" t="inlineStr">
         <is>
-          <t>Ag</t>
+          <t>Cd</t>
         </is>
       </c>
       <c r="C5" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="10" t="n">
-        <v>0</v>
+        <v>8.210000000000001</v>
       </c>
       <c r="E5" s="10" t="n">
-        <v>0</v>
+        <v>39.69</v>
       </c>
       <c r="F5" s="10" t="n">
-        <v>0</v>
+        <v>138.45</v>
       </c>
       <c r="G5" s="10" t="n">
-        <v>0</v>
+        <v>232.28</v>
+      </c>
+      <c r="H5" s="10" t="n">
+        <v>418.63</v>
       </c>
     </row>
     <row r="6">
@@ -8489,23 +8507,26 @@
       </c>
       <c r="B6" s="10" t="inlineStr">
         <is>
-          <t>Ag isomer</t>
+          <t>In</t>
         </is>
       </c>
       <c r="C6" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D6" s="10" t="n">
-        <v>20.26</v>
+        <v>132.05</v>
       </c>
       <c r="E6" s="10" t="n">
-        <v>35.63</v>
+        <v>488.97</v>
       </c>
       <c r="F6" s="10" t="n">
-        <v>191.71</v>
+        <v>1725.77</v>
       </c>
       <c r="G6" s="10" t="n">
-        <v>117.38</v>
+        <v>3268.5</v>
+      </c>
+      <c r="H6" s="10" t="n">
+        <v>5615.29</v>
       </c>
     </row>
     <row r="7">
@@ -8514,73 +8535,82 @@
       </c>
       <c r="B7" s="10" t="inlineStr">
         <is>
-          <t>Cd</t>
+          <t>In isomer</t>
         </is>
       </c>
       <c r="C7" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D7" s="10" t="n">
-        <v>8.210000000000001</v>
+        <v>182.67</v>
       </c>
       <c r="E7" s="10" t="n">
-        <v>39.69</v>
+        <v>676.41</v>
       </c>
       <c r="F7" s="10" t="n">
-        <v>138.45</v>
+        <v>2387.32</v>
       </c>
       <c r="G7" s="10" t="n">
-        <v>232.28</v>
+        <v>4521.44</v>
+      </c>
+      <c r="H7" s="10" t="n">
+        <v>7767.84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" s="10" t="inlineStr">
         <is>
-          <t>In</t>
+          <t>Ag</t>
         </is>
       </c>
       <c r="C8" s="10" t="n">
-        <v>0</v>
+        <v>128.26</v>
       </c>
       <c r="D8" s="10" t="n">
-        <v>132.05</v>
+        <v>618.21</v>
       </c>
       <c r="E8" s="10" t="n">
-        <v>488.97</v>
+        <v>499.04</v>
       </c>
       <c r="F8" s="10" t="n">
-        <v>1725.77</v>
+        <v>157.9</v>
       </c>
       <c r="G8" s="10" t="n">
-        <v>3268.5</v>
+        <v>17.58</v>
+      </c>
+      <c r="H8" s="10" t="n">
+        <v>1420.99</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="n">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="10" t="inlineStr">
         <is>
-          <t>In isomer</t>
+          <t>Ag isomer</t>
         </is>
       </c>
       <c r="C9" s="10" t="n">
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="D9" s="10" t="n">
-        <v>182.67</v>
+        <v>2.61</v>
       </c>
       <c r="E9" s="10" t="n">
-        <v>676.41</v>
+        <v>2.11</v>
       </c>
       <c r="F9" s="10" t="n">
-        <v>2387.32</v>
+        <v>0.67</v>
       </c>
       <c r="G9" s="10" t="n">
-        <v>4521.44</v>
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="H9" s="10" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -8589,23 +8619,26 @@
       </c>
       <c r="B10" s="10" t="inlineStr">
         <is>
-          <t>Ag</t>
+          <t>In</t>
         </is>
       </c>
       <c r="C10" s="10" t="n">
-        <v>128.26</v>
+        <v>733.38</v>
       </c>
       <c r="D10" s="10" t="n">
-        <v>618.21</v>
+        <v>2113.45</v>
       </c>
       <c r="E10" s="10" t="n">
-        <v>499.04</v>
+        <v>3233.39</v>
       </c>
       <c r="F10" s="10" t="n">
-        <v>157.9</v>
+        <v>2890.18</v>
       </c>
       <c r="G10" s="10" t="n">
-        <v>17.58</v>
+        <v>617.78</v>
+      </c>
+      <c r="H10" s="10" t="n">
+        <v>9588.18</v>
       </c>
     </row>
     <row r="11">
@@ -8614,123 +8647,138 @@
       </c>
       <c r="B11" s="10" t="inlineStr">
         <is>
-          <t>Ag isomer</t>
+          <t>In isomer</t>
         </is>
       </c>
       <c r="C11" s="10" t="n">
-        <v>0.54</v>
+        <v>734.03</v>
       </c>
       <c r="D11" s="10" t="n">
-        <v>2.61</v>
+        <v>2115.32</v>
       </c>
       <c r="E11" s="10" t="n">
-        <v>2.11</v>
+        <v>3236.26</v>
       </c>
       <c r="F11" s="10" t="n">
-        <v>0.67</v>
+        <v>2892.75</v>
       </c>
       <c r="G11" s="10" t="n">
-        <v>0.07000000000000001</v>
+        <v>618.33</v>
+      </c>
+      <c r="H11" s="10" t="n">
+        <v>9596.690000000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="10" t="inlineStr">
         <is>
-          <t>Cd</t>
+          <t>Ag</t>
         </is>
       </c>
       <c r="C12" s="10" t="n">
-        <v>0</v>
+        <v>0.87</v>
       </c>
       <c r="D12" s="10" t="n">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="E12" s="10" t="n">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F12" s="10" t="n">
         <v>0</v>
       </c>
       <c r="G12" s="10" t="n">
-        <v>0</v>
+        <v>0.11</v>
+      </c>
+      <c r="H12" s="10" t="n">
+        <v>1.61</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="10" t="inlineStr">
         <is>
-          <t>In</t>
+          <t>Ag isomer</t>
         </is>
       </c>
       <c r="C13" s="10" t="n">
-        <v>733.38</v>
+        <v>1242.15</v>
       </c>
       <c r="D13" s="10" t="n">
-        <v>2113.45</v>
+        <v>728.34</v>
       </c>
       <c r="E13" s="10" t="n">
-        <v>3233.39</v>
+        <v>177.58</v>
       </c>
       <c r="F13" s="10" t="n">
-        <v>2890.18</v>
+        <v>0</v>
       </c>
       <c r="G13" s="10" t="n">
-        <v>617.78</v>
+        <v>159.55</v>
+      </c>
+      <c r="H13" s="10" t="n">
+        <v>2307.62</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="10" t="inlineStr">
         <is>
-          <t>In isomer</t>
+          <t>Cd</t>
         </is>
       </c>
       <c r="C14" s="10" t="n">
-        <v>734.03</v>
+        <v>3051.43</v>
       </c>
       <c r="D14" s="10" t="n">
-        <v>2115.32</v>
+        <v>1878.54</v>
       </c>
       <c r="E14" s="10" t="n">
-        <v>3236.26</v>
+        <v>366.17</v>
       </c>
       <c r="F14" s="10" t="n">
-        <v>2892.75</v>
+        <v>0</v>
       </c>
       <c r="G14" s="10" t="n">
-        <v>618.33</v>
+        <v>0</v>
+      </c>
+      <c r="H14" s="10" t="n">
+        <v>5296.139999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="n">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" s="10" t="inlineStr">
         <is>
-          <t>Pd</t>
+          <t>In</t>
         </is>
       </c>
       <c r="C15" s="10" t="n">
-        <v>0</v>
+        <v>1312.67</v>
       </c>
       <c r="D15" s="10" t="n">
-        <v>0</v>
+        <v>1095.7</v>
       </c>
       <c r="E15" s="10" t="n">
-        <v>0</v>
+        <v>285.68</v>
       </c>
       <c r="F15" s="10" t="n">
-        <v>0</v>
+        <v>44.12</v>
       </c>
       <c r="G15" s="10" t="n">
         <v>0</v>
+      </c>
+      <c r="H15" s="10" t="n">
+        <v>2738.17</v>
       </c>
     </row>
     <row r="16">
@@ -8739,211 +8787,235 @@
       </c>
       <c r="B16" s="10" t="inlineStr">
         <is>
-          <t>Ag</t>
+          <t>In isomer</t>
         </is>
       </c>
       <c r="C16" s="10" t="n">
-        <v>0.87</v>
+        <v>1313.03</v>
       </c>
       <c r="D16" s="10" t="n">
-        <v>0.51</v>
+        <v>1096</v>
       </c>
       <c r="E16" s="10" t="n">
-        <v>0.12</v>
+        <v>285.76</v>
       </c>
       <c r="F16" s="10" t="n">
+        <v>44.13</v>
+      </c>
+      <c r="G16" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="10" t="n">
-        <v>0.11</v>
+      <c r="H16" s="10" t="n">
+        <v>2738.92</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B17" s="10" t="inlineStr">
         <is>
-          <t>Ag isomer</t>
+          <t>Ag</t>
         </is>
       </c>
       <c r="C17" s="10" t="n">
-        <v>1242.15</v>
+        <v>170.73</v>
       </c>
       <c r="D17" s="10" t="n">
-        <v>728.34</v>
+        <v>156.02</v>
       </c>
       <c r="E17" s="10" t="n">
-        <v>177.58</v>
+        <v>410.07</v>
       </c>
       <c r="F17" s="10" t="n">
-        <v>0</v>
+        <v>704.14</v>
       </c>
       <c r="G17" s="10" t="n">
-        <v>159.55</v>
+        <v>641.24</v>
+      </c>
+      <c r="H17" s="10" t="n">
+        <v>2082.2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B18" s="10" t="inlineStr">
         <is>
-          <t>Cd</t>
+          <t>Ag isomer</t>
         </is>
       </c>
       <c r="C18" s="10" t="n">
-        <v>3051.43</v>
+        <v>268.74</v>
       </c>
       <c r="D18" s="10" t="n">
-        <v>1878.54</v>
+        <v>245.59</v>
       </c>
       <c r="E18" s="10" t="n">
-        <v>366.17</v>
+        <v>645.49</v>
       </c>
       <c r="F18" s="10" t="n">
-        <v>0</v>
+        <v>1108.38</v>
       </c>
       <c r="G18" s="10" t="n">
-        <v>0</v>
+        <v>1009.37</v>
+      </c>
+      <c r="H18" s="10" t="n">
+        <v>3277.57</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B19" s="10" t="inlineStr">
         <is>
-          <t>In</t>
+          <t>Cd</t>
         </is>
       </c>
       <c r="C19" s="10" t="n">
-        <v>1312.67</v>
+        <v>480.19</v>
       </c>
       <c r="D19" s="10" t="n">
-        <v>1095.7</v>
+        <v>0</v>
       </c>
       <c r="E19" s="10" t="n">
-        <v>285.68</v>
+        <v>0</v>
       </c>
       <c r="F19" s="10" t="n">
-        <v>44.12</v>
+        <v>0</v>
       </c>
       <c r="G19" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H19" s="10" t="n">
+        <v>480.19</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="n">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="10" t="inlineStr">
         <is>
-          <t>In isomer</t>
+          <t>In</t>
         </is>
       </c>
       <c r="C20" s="10" t="n">
-        <v>1313.03</v>
+        <v>88.98</v>
       </c>
       <c r="D20" s="10" t="n">
-        <v>1096</v>
+        <v>0</v>
       </c>
       <c r="E20" s="10" t="n">
-        <v>285.76</v>
+        <v>0</v>
       </c>
       <c r="F20" s="10" t="n">
-        <v>44.13</v>
+        <v>0</v>
       </c>
       <c r="G20" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H20" s="10" t="n">
+        <v>88.98</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="n">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B21" s="10" t="inlineStr">
         <is>
-          <t>Pd</t>
+          <t>Ag</t>
         </is>
       </c>
       <c r="C21" s="10" t="n">
-        <v>0</v>
+        <v>720.05</v>
       </c>
       <c r="D21" s="10" t="n">
-        <v>0</v>
+        <v>1340.01</v>
       </c>
       <c r="E21" s="10" t="n">
-        <v>0</v>
+        <v>1382.42</v>
       </c>
       <c r="F21" s="10" t="n">
-        <v>0</v>
+        <v>586.04</v>
       </c>
       <c r="G21" s="10" t="n">
-        <v>0</v>
+        <v>55.04</v>
+      </c>
+      <c r="H21" s="10" t="n">
+        <v>4083.56</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22" s="10" t="inlineStr">
         <is>
-          <t>Ag</t>
+          <t>Pd</t>
         </is>
       </c>
       <c r="C22" s="10" t="n">
-        <v>170.73</v>
+        <v>1.32</v>
       </c>
       <c r="D22" s="10" t="n">
-        <v>156.02</v>
+        <v>2.27</v>
       </c>
       <c r="E22" s="10" t="n">
-        <v>410.07</v>
+        <v>1.75</v>
       </c>
       <c r="F22" s="10" t="n">
-        <v>704.14</v>
+        <v>0.4</v>
       </c>
       <c r="G22" s="10" t="n">
-        <v>641.24</v>
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="H22" s="10" t="n">
+        <v>5.81</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" s="10" t="inlineStr">
         <is>
-          <t>Ag isomer</t>
+          <t>Rh isomer</t>
         </is>
       </c>
       <c r="C23" s="10" t="n">
-        <v>268.74</v>
+        <v>46.57</v>
       </c>
       <c r="D23" s="10" t="n">
-        <v>245.59</v>
+        <v>31.8</v>
       </c>
       <c r="E23" s="10" t="n">
-        <v>645.49</v>
+        <v>18.65</v>
       </c>
       <c r="F23" s="10" t="n">
-        <v>1108.38</v>
+        <v>0</v>
       </c>
       <c r="G23" s="10" t="n">
-        <v>1009.37</v>
+        <v>0</v>
+      </c>
+      <c r="H23" s="10" t="n">
+        <v>97.02000000000001</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="n">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24" s="10" t="inlineStr">
         <is>
-          <t>Cd</t>
+          <t>Ru</t>
         </is>
       </c>
       <c r="C24" s="10" t="n">
-        <v>480.19</v>
+        <v>0.02</v>
       </c>
       <c r="D24" s="10" t="n">
         <v>0</v>
@@ -8957,24 +9029,27 @@
       <c r="G24" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H24" s="10" t="n">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B25" s="10" t="inlineStr">
         <is>
-          <t>In</t>
+          <t>Ag</t>
         </is>
       </c>
       <c r="C25" s="10" t="n">
-        <v>88.98</v>
+        <v>2726.38</v>
       </c>
       <c r="D25" s="10" t="n">
-        <v>0</v>
+        <v>1479.54</v>
       </c>
       <c r="E25" s="10" t="n">
-        <v>0</v>
+        <v>187.55</v>
       </c>
       <c r="F25" s="10" t="n">
         <v>0</v>
@@ -8982,24 +9057,27 @@
       <c r="G25" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H25" s="10" t="n">
+        <v>4393.47</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="n">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B26" s="10" t="inlineStr">
         <is>
-          <t>Pd</t>
+          <t>Ag isomer</t>
         </is>
       </c>
       <c r="C26" s="10" t="n">
-        <v>0</v>
+        <v>2826.64</v>
       </c>
       <c r="D26" s="10" t="n">
-        <v>0</v>
+        <v>1533.95</v>
       </c>
       <c r="E26" s="10" t="n">
-        <v>0</v>
+        <v>194.44</v>
       </c>
       <c r="F26" s="10" t="n">
         <v>0</v>
@@ -9007,68 +9085,77 @@
       <c r="G26" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H26" s="10" t="n">
+        <v>4555.03</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="10" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B27" s="10" t="inlineStr">
         <is>
-          <t>Ag</t>
+          <t>Rh</t>
         </is>
       </c>
       <c r="C27" s="10" t="n">
-        <v>720.05</v>
+        <v>0.04</v>
       </c>
       <c r="D27" s="10" t="n">
-        <v>1340.01</v>
+        <v>0</v>
       </c>
       <c r="E27" s="10" t="n">
-        <v>1382.42</v>
+        <v>0</v>
       </c>
       <c r="F27" s="10" t="n">
-        <v>586.04</v>
+        <v>0</v>
       </c>
       <c r="G27" s="10" t="n">
-        <v>55.04</v>
+        <v>0</v>
+      </c>
+      <c r="H27" s="10" t="n">
+        <v>0.04</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="10" t="n">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="10" t="inlineStr">
         <is>
-          <t>Pd</t>
+          <t>Rh isomer</t>
         </is>
       </c>
       <c r="C28" s="10" t="n">
-        <v>1.32</v>
+        <v>0.01</v>
       </c>
       <c r="D28" s="10" t="n">
-        <v>2.27</v>
+        <v>0</v>
       </c>
       <c r="E28" s="10" t="n">
-        <v>1.75</v>
+        <v>0</v>
       </c>
       <c r="F28" s="10" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G28" s="10" t="n">
-        <v>0.07000000000000001</v>
+        <v>0</v>
+      </c>
+      <c r="H28" s="10" t="n">
+        <v>0.01</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="10" t="n">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B29" s="10" t="inlineStr">
         <is>
-          <t>Rh</t>
+          <t>Ag</t>
         </is>
       </c>
       <c r="C29" s="10" t="n">
-        <v>0</v>
+        <v>86.88</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>0</v>
@@ -9082,24 +9169,27 @@
       <c r="G29" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H29" s="10" t="n">
+        <v>86.88</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="10" t="n">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B30" s="10" t="inlineStr">
         <is>
-          <t>Rh isomer</t>
+          <t>Pd</t>
         </is>
       </c>
       <c r="C30" s="10" t="n">
-        <v>46.57</v>
+        <v>15.77</v>
       </c>
       <c r="D30" s="10" t="n">
-        <v>31.8</v>
+        <v>0</v>
       </c>
       <c r="E30" s="10" t="n">
-        <v>18.65</v>
+        <v>0</v>
       </c>
       <c r="F30" s="10" t="n">
         <v>0</v>
@@ -9107,99 +9197,111 @@
       <c r="G30" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H30" s="10" t="n">
+        <v>15.77</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="10" t="n">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B31" s="10" t="inlineStr">
         <is>
-          <t>Ru</t>
+          <t>Rh isomer</t>
         </is>
       </c>
       <c r="C31" s="10" t="n">
-        <v>0.02</v>
+        <v>0.15</v>
       </c>
       <c r="D31" s="10" t="n">
-        <v>0</v>
+        <v>0.54</v>
       </c>
       <c r="E31" s="10" t="n">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="F31" s="10" t="n">
-        <v>0</v>
+        <v>1.27</v>
       </c>
       <c r="G31" s="10" t="n">
-        <v>0</v>
+        <v>0.28</v>
+      </c>
+      <c r="H31" s="10" t="n">
+        <v>3.54</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="10" t="n">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B32" s="10" t="inlineStr">
         <is>
-          <t>Ag</t>
+          <t>Rh</t>
         </is>
       </c>
       <c r="C32" s="10" t="n">
-        <v>2726.38</v>
+        <v>19.96</v>
       </c>
       <c r="D32" s="10" t="n">
-        <v>1479.54</v>
+        <v>24.95</v>
       </c>
       <c r="E32" s="10" t="n">
-        <v>187.55</v>
+        <v>12.44</v>
       </c>
       <c r="F32" s="10" t="n">
-        <v>0</v>
+        <v>2.93</v>
       </c>
       <c r="G32" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H32" s="10" t="n">
+        <v>60.27999999999999</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="10" t="n">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B33" s="10" t="inlineStr">
         <is>
-          <t>Ag isomer</t>
+          <t>Rh isomer</t>
         </is>
       </c>
       <c r="C33" s="10" t="n">
-        <v>2826.64</v>
+        <v>600.38</v>
       </c>
       <c r="D33" s="10" t="n">
-        <v>1533.95</v>
+        <v>750.47</v>
       </c>
       <c r="E33" s="10" t="n">
-        <v>194.44</v>
+        <v>374.33</v>
       </c>
       <c r="F33" s="10" t="n">
-        <v>0</v>
+        <v>88.25</v>
       </c>
       <c r="G33" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H33" s="10" t="n">
+        <v>1813.43</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="10" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B34" s="10" t="inlineStr">
         <is>
-          <t>Pd</t>
+          <t>Rh</t>
         </is>
       </c>
       <c r="C34" s="10" t="n">
-        <v>0</v>
+        <v>1.71</v>
       </c>
       <c r="D34" s="10" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E34" s="10" t="n">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="F34" s="10" t="n">
         <v>0</v>
@@ -9207,24 +9309,27 @@
       <c r="G34" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H34" s="10" t="n">
+        <v>2.14</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="10" t="n">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B35" s="10" t="inlineStr">
         <is>
-          <t>Rh</t>
+          <t>Rh isomer</t>
         </is>
       </c>
       <c r="C35" s="10" t="n">
-        <v>0.04</v>
+        <v>131.16</v>
       </c>
       <c r="D35" s="10" t="n">
-        <v>0</v>
+        <v>30.5</v>
       </c>
       <c r="E35" s="10" t="n">
-        <v>0</v>
+        <v>2.44</v>
       </c>
       <c r="F35" s="10" t="n">
         <v>0</v>
@@ -9232,18 +9337,21 @@
       <c r="G35" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H35" s="10" t="n">
+        <v>164.1</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="10" t="n">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B36" s="10" t="inlineStr">
         <is>
-          <t>Rh isomer</t>
+          <t>Rh</t>
         </is>
       </c>
       <c r="C36" s="10" t="n">
-        <v>0.01</v>
+        <v>22.06</v>
       </c>
       <c r="D36" s="10" t="n">
         <v>0</v>
@@ -9257,18 +9365,21 @@
       <c r="G36" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H36" s="10" t="n">
+        <v>22.06</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="10" t="n">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B37" s="10" t="inlineStr">
         <is>
-          <t>Ag</t>
+          <t>Rh isomer</t>
         </is>
       </c>
       <c r="C37" s="10" t="n">
-        <v>86.88</v>
+        <v>22.25</v>
       </c>
       <c r="D37" s="10" t="n">
         <v>0</v>
@@ -9282,21 +9393,24 @@
       <c r="G37" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H37" s="10" t="n">
+        <v>22.25</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="10" t="n">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B38" s="10" t="inlineStr">
         <is>
-          <t>Pd</t>
+          <t>Tc isomer</t>
         </is>
       </c>
       <c r="C38" s="10" t="n">
-        <v>15.77</v>
+        <v>0.01</v>
       </c>
       <c r="D38" s="10" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="E38" s="10" t="n">
         <v>0</v>
@@ -9307,18 +9421,21 @@
       <c r="G38" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H38" s="10" t="n">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="10" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B39" s="10" t="inlineStr">
         <is>
-          <t>Rh</t>
+          <t>Tc</t>
         </is>
       </c>
       <c r="C39" s="10" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="D39" s="10" t="n">
         <v>0</v>
@@ -9332,46 +9449,52 @@
       <c r="G39" s="10" t="n">
         <v>0</v>
       </c>
+      <c r="H39" s="10" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="10" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B40" s="10" t="inlineStr">
         <is>
-          <t>Rh isomer</t>
+          <t>Tc isomer</t>
         </is>
       </c>
       <c r="C40" s="10" t="n">
-        <v>0.15</v>
+        <v>24.65</v>
       </c>
       <c r="D40" s="10" t="n">
-        <v>0.54</v>
+        <v>0</v>
       </c>
       <c r="E40" s="10" t="n">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="F40" s="10" t="n">
-        <v>1.27</v>
+        <v>0</v>
       </c>
       <c r="G40" s="10" t="n">
-        <v>0.28</v>
+        <v>0</v>
+      </c>
+      <c r="H40" s="10" t="n">
+        <v>24.65</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="10" t="n">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B41" s="10" t="inlineStr">
         <is>
-          <t>Ru</t>
+          <t>Nb isomer</t>
         </is>
       </c>
       <c r="C41" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D41" s="10" t="n">
-        <v>0</v>
+        <v>20.23</v>
       </c>
       <c r="E41" s="10" t="n">
         <v>0</v>
@@ -9382,424 +9505,8 @@
       <c r="G41" s="10" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="B42" s="10" t="inlineStr">
-        <is>
-          <t>Rh</t>
-        </is>
-      </c>
-      <c r="C42" s="10" t="n">
-        <v>19.96</v>
-      </c>
-      <c r="D42" s="10" t="n">
-        <v>24.95</v>
-      </c>
-      <c r="E42" s="10" t="n">
-        <v>12.44</v>
-      </c>
-      <c r="F42" s="10" t="n">
-        <v>2.93</v>
-      </c>
-      <c r="G42" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="B43" s="10" t="inlineStr">
-        <is>
-          <t>Rh isomer</t>
-        </is>
-      </c>
-      <c r="C43" s="10" t="n">
-        <v>600.38</v>
-      </c>
-      <c r="D43" s="10" t="n">
-        <v>750.47</v>
-      </c>
-      <c r="E43" s="10" t="n">
-        <v>374.33</v>
-      </c>
-      <c r="F43" s="10" t="n">
-        <v>88.25</v>
-      </c>
-      <c r="G43" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="B44" s="10" t="inlineStr">
-        <is>
-          <t>Ru</t>
-        </is>
-      </c>
-      <c r="C44" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="10" t="n">
-        <v>99</v>
-      </c>
-      <c r="B45" s="10" t="inlineStr">
-        <is>
-          <t>Rh</t>
-        </is>
-      </c>
-      <c r="C45" s="10" t="n">
-        <v>1.71</v>
-      </c>
-      <c r="D45" s="10" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="E45" s="10" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="F45" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="10" t="n">
-        <v>99</v>
-      </c>
-      <c r="B46" s="10" t="inlineStr">
-        <is>
-          <t>Rh isomer</t>
-        </is>
-      </c>
-      <c r="C46" s="10" t="n">
-        <v>131.16</v>
-      </c>
-      <c r="D46" s="10" t="n">
-        <v>30.5</v>
-      </c>
-      <c r="E46" s="10" t="n">
-        <v>2.44</v>
-      </c>
-      <c r="F46" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="10" t="n">
-        <v>99</v>
-      </c>
-      <c r="B47" s="10" t="inlineStr">
-        <is>
-          <t>Ru</t>
-        </is>
-      </c>
-      <c r="C47" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G47" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="10" t="n">
-        <v>98</v>
-      </c>
-      <c r="B48" s="10" t="inlineStr">
-        <is>
-          <t>Rh</t>
-        </is>
-      </c>
-      <c r="C48" s="10" t="n">
-        <v>22.06</v>
-      </c>
-      <c r="D48" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="10" t="n">
-        <v>98</v>
-      </c>
-      <c r="B49" s="10" t="inlineStr">
-        <is>
-          <t>Rh isomer</t>
-        </is>
-      </c>
-      <c r="C49" s="10" t="n">
-        <v>22.25</v>
-      </c>
-      <c r="D49" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G49" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="10" t="n">
-        <v>98</v>
-      </c>
-      <c r="B50" s="10" t="inlineStr">
-        <is>
-          <t>Ru</t>
-        </is>
-      </c>
-      <c r="C50" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G50" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="10" t="n">
-        <v>98</v>
-      </c>
-      <c r="B51" s="10" t="inlineStr">
-        <is>
-          <t>Tc</t>
-        </is>
-      </c>
-      <c r="C51" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G51" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="10" t="n">
-        <v>97</v>
-      </c>
-      <c r="B52" s="10" t="inlineStr">
-        <is>
-          <t>Tc</t>
-        </is>
-      </c>
-      <c r="C52" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D52" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="10" t="n">
-        <v>97</v>
-      </c>
-      <c r="B53" s="10" t="inlineStr">
-        <is>
-          <t>Tc isomer</t>
-        </is>
-      </c>
-      <c r="C53" s="10" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="D53" s="10" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="E53" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G53" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="10" t="n">
-        <v>96</v>
-      </c>
-      <c r="B54" s="10" t="inlineStr">
-        <is>
-          <t>Tc</t>
-        </is>
-      </c>
-      <c r="C54" s="10" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="D54" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="10" t="n">
-        <v>96</v>
-      </c>
-      <c r="B55" s="10" t="inlineStr">
-        <is>
-          <t>Tc isomer</t>
-        </is>
-      </c>
-      <c r="C55" s="10" t="n">
-        <v>24.65</v>
-      </c>
-      <c r="D55" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="10" t="n">
-        <v>94</v>
-      </c>
-      <c r="B56" s="10" t="inlineStr">
-        <is>
-          <t>Nb</t>
-        </is>
-      </c>
-      <c r="C56" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D56" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="10" t="n">
-        <v>94</v>
-      </c>
-      <c r="B57" s="10" t="inlineStr">
-        <is>
-          <t>Nb isomer</t>
-        </is>
-      </c>
-      <c r="C57" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" s="10" t="n">
+      <c r="H41" s="10" t="n">
         <v>20.23</v>
-      </c>
-      <c r="E57" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F57" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G57" s="10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="10" t="inlineStr"/>
-      <c r="B58" s="10" t="inlineStr"/>
-      <c r="C58" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D58" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E58" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F58" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" s="10" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add A(Bq) Calculation after beam stop with different cd time
</commit_message>
<xml_diff>
--- a/example/DoesCal.xlsx
+++ b/example/DoesCal.xlsx
@@ -12,7 +12,7 @@
     <sheet name="6um_362MeV" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="3um_391MeV" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="12um_303MeV" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Summary_A" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Summary_Act" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
@@ -8329,7 +8329,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8345,6 +8345,11 @@
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="14" customWidth="1" min="7" max="7"/>
     <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="10" max="10"/>
+    <col width="14" customWidth="1" min="11" max="11"/>
+    <col width="14" customWidth="1" min="12" max="12"/>
+    <col width="14" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -8360,32 +8365,57 @@
       </c>
       <c r="C1" s="9" t="inlineStr">
         <is>
+          <t>t1/2</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
+        <is>
           <t>A(Bq)@0um</t>
         </is>
       </c>
-      <c r="D1" s="9" t="inlineStr">
+      <c r="F1" s="9" t="inlineStr">
         <is>
           <t>A(Bq)@3um</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="G1" s="9" t="inlineStr">
         <is>
           <t>A(Bq)@6um</t>
         </is>
       </c>
-      <c r="F1" s="9" t="inlineStr">
+      <c r="H1" s="9" t="inlineStr">
         <is>
           <t>A(Bq)@9um</t>
         </is>
       </c>
-      <c r="G1" s="9" t="inlineStr">
+      <c r="I1" s="9" t="inlineStr">
         <is>
           <t>A(Bq)@12um</t>
         </is>
       </c>
-      <c r="H1" s="9" t="inlineStr">
+      <c r="J1" s="9" t="inlineStr">
         <is>
           <t>A(Bq)@cd = 0s</t>
+        </is>
+      </c>
+      <c r="K1" s="9" t="inlineStr">
+        <is>
+          <t>A(Bq)@t=15 m</t>
+        </is>
+      </c>
+      <c r="L1" s="9" t="inlineStr">
+        <is>
+          <t>A(Bq)@t=1 hour</t>
+        </is>
+      </c>
+      <c r="M1" s="9" t="inlineStr">
+        <is>
+          <t>A(Bq)@t=1 day</t>
         </is>
       </c>
     </row>
@@ -8399,22 +8429,39 @@
         </is>
       </c>
       <c r="C2" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="10" t="n">
-        <v>0</v>
+        <v>58</v>
+      </c>
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
       </c>
       <c r="E2" s="10" t="n">
         <v>0</v>
       </c>
       <c r="F2" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="10" t="n">
         <v>15.09</v>
       </c>
-      <c r="G2" s="10" t="n">
+      <c r="I2" s="10" t="n">
         <v>125.87</v>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="J2" s="10" t="n">
         <v>140.96</v>
+      </c>
+      <c r="K2" s="10" t="n">
+        <v>117.83</v>
+      </c>
+      <c r="L2" s="10" t="n">
+        <v>68.83</v>
+      </c>
+      <c r="M2" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -8427,22 +8474,39 @@
         </is>
       </c>
       <c r="C3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="10" t="n">
-        <v>0</v>
+        <v>39.6</v>
+      </c>
+      <c r="D3" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
       </c>
       <c r="E3" s="10" t="n">
         <v>0</v>
       </c>
       <c r="F3" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="10" t="n">
         <v>19.16</v>
       </c>
-      <c r="G3" s="10" t="n">
+      <c r="I3" s="10" t="n">
         <v>159.89</v>
       </c>
-      <c r="H3" s="10" t="n">
+      <c r="J3" s="10" t="n">
         <v>179.05</v>
+      </c>
+      <c r="K3" s="10" t="n">
+        <v>137.71</v>
+      </c>
+      <c r="L3" s="10" t="n">
+        <v>62.66</v>
+      </c>
+      <c r="M3" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -8455,22 +8519,39 @@
         </is>
       </c>
       <c r="C4" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="10" t="n">
+        <v>44.3</v>
+      </c>
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10" t="n">
         <v>20.26</v>
       </c>
-      <c r="E4" s="10" t="n">
+      <c r="G4" s="10" t="n">
         <v>35.63</v>
       </c>
-      <c r="F4" s="10" t="n">
+      <c r="H4" s="10" t="n">
         <v>191.71</v>
       </c>
-      <c r="G4" s="10" t="n">
+      <c r="I4" s="10" t="n">
         <v>117.38</v>
       </c>
-      <c r="H4" s="10" t="n">
+      <c r="J4" s="10" t="n">
         <v>364.98</v>
+      </c>
+      <c r="K4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -8483,22 +8564,39 @@
         </is>
       </c>
       <c r="C5" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="10" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="D5" s="10" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E5" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="10" t="n">
         <v>8.210000000000001</v>
       </c>
-      <c r="E5" s="10" t="n">
+      <c r="G5" s="10" t="n">
         <v>39.69</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="H5" s="10" t="n">
         <v>138.45</v>
       </c>
-      <c r="G5" s="10" t="n">
+      <c r="I5" s="10" t="n">
         <v>232.28</v>
       </c>
-      <c r="H5" s="10" t="n">
+      <c r="J5" s="10" t="n">
         <v>418.63</v>
+      </c>
+      <c r="K5" s="10" t="n">
+        <v>407.62</v>
+      </c>
+      <c r="L5" s="10" t="n">
+        <v>376.29</v>
+      </c>
+      <c r="M5" s="10" t="n">
+        <v>32.4</v>
       </c>
     </row>
     <row r="6">
@@ -8511,22 +8609,39 @@
         </is>
       </c>
       <c r="C6" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="10" t="n">
+        <v>32.4</v>
+      </c>
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="n">
         <v>132.05</v>
       </c>
-      <c r="E6" s="10" t="n">
+      <c r="G6" s="10" t="n">
         <v>488.97</v>
       </c>
-      <c r="F6" s="10" t="n">
+      <c r="H6" s="10" t="n">
         <v>1725.77</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="I6" s="10" t="n">
         <v>3268.5</v>
       </c>
-      <c r="H6" s="10" t="n">
+      <c r="J6" s="10" t="n">
         <v>5615.29</v>
+      </c>
+      <c r="K6" s="10" t="n">
+        <v>4074.14</v>
+      </c>
+      <c r="L6" s="10" t="n">
+        <v>1556.06</v>
+      </c>
+      <c r="M6" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -8539,22 +8654,39 @@
         </is>
       </c>
       <c r="C7" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="10" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="D7" s="10" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E7" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10" t="n">
         <v>182.67</v>
       </c>
-      <c r="E7" s="10" t="n">
+      <c r="G7" s="10" t="n">
         <v>676.41</v>
       </c>
-      <c r="F7" s="10" t="n">
+      <c r="H7" s="10" t="n">
         <v>2387.32</v>
       </c>
-      <c r="G7" s="10" t="n">
+      <c r="I7" s="10" t="n">
         <v>4521.44</v>
       </c>
-      <c r="H7" s="10" t="n">
+      <c r="J7" s="10" t="n">
         <v>7767.84</v>
+      </c>
+      <c r="K7" s="10" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="L7" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -8567,22 +8699,39 @@
         </is>
       </c>
       <c r="C8" s="10" t="n">
+        <v>23.96</v>
+      </c>
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="n">
         <v>128.26</v>
       </c>
-      <c r="D8" s="10" t="n">
+      <c r="F8" s="10" t="n">
         <v>618.21</v>
       </c>
-      <c r="E8" s="10" t="n">
+      <c r="G8" s="10" t="n">
         <v>499.04</v>
       </c>
-      <c r="F8" s="10" t="n">
+      <c r="H8" s="10" t="n">
         <v>157.9</v>
       </c>
-      <c r="G8" s="10" t="n">
+      <c r="I8" s="10" t="n">
         <v>17.58</v>
       </c>
-      <c r="H8" s="10" t="n">
+      <c r="J8" s="10" t="n">
         <v>1420.99</v>
+      </c>
+      <c r="K8" s="10" t="n">
+        <v>920.8200000000001</v>
+      </c>
+      <c r="L8" s="10" t="n">
+        <v>250.56</v>
+      </c>
+      <c r="M8" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -8595,22 +8744,39 @@
         </is>
       </c>
       <c r="C9" s="10" t="n">
+        <v>8.279999999999999</v>
+      </c>
+      <c r="D9" s="10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E9" s="10" t="n">
         <v>0.54</v>
       </c>
-      <c r="D9" s="10" t="n">
+      <c r="F9" s="10" t="n">
         <v>2.61</v>
       </c>
-      <c r="E9" s="10" t="n">
+      <c r="G9" s="10" t="n">
         <v>2.11</v>
       </c>
-      <c r="F9" s="10" t="n">
+      <c r="H9" s="10" t="n">
         <v>0.67</v>
       </c>
-      <c r="G9" s="10" t="n">
+      <c r="I9" s="10" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="H9" s="10" t="n">
+      <c r="J9" s="10" t="n">
         <v>6</v>
+      </c>
+      <c r="K9" s="10" t="n">
+        <v>5.99</v>
+      </c>
+      <c r="L9" s="10" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="M9" s="10" t="n">
+        <v>5.52</v>
       </c>
     </row>
     <row r="10">
@@ -8623,22 +8789,39 @@
         </is>
       </c>
       <c r="C10" s="10" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D10" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E10" s="10" t="n">
         <v>733.38</v>
       </c>
-      <c r="D10" s="10" t="n">
+      <c r="F10" s="10" t="n">
         <v>2113.45</v>
       </c>
-      <c r="E10" s="10" t="n">
+      <c r="G10" s="10" t="n">
         <v>3233.39</v>
       </c>
-      <c r="F10" s="10" t="n">
+      <c r="H10" s="10" t="n">
         <v>2890.18</v>
       </c>
-      <c r="G10" s="10" t="n">
+      <c r="I10" s="10" t="n">
         <v>617.78</v>
       </c>
-      <c r="H10" s="10" t="n">
+      <c r="J10" s="10" t="n">
         <v>9588.18</v>
+      </c>
+      <c r="K10" s="10" t="n">
+        <v>1793.05</v>
+      </c>
+      <c r="L10" s="10" t="n">
+        <v>11.73</v>
+      </c>
+      <c r="M10" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -8651,22 +8834,39 @@
         </is>
       </c>
       <c r="C11" s="10" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="D11" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E11" s="10" t="n">
         <v>734.03</v>
       </c>
-      <c r="D11" s="10" t="n">
+      <c r="F11" s="10" t="n">
         <v>2115.32</v>
       </c>
-      <c r="E11" s="10" t="n">
+      <c r="G11" s="10" t="n">
         <v>3236.26</v>
       </c>
-      <c r="F11" s="10" t="n">
+      <c r="H11" s="10" t="n">
         <v>2892.75</v>
       </c>
-      <c r="G11" s="10" t="n">
+      <c r="I11" s="10" t="n">
         <v>618.33</v>
       </c>
-      <c r="H11" s="10" t="n">
+      <c r="J11" s="10" t="n">
         <v>9596.690000000001</v>
+      </c>
+      <c r="K11" s="10" t="n">
+        <v>1300.02</v>
+      </c>
+      <c r="L11" s="10" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="M11" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -8679,22 +8879,39 @@
         </is>
       </c>
       <c r="C12" s="10" t="n">
+        <v>41.29</v>
+      </c>
+      <c r="D12" s="10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E12" s="10" t="n">
         <v>0.87</v>
       </c>
-      <c r="D12" s="10" t="n">
+      <c r="F12" s="10" t="n">
         <v>0.51</v>
       </c>
-      <c r="E12" s="10" t="n">
+      <c r="G12" s="10" t="n">
         <v>0.12</v>
       </c>
-      <c r="F12" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="10" t="n">
+      <c r="H12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="10" t="n">
         <v>0.11</v>
       </c>
-      <c r="H12" s="10" t="n">
+      <c r="J12" s="10" t="n">
         <v>1.61</v>
+      </c>
+      <c r="K12" s="10" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="L12" s="10" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="M12" s="10" t="n">
+        <v>1.58</v>
       </c>
     </row>
     <row r="13">
@@ -8707,22 +8924,39 @@
         </is>
       </c>
       <c r="C13" s="10" t="n">
+        <v>7.23</v>
+      </c>
+      <c r="D13" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E13" s="10" t="n">
         <v>1242.15</v>
       </c>
-      <c r="D13" s="10" t="n">
+      <c r="F13" s="10" t="n">
         <v>728.34</v>
       </c>
-      <c r="E13" s="10" t="n">
+      <c r="G13" s="10" t="n">
         <v>177.58</v>
       </c>
-      <c r="F13" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="10" t="n">
+      <c r="H13" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10" t="n">
         <v>159.55</v>
       </c>
-      <c r="H13" s="10" t="n">
+      <c r="J13" s="10" t="n">
         <v>2307.62</v>
+      </c>
+      <c r="K13" s="10" t="n">
+        <v>547.97</v>
+      </c>
+      <c r="L13" s="10" t="n">
+        <v>7.34</v>
+      </c>
+      <c r="M13" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -8735,22 +8969,39 @@
         </is>
       </c>
       <c r="C14" s="10" t="n">
+        <v>55.5</v>
+      </c>
+      <c r="D14" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E14" s="10" t="n">
         <v>3051.43</v>
       </c>
-      <c r="D14" s="10" t="n">
+      <c r="F14" s="10" t="n">
         <v>1878.54</v>
       </c>
-      <c r="E14" s="10" t="n">
+      <c r="G14" s="10" t="n">
         <v>366.17</v>
       </c>
-      <c r="F14" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="H14" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10" t="n">
         <v>5296.139999999999</v>
+      </c>
+      <c r="K14" s="10" t="n">
+        <v>4391.54</v>
+      </c>
+      <c r="L14" s="10" t="n">
+        <v>2503.75</v>
+      </c>
+      <c r="M14" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -8763,22 +9014,39 @@
         </is>
       </c>
       <c r="C15" s="10" t="n">
+        <v>5.07</v>
+      </c>
+      <c r="D15" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E15" s="10" t="n">
         <v>1312.67</v>
       </c>
-      <c r="D15" s="10" t="n">
+      <c r="F15" s="10" t="n">
         <v>1095.7</v>
       </c>
-      <c r="E15" s="10" t="n">
+      <c r="G15" s="10" t="n">
         <v>285.68</v>
       </c>
-      <c r="F15" s="10" t="n">
+      <c r="H15" s="10" t="n">
         <v>44.12</v>
       </c>
-      <c r="G15" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="10" t="n">
+      <c r="I15" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="10" t="n">
         <v>2738.17</v>
+      </c>
+      <c r="K15" s="10" t="n">
+        <v>352.39</v>
+      </c>
+      <c r="L15" s="10" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="M15" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -8791,22 +9059,39 @@
         </is>
       </c>
       <c r="C16" s="10" t="n">
+        <v>48</v>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E16" s="10" t="n">
         <v>1313.03</v>
       </c>
-      <c r="D16" s="10" t="n">
+      <c r="F16" s="10" t="n">
         <v>1096</v>
       </c>
-      <c r="E16" s="10" t="n">
+      <c r="G16" s="10" t="n">
         <v>285.76</v>
       </c>
-      <c r="F16" s="10" t="n">
+      <c r="H16" s="10" t="n">
         <v>44.13</v>
       </c>
-      <c r="G16" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="10" t="n">
+      <c r="I16" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="10" t="n">
         <v>2738.92</v>
+      </c>
+      <c r="K16" s="10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L16" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -8819,22 +9104,39 @@
         </is>
       </c>
       <c r="C17" s="10" t="n">
+        <v>69.2</v>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E17" s="10" t="n">
         <v>170.73</v>
       </c>
-      <c r="D17" s="10" t="n">
+      <c r="F17" s="10" t="n">
         <v>156.02</v>
       </c>
-      <c r="E17" s="10" t="n">
+      <c r="G17" s="10" t="n">
         <v>410.07</v>
       </c>
-      <c r="F17" s="10" t="n">
+      <c r="H17" s="10" t="n">
         <v>704.14</v>
       </c>
-      <c r="G17" s="10" t="n">
+      <c r="I17" s="10" t="n">
         <v>641.24</v>
       </c>
-      <c r="H17" s="10" t="n">
+      <c r="J17" s="10" t="n">
         <v>2082.2</v>
+      </c>
+      <c r="K17" s="10" t="n">
+        <v>1791.78</v>
+      </c>
+      <c r="L17" s="10" t="n">
+        <v>1141.75</v>
+      </c>
+      <c r="M17" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -8847,22 +9149,39 @@
         </is>
       </c>
       <c r="C18" s="10" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="D18" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E18" s="10" t="n">
         <v>268.74</v>
       </c>
-      <c r="D18" s="10" t="n">
+      <c r="F18" s="10" t="n">
         <v>245.59</v>
       </c>
-      <c r="E18" s="10" t="n">
+      <c r="G18" s="10" t="n">
         <v>645.49</v>
       </c>
-      <c r="F18" s="10" t="n">
+      <c r="H18" s="10" t="n">
         <v>1108.38</v>
       </c>
-      <c r="G18" s="10" t="n">
+      <c r="I18" s="10" t="n">
         <v>1009.37</v>
       </c>
-      <c r="H18" s="10" t="n">
+      <c r="J18" s="10" t="n">
         <v>3277.57</v>
+      </c>
+      <c r="K18" s="10" t="n">
+        <v>2403.21</v>
+      </c>
+      <c r="L18" s="10" t="n">
+        <v>947.35</v>
+      </c>
+      <c r="M18" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -8875,14 +9194,16 @@
         </is>
       </c>
       <c r="C19" s="10" t="n">
+        <v>57.7</v>
+      </c>
+      <c r="D19" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E19" s="10" t="n">
         <v>480.19</v>
       </c>
-      <c r="D19" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="F19" s="10" t="n">
         <v>0</v>
       </c>
@@ -8890,7 +9211,22 @@
         <v>0</v>
       </c>
       <c r="H19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="10" t="n">
         <v>480.19</v>
+      </c>
+      <c r="K19" s="10" t="n">
+        <v>401.03</v>
+      </c>
+      <c r="L19" s="10" t="n">
+        <v>233.59</v>
+      </c>
+      <c r="M19" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -8903,14 +9239,16 @@
         </is>
       </c>
       <c r="C20" s="10" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="D20" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E20" s="10" t="n">
         <v>88.98</v>
       </c>
-      <c r="D20" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="F20" s="10" t="n">
         <v>0</v>
       </c>
@@ -8918,7 +9256,22 @@
         <v>0</v>
       </c>
       <c r="H20" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="10" t="n">
         <v>88.98</v>
+      </c>
+      <c r="K20" s="10" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="L20" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -8931,22 +9284,39 @@
         </is>
       </c>
       <c r="C21" s="10" t="n">
+        <v>65.7</v>
+      </c>
+      <c r="D21" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E21" s="10" t="n">
         <v>720.05</v>
       </c>
-      <c r="D21" s="10" t="n">
+      <c r="F21" s="10" t="n">
         <v>1340.01</v>
       </c>
-      <c r="E21" s="10" t="n">
+      <c r="G21" s="10" t="n">
         <v>1382.42</v>
       </c>
-      <c r="F21" s="10" t="n">
+      <c r="H21" s="10" t="n">
         <v>586.04</v>
       </c>
-      <c r="G21" s="10" t="n">
+      <c r="I21" s="10" t="n">
         <v>55.04</v>
       </c>
-      <c r="H21" s="10" t="n">
+      <c r="J21" s="10" t="n">
         <v>4083.56</v>
+      </c>
+      <c r="K21" s="10" t="n">
+        <v>3485.98</v>
+      </c>
+      <c r="L21" s="10" t="n">
+        <v>2168.62</v>
+      </c>
+      <c r="M21" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -8959,22 +9329,39 @@
         </is>
       </c>
       <c r="C22" s="10" t="n">
+        <v>16.991</v>
+      </c>
+      <c r="D22" s="10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E22" s="10" t="n">
         <v>1.32</v>
       </c>
-      <c r="D22" s="10" t="n">
+      <c r="F22" s="10" t="n">
         <v>2.27</v>
       </c>
-      <c r="E22" s="10" t="n">
+      <c r="G22" s="10" t="n">
         <v>1.75</v>
       </c>
-      <c r="F22" s="10" t="n">
+      <c r="H22" s="10" t="n">
         <v>0.4</v>
       </c>
-      <c r="G22" s="10" t="n">
+      <c r="I22" s="10" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="H22" s="10" t="n">
+      <c r="J22" s="10" t="n">
         <v>5.81</v>
+      </c>
+      <c r="K22" s="10" t="n">
+        <v>5.81</v>
+      </c>
+      <c r="L22" s="10" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="M22" s="10" t="n">
+        <v>5.58</v>
       </c>
     </row>
     <row r="23">
@@ -8987,22 +9374,39 @@
         </is>
       </c>
       <c r="C23" s="10" t="n">
+        <v>56.114</v>
+      </c>
+      <c r="D23" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E23" s="10" t="n">
         <v>46.57</v>
       </c>
-      <c r="D23" s="10" t="n">
+      <c r="F23" s="10" t="n">
         <v>31.8</v>
       </c>
-      <c r="E23" s="10" t="n">
+      <c r="G23" s="10" t="n">
         <v>18.65</v>
       </c>
-      <c r="F23" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="H23" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="10" t="n">
         <v>97.02000000000001</v>
+      </c>
+      <c r="K23" s="10" t="n">
+        <v>80.61</v>
+      </c>
+      <c r="L23" s="10" t="n">
+        <v>46.24</v>
+      </c>
+      <c r="M23" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -9015,14 +9419,16 @@
         </is>
       </c>
       <c r="C24" s="10" t="n">
+        <v>39.247</v>
+      </c>
+      <c r="D24" s="10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E24" s="10" t="n">
         <v>0.02</v>
       </c>
-      <c r="D24" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="F24" s="10" t="n">
         <v>0</v>
       </c>
@@ -9030,6 +9436,21 @@
         <v>0</v>
       </c>
       <c r="H24" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="10" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="K24" s="10" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="L24" s="10" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="M24" s="10" t="n">
         <v>0.02</v>
       </c>
     </row>
@@ -9043,22 +9464,39 @@
         </is>
       </c>
       <c r="C25" s="10" t="n">
+        <v>12.9</v>
+      </c>
+      <c r="D25" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E25" s="10" t="n">
         <v>2726.38</v>
       </c>
-      <c r="D25" s="10" t="n">
+      <c r="F25" s="10" t="n">
         <v>1479.54</v>
       </c>
-      <c r="E25" s="10" t="n">
+      <c r="G25" s="10" t="n">
         <v>187.55</v>
       </c>
-      <c r="F25" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="H25" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="10" t="n">
         <v>4393.47</v>
+      </c>
+      <c r="K25" s="10" t="n">
+        <v>1962.67</v>
+      </c>
+      <c r="L25" s="10" t="n">
+        <v>174.97</v>
+      </c>
+      <c r="M25" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -9071,22 +9509,39 @@
         </is>
       </c>
       <c r="C26" s="10" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="D26" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E26" s="10" t="n">
         <v>2826.64</v>
       </c>
-      <c r="D26" s="10" t="n">
+      <c r="F26" s="10" t="n">
         <v>1533.95</v>
       </c>
-      <c r="E26" s="10" t="n">
+      <c r="G26" s="10" t="n">
         <v>194.44</v>
       </c>
-      <c r="F26" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="H26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="10" t="n">
         <v>4555.03</v>
+      </c>
+      <c r="K26" s="10" t="n">
+        <v>1180.85</v>
+      </c>
+      <c r="L26" s="10" t="n">
+        <v>20.57</v>
+      </c>
+      <c r="M26" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -9099,14 +9554,16 @@
         </is>
       </c>
       <c r="C27" s="10" t="n">
+        <v>207.3</v>
+      </c>
+      <c r="D27" s="10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E27" s="10" t="n">
         <v>0.04</v>
       </c>
-      <c r="D27" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="F27" s="10" t="n">
         <v>0</v>
       </c>
@@ -9114,6 +9571,21 @@
         <v>0</v>
       </c>
       <c r="H27" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="10" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="K27" s="10" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="L27" s="10" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="M27" s="10" t="n">
         <v>0.04</v>
       </c>
     </row>
@@ -9127,14 +9599,16 @@
         </is>
       </c>
       <c r="C28" s="10" t="n">
+        <v>3.742</v>
+      </c>
+      <c r="D28" s="10" t="inlineStr">
+        <is>
+          <t>y</t>
+        </is>
+      </c>
+      <c r="E28" s="10" t="n">
         <v>0.01</v>
       </c>
-      <c r="D28" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="F28" s="10" t="n">
         <v>0</v>
       </c>
@@ -9142,6 +9616,21 @@
         <v>0</v>
       </c>
       <c r="H28" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="K28" s="10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="L28" s="10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M28" s="10" t="n">
         <v>0.01</v>
       </c>
     </row>
@@ -9155,14 +9644,16 @@
         </is>
       </c>
       <c r="C29" s="10" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="D29" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E29" s="10" t="n">
         <v>86.88</v>
       </c>
-      <c r="D29" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="F29" s="10" t="n">
         <v>0</v>
       </c>
@@ -9170,7 +9661,22 @@
         <v>0</v>
       </c>
       <c r="H29" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="10" t="n">
         <v>86.88</v>
+      </c>
+      <c r="K29" s="10" t="n">
+        <v>34.06</v>
+      </c>
+      <c r="L29" s="10" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="M29" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -9183,14 +9689,16 @@
         </is>
       </c>
       <c r="C30" s="10" t="n">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="D30" s="10" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E30" s="10" t="n">
         <v>15.77</v>
       </c>
-      <c r="D30" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="F30" s="10" t="n">
         <v>0</v>
       </c>
@@ -9198,7 +9706,22 @@
         <v>0</v>
       </c>
       <c r="H30" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="10" t="n">
         <v>15.77</v>
+      </c>
+      <c r="K30" s="10" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="L30" s="10" t="n">
+        <v>14.53</v>
+      </c>
+      <c r="M30" s="10" t="n">
+        <v>2.21</v>
       </c>
     </row>
     <row r="31">
@@ -9211,22 +9734,39 @@
         </is>
       </c>
       <c r="C31" s="10" t="n">
+        <v>4.34</v>
+      </c>
+      <c r="D31" s="10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E31" s="10" t="n">
         <v>0.15</v>
       </c>
-      <c r="D31" s="10" t="n">
+      <c r="F31" s="10" t="n">
         <v>0.54</v>
       </c>
-      <c r="E31" s="10" t="n">
+      <c r="G31" s="10" t="n">
         <v>1.3</v>
       </c>
-      <c r="F31" s="10" t="n">
+      <c r="H31" s="10" t="n">
         <v>1.27</v>
       </c>
-      <c r="G31" s="10" t="n">
+      <c r="I31" s="10" t="n">
         <v>0.28</v>
       </c>
-      <c r="H31" s="10" t="n">
+      <c r="J31" s="10" t="n">
         <v>3.54</v>
+      </c>
+      <c r="K31" s="10" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="L31" s="10" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="M31" s="10" t="n">
+        <v>3.02</v>
       </c>
     </row>
     <row r="32">
@@ -9239,22 +9779,39 @@
         </is>
       </c>
       <c r="C32" s="10" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="D32" s="10" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E32" s="10" t="n">
         <v>19.96</v>
       </c>
-      <c r="D32" s="10" t="n">
+      <c r="F32" s="10" t="n">
         <v>24.95</v>
       </c>
-      <c r="E32" s="10" t="n">
+      <c r="G32" s="10" t="n">
         <v>12.44</v>
       </c>
-      <c r="F32" s="10" t="n">
+      <c r="H32" s="10" t="n">
         <v>2.93</v>
       </c>
-      <c r="G32" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" s="10" t="n">
+      <c r="I32" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="10" t="n">
         <v>60.27999999999999</v>
+      </c>
+      <c r="K32" s="10" t="n">
+        <v>59.77</v>
+      </c>
+      <c r="L32" s="10" t="n">
+        <v>58.28</v>
+      </c>
+      <c r="M32" s="10" t="n">
+        <v>26.78</v>
       </c>
     </row>
     <row r="33">
@@ -9267,22 +9824,39 @@
         </is>
       </c>
       <c r="C33" s="10" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D33" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E33" s="10" t="n">
         <v>600.38</v>
       </c>
-      <c r="D33" s="10" t="n">
+      <c r="F33" s="10" t="n">
         <v>750.47</v>
       </c>
-      <c r="E33" s="10" t="n">
+      <c r="G33" s="10" t="n">
         <v>374.33</v>
       </c>
-      <c r="F33" s="10" t="n">
+      <c r="H33" s="10" t="n">
         <v>88.25</v>
       </c>
-      <c r="G33" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" s="10" t="n">
+      <c r="I33" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="10" t="n">
         <v>1813.43</v>
+      </c>
+      <c r="K33" s="10" t="n">
+        <v>189.27</v>
+      </c>
+      <c r="L33" s="10" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="M33" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -9295,22 +9869,39 @@
         </is>
       </c>
       <c r="C34" s="10" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="D34" s="10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E34" s="10" t="n">
         <v>1.71</v>
       </c>
-      <c r="D34" s="10" t="n">
+      <c r="F34" s="10" t="n">
         <v>0.4</v>
       </c>
-      <c r="E34" s="10" t="n">
+      <c r="G34" s="10" t="n">
         <v>0.03</v>
       </c>
-      <c r="F34" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="H34" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="10" t="n">
         <v>2.14</v>
+      </c>
+      <c r="K34" s="10" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="L34" s="10" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="M34" s="10" t="n">
+        <v>2.05</v>
       </c>
     </row>
     <row r="35">
@@ -9323,22 +9914,39 @@
         </is>
       </c>
       <c r="C35" s="10" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D35" s="10" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="E35" s="10" t="n">
         <v>131.16</v>
       </c>
-      <c r="D35" s="10" t="n">
+      <c r="F35" s="10" t="n">
         <v>30.5</v>
       </c>
-      <c r="E35" s="10" t="n">
+      <c r="G35" s="10" t="n">
         <v>2.44</v>
       </c>
-      <c r="F35" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="H35" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="10" t="n">
         <v>164.1</v>
+      </c>
+      <c r="K35" s="10" t="n">
+        <v>158.16</v>
+      </c>
+      <c r="L35" s="10" t="n">
+        <v>141.6</v>
+      </c>
+      <c r="M35" s="10" t="n">
+        <v>4.77</v>
       </c>
     </row>
     <row r="36">
@@ -9351,14 +9959,16 @@
         </is>
       </c>
       <c r="C36" s="10" t="n">
+        <v>8.720000000000001</v>
+      </c>
+      <c r="D36" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E36" s="10" t="n">
         <v>22.06</v>
       </c>
-      <c r="D36" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="F36" s="10" t="n">
         <v>0</v>
       </c>
@@ -9366,7 +9976,22 @@
         <v>0</v>
       </c>
       <c r="H36" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="10" t="n">
         <v>22.06</v>
+      </c>
+      <c r="K36" s="10" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="L36" s="10" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="M36" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -9379,14 +10004,16 @@
         </is>
       </c>
       <c r="C37" s="10" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="D37" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E37" s="10" t="n">
         <v>22.25</v>
       </c>
-      <c r="D37" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="F37" s="10" t="n">
         <v>0</v>
       </c>
@@ -9394,7 +10021,22 @@
         <v>0</v>
       </c>
       <c r="H37" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="10" t="n">
         <v>22.25</v>
+      </c>
+      <c r="K37" s="10" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="L37" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -9407,21 +10049,38 @@
         </is>
       </c>
       <c r="C38" s="10" t="n">
+        <v>91</v>
+      </c>
+      <c r="D38" s="10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E38" s="10" t="n">
         <v>0.01</v>
       </c>
-      <c r="D38" s="10" t="n">
+      <c r="F38" s="10" t="n">
         <v>0.02</v>
       </c>
-      <c r="E38" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="G38" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="10" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="K38" s="10" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="L38" s="10" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M38" s="10" t="n">
         <v>0.03</v>
       </c>
     </row>
@@ -9435,14 +10094,16 @@
         </is>
       </c>
       <c r="C39" s="10" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="D39" s="10" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E39" s="10" t="n">
         <v>0.3</v>
       </c>
-      <c r="D39" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="F39" s="10" t="n">
         <v>0</v>
       </c>
@@ -9450,7 +10111,22 @@
         <v>0</v>
       </c>
       <c r="H39" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="10" t="n">
         <v>0.3</v>
+      </c>
+      <c r="K39" s="10" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L39" s="10" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="M39" s="10" t="n">
+        <v>0.26</v>
       </c>
     </row>
     <row r="40">
@@ -9463,14 +10139,16 @@
         </is>
       </c>
       <c r="C40" s="10" t="n">
+        <v>51.5</v>
+      </c>
+      <c r="D40" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E40" s="10" t="n">
         <v>24.65</v>
       </c>
-      <c r="D40" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="F40" s="10" t="n">
         <v>0</v>
       </c>
@@ -9478,7 +10156,22 @@
         <v>0</v>
       </c>
       <c r="H40" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="10" t="n">
         <v>24.65</v>
+      </c>
+      <c r="K40" s="10" t="n">
+        <v>20.14</v>
+      </c>
+      <c r="L40" s="10" t="n">
+        <v>10.99</v>
+      </c>
+      <c r="M40" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -9491,22 +10184,39 @@
         </is>
       </c>
       <c r="C41" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" s="10" t="n">
+        <v>6.263</v>
+      </c>
+      <c r="D41" s="10" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E41" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="10" t="n">
         <v>20.23</v>
       </c>
-      <c r="E41" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="10" t="n">
-        <v>0</v>
-      </c>
       <c r="G41" s="10" t="n">
         <v>0</v>
       </c>
       <c r="H41" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" s="10" t="n">
         <v>20.23</v>
+      </c>
+      <c r="K41" s="10" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="L41" s="10" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M41" s="10" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>